<commit_message>
Added in the VU0/1 registers (and other. misc ones)
</commit_message>
<xml_diff>
--- a/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
+++ b/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\Dev\Projects\PCSX2_Rewrite\PCSX2_Core\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="145">
   <si>
     <t>Field Name</t>
   </si>
@@ -228,6 +228,237 @@
   </si>
   <si>
     <t>DBF</t>
+  </si>
+  <si>
+    <t>MAC</t>
+  </si>
+  <si>
+    <t>Zw</t>
+  </si>
+  <si>
+    <t>Zz</t>
+  </si>
+  <si>
+    <t>Zy</t>
+  </si>
+  <si>
+    <t>Zx</t>
+  </si>
+  <si>
+    <t>Sw</t>
+  </si>
+  <si>
+    <t>Sz</t>
+  </si>
+  <si>
+    <t>Sy</t>
+  </si>
+  <si>
+    <t>Sx</t>
+  </si>
+  <si>
+    <t>Uw</t>
+  </si>
+  <si>
+    <t>Uy</t>
+  </si>
+  <si>
+    <t>Ux</t>
+  </si>
+  <si>
+    <t>Uz</t>
+  </si>
+  <si>
+    <t>Ow</t>
+  </si>
+  <si>
+    <t>Oz</t>
+  </si>
+  <si>
+    <t>Oy</t>
+  </si>
+  <si>
+    <t>Ox</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>ZS</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>Clipping</t>
+  </si>
+  <si>
+    <t>NegX_0</t>
+  </si>
+  <si>
+    <t>PosX_0</t>
+  </si>
+  <si>
+    <t>NegY_0</t>
+  </si>
+  <si>
+    <t>PosY_0</t>
+  </si>
+  <si>
+    <t>NegZ_0</t>
+  </si>
+  <si>
+    <t>PosZ_0</t>
+  </si>
+  <si>
+    <t>NegX_1</t>
+  </si>
+  <si>
+    <t>PosX_1</t>
+  </si>
+  <si>
+    <t>NegY_1</t>
+  </si>
+  <si>
+    <t>PosY_1</t>
+  </si>
+  <si>
+    <t>NegZ_1</t>
+  </si>
+  <si>
+    <t>PosZ_1</t>
+  </si>
+  <si>
+    <t>NegX_2</t>
+  </si>
+  <si>
+    <t>PosX_2</t>
+  </si>
+  <si>
+    <t>NegY_2</t>
+  </si>
+  <si>
+    <t>PosY_2</t>
+  </si>
+  <si>
+    <t>NegZ_2</t>
+  </si>
+  <si>
+    <t>PosZ_2</t>
+  </si>
+  <si>
+    <t>NegX_3</t>
+  </si>
+  <si>
+    <t>PosX_3</t>
+  </si>
+  <si>
+    <t>NegY_3</t>
+  </si>
+  <si>
+    <t>PosY_3</t>
+  </si>
+  <si>
+    <t>NegZ_3</t>
+  </si>
+  <si>
+    <t>PosZ_3</t>
+  </si>
+  <si>
+    <t>CMSAR</t>
+  </si>
+  <si>
+    <t>FB0</t>
+  </si>
+  <si>
+    <t>RS0</t>
+  </si>
+  <si>
+    <t>DE0</t>
+  </si>
+  <si>
+    <t>TE0</t>
+  </si>
+  <si>
+    <t>FB1</t>
+  </si>
+  <si>
+    <t>RS1</t>
+  </si>
+  <si>
+    <t>DE1</t>
+  </si>
+  <si>
+    <t>TE1</t>
+  </si>
+  <si>
+    <t>VBS0</t>
+  </si>
+  <si>
+    <t>VBS1</t>
+  </si>
+  <si>
+    <t>VDS0</t>
+  </si>
+  <si>
+    <t>VTS0</t>
+  </si>
+  <si>
+    <t>VFS0</t>
+  </si>
+  <si>
+    <t>DIV0</t>
+  </si>
+  <si>
+    <t>IBS0</t>
+  </si>
+  <si>
+    <t>VDS1</t>
+  </si>
+  <si>
+    <t>VTS1</t>
+  </si>
+  <si>
+    <t>VFS1</t>
+  </si>
+  <si>
+    <t>VGW1</t>
+  </si>
+  <si>
+    <t>DIV1</t>
+  </si>
+  <si>
+    <t>EFU1</t>
   </si>
 </sst>
 </file>
@@ -545,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H67" sqref="H2:H67"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +790,7 @@
     <col min="4" max="4" width="15.109375" customWidth="1"/>
     <col min="5" max="5" width="13.109375" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="8" max="8" width="29.109375" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1"/>
     <col min="9" max="9" width="32" customWidth="1"/>
     <col min="10" max="10" width="43.109375" customWidth="1"/>
   </cols>
@@ -2012,6 +2243,1898 @@
         <v>registerField(Fields::ME1, "ME1", 2, 1, 0);</v>
       </c>
     </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="H71" t="str">
+        <f>"class VectorUnitRegister_"&amp;A71&amp;"_t;"</f>
+        <v>class VectorUnitRegister_MAC_t;</v>
+      </c>
+      <c r="I71" t="str">
+        <f t="shared" ref="I71" si="3">"static constexpr u8 "&amp;C71&amp;" = "&amp;B71&amp;";"</f>
+        <v>static constexpr u8 Zw = 0;</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" ref="J71" si="4">"registerField(Fields::"&amp;C71&amp;", """&amp;C71&amp;""", "&amp;D71&amp;", "&amp;E71&amp;", "&amp;F71&amp;");"</f>
+        <v>registerField(Fields::Zw, "Zw", 0, 1, 0);</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>70</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="I72" t="str">
+        <f t="shared" ref="I72:I85" si="5">"static constexpr u8 "&amp;C72&amp;" = "&amp;B72&amp;";"</f>
+        <v>static constexpr u8 Zz = 1;</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" ref="J72:J85" si="6">"registerField(Fields::"&amp;C72&amp;", """&amp;C72&amp;""", "&amp;D72&amp;", "&amp;E72&amp;", "&amp;F72&amp;");"</f>
+        <v>registerField(Fields::Zz, "Zz", 1, 1, 0);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
+        <v>71</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="I73" t="str">
+        <f t="shared" si="5"/>
+        <v>static constexpr u8 Zy = 2;</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" si="6"/>
+        <v>registerField(Fields::Zy, "Zy", 2, 1, 0);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>3</v>
+      </c>
+      <c r="C74" t="s">
+        <v>72</v>
+      </c>
+      <c r="D74">
+        <v>3</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="I74" t="str">
+        <f t="shared" si="5"/>
+        <v>static constexpr u8 Zx = 3;</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" si="6"/>
+        <v>registerField(Fields::Zx, "Zx", 3, 1, 0);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <v>4</v>
+      </c>
+      <c r="C75" t="s">
+        <v>73</v>
+      </c>
+      <c r="D75">
+        <v>4</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="I75" t="str">
+        <f t="shared" si="5"/>
+        <v>static constexpr u8 Sw = 4;</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" si="6"/>
+        <v>registerField(Fields::Sw, "Sw", 4, 1, 0);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>5</v>
+      </c>
+      <c r="C76" t="s">
+        <v>74</v>
+      </c>
+      <c r="D76">
+        <v>5</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="I76" t="str">
+        <f t="shared" si="5"/>
+        <v>static constexpr u8 Sz = 5;</v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" si="6"/>
+        <v>registerField(Fields::Sz, "Sz", 5, 1, 0);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>6</v>
+      </c>
+      <c r="C77" t="s">
+        <v>75</v>
+      </c>
+      <c r="D77">
+        <v>6</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="I77" t="str">
+        <f t="shared" si="5"/>
+        <v>static constexpr u8 Sy = 6;</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="6"/>
+        <v>registerField(Fields::Sy, "Sy", 6, 1, 0);</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D78">
+        <v>7</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="I78" t="str">
+        <f t="shared" si="5"/>
+        <v>static constexpr u8 Sx = 7;</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="6"/>
+        <v>registerField(Fields::Sx, "Sx", 7, 1, 0);</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>8</v>
+      </c>
+      <c r="C79" t="s">
+        <v>77</v>
+      </c>
+      <c r="D79">
+        <v>8</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="I79" t="str">
+        <f t="shared" si="5"/>
+        <v>static constexpr u8 Uw = 8;</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="6"/>
+        <v>registerField(Fields::Uw, "Uw", 8, 1, 0);</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>9</v>
+      </c>
+      <c r="C80" t="s">
+        <v>80</v>
+      </c>
+      <c r="D80">
+        <v>9</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="I80" t="str">
+        <f t="shared" si="5"/>
+        <v>static constexpr u8 Uz = 9;</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" si="6"/>
+        <v>registerField(Fields::Uz, "Uz", 9, 1, 0);</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>10</v>
+      </c>
+      <c r="C81" t="s">
+        <v>78</v>
+      </c>
+      <c r="D81">
+        <v>10</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="I81" t="str">
+        <f t="shared" si="5"/>
+        <v>static constexpr u8 Uy = 10;</v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" si="6"/>
+        <v>registerField(Fields::Uy, "Uy", 10, 1, 0);</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <v>11</v>
+      </c>
+      <c r="C82" t="s">
+        <v>79</v>
+      </c>
+      <c r="D82">
+        <v>11</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="I82" t="str">
+        <f t="shared" si="5"/>
+        <v>static constexpr u8 Ux = 11;</v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" si="6"/>
+        <v>registerField(Fields::Ux, "Ux", 11, 1, 0);</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <v>12</v>
+      </c>
+      <c r="C83" t="s">
+        <v>81</v>
+      </c>
+      <c r="D83">
+        <v>12</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="I83" t="str">
+        <f t="shared" si="5"/>
+        <v>static constexpr u8 Ow = 12;</v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" si="6"/>
+        <v>registerField(Fields::Ow, "Ow", 12, 1, 0);</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>13</v>
+      </c>
+      <c r="C84" t="s">
+        <v>82</v>
+      </c>
+      <c r="D84">
+        <v>13</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="I84" t="str">
+        <f t="shared" si="5"/>
+        <v>static constexpr u8 Oz = 13;</v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" si="6"/>
+        <v>registerField(Fields::Oz, "Oz", 13, 1, 0);</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>14</v>
+      </c>
+      <c r="C85" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85">
+        <v>14</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="I85" t="str">
+        <f t="shared" si="5"/>
+        <v>static constexpr u8 Oy = 14;</v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" si="6"/>
+        <v>registerField(Fields::Oy, "Oy", 14, 1, 0);</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <v>15</v>
+      </c>
+      <c r="C86" t="s">
+        <v>84</v>
+      </c>
+      <c r="D86">
+        <v>15</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="I86" t="str">
+        <f t="shared" ref="I86" si="7">"static constexpr u8 "&amp;C86&amp;" = "&amp;B86&amp;";"</f>
+        <v>static constexpr u8 Ox = 15;</v>
+      </c>
+      <c r="J86" t="str">
+        <f t="shared" ref="J86" si="8">"registerField(Fields::"&amp;C86&amp;", """&amp;C86&amp;""", "&amp;D86&amp;", "&amp;E86&amp;", "&amp;F86&amp;");"</f>
+        <v>registerField(Fields::Ox, "Ox", 15, 1, 0);</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>85</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88" t="s">
+        <v>86</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="H88" t="str">
+        <f>"class VectorUnitRegister_"&amp;A88&amp;"_t;"</f>
+        <v>class VectorUnitRegister_Status_t;</v>
+      </c>
+      <c r="I88" t="str">
+        <f t="shared" ref="I88" si="9">"static constexpr u8 "&amp;C88&amp;" = "&amp;B88&amp;";"</f>
+        <v>static constexpr u8 Z = 0;</v>
+      </c>
+      <c r="J88" t="str">
+        <f t="shared" ref="J88" si="10">"registerField(Fields::"&amp;C88&amp;", """&amp;C88&amp;""", "&amp;D88&amp;", "&amp;E88&amp;", "&amp;F88&amp;");"</f>
+        <v>registerField(Fields::Z, "Z", 0, 1, 0);</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89" t="s">
+        <v>87</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="I89" t="str">
+        <f t="shared" ref="I89:I99" si="11">"static constexpr u8 "&amp;C89&amp;" = "&amp;B89&amp;";"</f>
+        <v>static constexpr u8 S = 1;</v>
+      </c>
+      <c r="J89" t="str">
+        <f t="shared" ref="J89:J99" si="12">"registerField(Fields::"&amp;C89&amp;", """&amp;C89&amp;""", "&amp;D89&amp;", "&amp;E89&amp;", "&amp;F89&amp;");"</f>
+        <v>registerField(Fields::S, "S", 1, 1, 0);</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>2</v>
+      </c>
+      <c r="C90" t="s">
+        <v>88</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="I90" t="str">
+        <f t="shared" si="11"/>
+        <v>static constexpr u8 U = 2;</v>
+      </c>
+      <c r="J90" t="str">
+        <f t="shared" si="12"/>
+        <v>registerField(Fields::U, "U", 2, 1, 0);</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>3</v>
+      </c>
+      <c r="C91" t="s">
+        <v>89</v>
+      </c>
+      <c r="D91">
+        <v>3</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="I91" t="str">
+        <f t="shared" si="11"/>
+        <v>static constexpr u8 O = 3;</v>
+      </c>
+      <c r="J91" t="str">
+        <f t="shared" si="12"/>
+        <v>registerField(Fields::O, "O", 3, 1, 0);</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <v>4</v>
+      </c>
+      <c r="C92" t="s">
+        <v>90</v>
+      </c>
+      <c r="D92">
+        <v>4</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="I92" t="str">
+        <f t="shared" si="11"/>
+        <v>static constexpr u8 I = 4;</v>
+      </c>
+      <c r="J92" t="str">
+        <f t="shared" si="12"/>
+        <v>registerField(Fields::I, "I", 4, 1, 0);</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B93">
+        <v>5</v>
+      </c>
+      <c r="C93" t="s">
+        <v>91</v>
+      </c>
+      <c r="D93">
+        <v>5</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="I93" t="str">
+        <f t="shared" si="11"/>
+        <v>static constexpr u8 D = 5;</v>
+      </c>
+      <c r="J93" t="str">
+        <f t="shared" si="12"/>
+        <v>registerField(Fields::D, "D", 5, 1, 0);</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B94">
+        <v>6</v>
+      </c>
+      <c r="C94" t="s">
+        <v>92</v>
+      </c>
+      <c r="D94">
+        <v>6</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="I94" t="str">
+        <f t="shared" si="11"/>
+        <v>static constexpr u8 ZS = 6;</v>
+      </c>
+      <c r="J94" t="str">
+        <f t="shared" si="12"/>
+        <v>registerField(Fields::ZS, "ZS", 6, 1, 0);</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B95">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s">
+        <v>93</v>
+      </c>
+      <c r="D95">
+        <v>7</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="I95" t="str">
+        <f t="shared" si="11"/>
+        <v>static constexpr u8 SS = 7;</v>
+      </c>
+      <c r="J95" t="str">
+        <f t="shared" si="12"/>
+        <v>registerField(Fields::SS, "SS", 7, 1, 0);</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B96">
+        <v>8</v>
+      </c>
+      <c r="C96" t="s">
+        <v>94</v>
+      </c>
+      <c r="D96">
+        <v>8</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="I96" t="str">
+        <f t="shared" si="11"/>
+        <v>static constexpr u8 US = 8;</v>
+      </c>
+      <c r="J96" t="str">
+        <f t="shared" si="12"/>
+        <v>registerField(Fields::US, "US", 8, 1, 0);</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B97">
+        <v>9</v>
+      </c>
+      <c r="C97" t="s">
+        <v>95</v>
+      </c>
+      <c r="D97">
+        <v>9</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="I97" t="str">
+        <f t="shared" si="11"/>
+        <v>static constexpr u8 OS = 9;</v>
+      </c>
+      <c r="J97" t="str">
+        <f t="shared" si="12"/>
+        <v>registerField(Fields::OS, "OS", 9, 1, 0);</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B98">
+        <v>10</v>
+      </c>
+      <c r="C98" t="s">
+        <v>96</v>
+      </c>
+      <c r="D98">
+        <v>10</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="I98" t="str">
+        <f t="shared" si="11"/>
+        <v>static constexpr u8 IS = 10;</v>
+      </c>
+      <c r="J98" t="str">
+        <f t="shared" si="12"/>
+        <v>registerField(Fields::IS, "IS", 10, 1, 0);</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B99">
+        <v>11</v>
+      </c>
+      <c r="C99" t="s">
+        <v>97</v>
+      </c>
+      <c r="D99">
+        <v>11</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="I99" t="str">
+        <f t="shared" si="11"/>
+        <v>static constexpr u8 DS = 11;</v>
+      </c>
+      <c r="J99" t="str">
+        <f t="shared" si="12"/>
+        <v>registerField(Fields::DS, "DS", 11, 1, 0);</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>98</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101" t="s">
+        <v>99</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="H101" t="str">
+        <f>"class VectorUnitRegister_"&amp;A101&amp;"_t;"</f>
+        <v>class VectorUnitRegister_Clipping_t;</v>
+      </c>
+      <c r="I101" t="str">
+        <f t="shared" ref="I101" si="13">"static constexpr u8 "&amp;C101&amp;" = "&amp;B101&amp;";"</f>
+        <v>static constexpr u8 NegX_0 = 0;</v>
+      </c>
+      <c r="J101" t="str">
+        <f t="shared" ref="J101" si="14">"registerField(Fields::"&amp;C101&amp;", """&amp;C101&amp;""", "&amp;D101&amp;", "&amp;E101&amp;", "&amp;F101&amp;");"</f>
+        <v>registerField(Fields::NegX_0, "NegX_0", 0, 1, 0);</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>100</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="I102" t="str">
+        <f t="shared" ref="I102:I124" si="15">"static constexpr u8 "&amp;C102&amp;" = "&amp;B102&amp;";"</f>
+        <v>static constexpr u8 PosX_0 = 1;</v>
+      </c>
+      <c r="J102" t="str">
+        <f t="shared" ref="J102:J124" si="16">"registerField(Fields::"&amp;C102&amp;", """&amp;C102&amp;""", "&amp;D102&amp;", "&amp;E102&amp;", "&amp;F102&amp;");"</f>
+        <v>registerField(Fields::PosX_0, "PosX_0", 1, 1, 0);</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103" t="s">
+        <v>101</v>
+      </c>
+      <c r="D103">
+        <v>2</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="I103" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 NegY_0 = 2;</v>
+      </c>
+      <c r="J103" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::NegY_0, "NegY_0", 2, 1, 0);</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B104">
+        <v>3</v>
+      </c>
+      <c r="C104" t="s">
+        <v>102</v>
+      </c>
+      <c r="D104">
+        <v>3</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="I104" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 PosY_0 = 3;</v>
+      </c>
+      <c r="J104" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::PosY_0, "PosY_0", 3, 1, 0);</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B105">
+        <v>4</v>
+      </c>
+      <c r="C105" t="s">
+        <v>103</v>
+      </c>
+      <c r="D105">
+        <v>4</v>
+      </c>
+      <c r="E105">
+        <v>1</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="I105" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 NegZ_0 = 4;</v>
+      </c>
+      <c r="J105" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::NegZ_0, "NegZ_0", 4, 1, 0);</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B106">
+        <v>5</v>
+      </c>
+      <c r="C106" t="s">
+        <v>104</v>
+      </c>
+      <c r="D106">
+        <v>5</v>
+      </c>
+      <c r="E106">
+        <v>1</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="I106" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 PosZ_0 = 5;</v>
+      </c>
+      <c r="J106" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::PosZ_0, "PosZ_0", 5, 1, 0);</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B107">
+        <v>6</v>
+      </c>
+      <c r="C107" t="s">
+        <v>105</v>
+      </c>
+      <c r="D107">
+        <v>6</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="I107" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 NegX_1 = 6;</v>
+      </c>
+      <c r="J107" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::NegX_1, "NegX_1", 6, 1, 0);</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B108">
+        <v>7</v>
+      </c>
+      <c r="C108" t="s">
+        <v>106</v>
+      </c>
+      <c r="D108">
+        <v>7</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="I108" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 PosX_1 = 7;</v>
+      </c>
+      <c r="J108" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::PosX_1, "PosX_1", 7, 1, 0);</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B109">
+        <v>8</v>
+      </c>
+      <c r="C109" t="s">
+        <v>107</v>
+      </c>
+      <c r="D109">
+        <v>8</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+      <c r="I109" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 NegY_1 = 8;</v>
+      </c>
+      <c r="J109" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::NegY_1, "NegY_1", 8, 1, 0);</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B110">
+        <v>9</v>
+      </c>
+      <c r="C110" t="s">
+        <v>108</v>
+      </c>
+      <c r="D110">
+        <v>9</v>
+      </c>
+      <c r="E110">
+        <v>1</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+      <c r="I110" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 PosY_1 = 9;</v>
+      </c>
+      <c r="J110" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::PosY_1, "PosY_1", 9, 1, 0);</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B111">
+        <v>10</v>
+      </c>
+      <c r="C111" t="s">
+        <v>109</v>
+      </c>
+      <c r="D111">
+        <v>10</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
+      </c>
+      <c r="I111" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 NegZ_1 = 10;</v>
+      </c>
+      <c r="J111" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::NegZ_1, "NegZ_1", 10, 1, 0);</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B112">
+        <v>11</v>
+      </c>
+      <c r="C112" t="s">
+        <v>110</v>
+      </c>
+      <c r="D112">
+        <v>11</v>
+      </c>
+      <c r="E112">
+        <v>1</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="I112" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 PosZ_1 = 11;</v>
+      </c>
+      <c r="J112" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::PosZ_1, "PosZ_1", 11, 1, 0);</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B113">
+        <v>12</v>
+      </c>
+      <c r="C113" t="s">
+        <v>111</v>
+      </c>
+      <c r="D113">
+        <v>12</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="I113" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 NegX_2 = 12;</v>
+      </c>
+      <c r="J113" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::NegX_2, "NegX_2", 12, 1, 0);</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B114">
+        <v>13</v>
+      </c>
+      <c r="C114" t="s">
+        <v>112</v>
+      </c>
+      <c r="D114">
+        <v>13</v>
+      </c>
+      <c r="E114">
+        <v>1</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+      <c r="I114" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 PosX_2 = 13;</v>
+      </c>
+      <c r="J114" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::PosX_2, "PosX_2", 13, 1, 0);</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B115">
+        <v>14</v>
+      </c>
+      <c r="C115" t="s">
+        <v>113</v>
+      </c>
+      <c r="D115">
+        <v>14</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
+      </c>
+      <c r="I115" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 NegY_2 = 14;</v>
+      </c>
+      <c r="J115" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::NegY_2, "NegY_2", 14, 1, 0);</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B116">
+        <v>15</v>
+      </c>
+      <c r="C116" t="s">
+        <v>114</v>
+      </c>
+      <c r="D116">
+        <v>15</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+      <c r="F116">
+        <v>0</v>
+      </c>
+      <c r="I116" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 PosY_2 = 15;</v>
+      </c>
+      <c r="J116" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::PosY_2, "PosY_2", 15, 1, 0);</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B117">
+        <v>16</v>
+      </c>
+      <c r="C117" t="s">
+        <v>115</v>
+      </c>
+      <c r="D117">
+        <v>16</v>
+      </c>
+      <c r="E117">
+        <v>1</v>
+      </c>
+      <c r="F117">
+        <v>0</v>
+      </c>
+      <c r="I117" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 NegZ_2 = 16;</v>
+      </c>
+      <c r="J117" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::NegZ_2, "NegZ_2", 16, 1, 0);</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B118">
+        <v>17</v>
+      </c>
+      <c r="C118" t="s">
+        <v>116</v>
+      </c>
+      <c r="D118">
+        <v>17</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <v>0</v>
+      </c>
+      <c r="I118" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 PosZ_2 = 17;</v>
+      </c>
+      <c r="J118" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::PosZ_2, "PosZ_2", 17, 1, 0);</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B119">
+        <v>18</v>
+      </c>
+      <c r="C119" t="s">
+        <v>117</v>
+      </c>
+      <c r="D119">
+        <v>18</v>
+      </c>
+      <c r="E119">
+        <v>1</v>
+      </c>
+      <c r="F119">
+        <v>0</v>
+      </c>
+      <c r="I119" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 NegX_3 = 18;</v>
+      </c>
+      <c r="J119" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::NegX_3, "NegX_3", 18, 1, 0);</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B120">
+        <v>19</v>
+      </c>
+      <c r="C120" t="s">
+        <v>118</v>
+      </c>
+      <c r="D120">
+        <v>19</v>
+      </c>
+      <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="F120">
+        <v>0</v>
+      </c>
+      <c r="I120" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 PosX_3 = 19;</v>
+      </c>
+      <c r="J120" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::PosX_3, "PosX_3", 19, 1, 0);</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B121">
+        <v>20</v>
+      </c>
+      <c r="C121" t="s">
+        <v>119</v>
+      </c>
+      <c r="D121">
+        <v>20</v>
+      </c>
+      <c r="E121">
+        <v>1</v>
+      </c>
+      <c r="F121">
+        <v>0</v>
+      </c>
+      <c r="I121" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 NegY_3 = 20;</v>
+      </c>
+      <c r="J121" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::NegY_3, "NegY_3", 20, 1, 0);</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B122">
+        <v>21</v>
+      </c>
+      <c r="C122" t="s">
+        <v>120</v>
+      </c>
+      <c r="D122">
+        <v>21</v>
+      </c>
+      <c r="E122">
+        <v>1</v>
+      </c>
+      <c r="F122">
+        <v>0</v>
+      </c>
+      <c r="I122" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 PosY_3 = 21;</v>
+      </c>
+      <c r="J122" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::PosY_3, "PosY_3", 21, 1, 0);</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B123">
+        <v>22</v>
+      </c>
+      <c r="C123" t="s">
+        <v>121</v>
+      </c>
+      <c r="D123">
+        <v>22</v>
+      </c>
+      <c r="E123">
+        <v>1</v>
+      </c>
+      <c r="F123">
+        <v>0</v>
+      </c>
+      <c r="I123" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 NegZ_3 = 22;</v>
+      </c>
+      <c r="J123" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::NegZ_3, "NegZ_3", 22, 1, 0);</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B124">
+        <v>23</v>
+      </c>
+      <c r="C124" t="s">
+        <v>122</v>
+      </c>
+      <c r="D124">
+        <v>23</v>
+      </c>
+      <c r="E124">
+        <v>1</v>
+      </c>
+      <c r="F124">
+        <v>0</v>
+      </c>
+      <c r="I124" t="str">
+        <f t="shared" si="15"/>
+        <v>static constexpr u8 PosZ_3 = 23;</v>
+      </c>
+      <c r="J124" t="str">
+        <f t="shared" si="16"/>
+        <v>registerField(Fields::PosZ_3, "PosZ_3", 23, 1, 0);</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>123</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="C126" t="s">
+        <v>123</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+      <c r="E126">
+        <v>16</v>
+      </c>
+      <c r="F126">
+        <v>0</v>
+      </c>
+      <c r="H126" t="str">
+        <f>"class VectorUnitRegister_"&amp;A126&amp;"_t;"</f>
+        <v>class VectorUnitRegister_CMSAR_t;</v>
+      </c>
+      <c r="I126" t="str">
+        <f t="shared" ref="I126" si="17">"static constexpr u8 "&amp;C126&amp;" = "&amp;B126&amp;";"</f>
+        <v>static constexpr u8 CMSAR = 0;</v>
+      </c>
+      <c r="J126" t="str">
+        <f t="shared" ref="J126" si="18">"registerField(Fields::"&amp;C126&amp;", """&amp;C126&amp;""", "&amp;D126&amp;", "&amp;E126&amp;", "&amp;F126&amp;");"</f>
+        <v>registerField(Fields::CMSAR, "CMSAR", 0, 16, 0);</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>55</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128" t="s">
+        <v>124</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>1</v>
+      </c>
+      <c r="F128">
+        <v>0</v>
+      </c>
+      <c r="H128" t="str">
+        <f>"class VURegister_"&amp;A128&amp;"_t;"</f>
+        <v>class VURegister_FBRST_t;</v>
+      </c>
+      <c r="I128" t="str">
+        <f t="shared" ref="I128" si="19">"static constexpr u8 "&amp;C128&amp;" = "&amp;B128&amp;";"</f>
+        <v>static constexpr u8 FB0 = 0;</v>
+      </c>
+      <c r="J128" t="str">
+        <f t="shared" ref="J128" si="20">"registerField(Fields::"&amp;C128&amp;", """&amp;C128&amp;""", "&amp;D128&amp;", "&amp;E128&amp;", "&amp;F128&amp;");"</f>
+        <v>registerField(Fields::FB0, "FB0", 0, 1, 0);</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="C129" t="s">
+        <v>125</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+      <c r="F129">
+        <v>0</v>
+      </c>
+      <c r="I129" t="str">
+        <f t="shared" ref="I129:I135" si="21">"static constexpr u8 "&amp;C129&amp;" = "&amp;B129&amp;";"</f>
+        <v>static constexpr u8 RS0 = 1;</v>
+      </c>
+      <c r="J129" t="str">
+        <f t="shared" ref="J129:J135" si="22">"registerField(Fields::"&amp;C129&amp;", """&amp;C129&amp;""", "&amp;D129&amp;", "&amp;E129&amp;", "&amp;F129&amp;");"</f>
+        <v>registerField(Fields::RS0, "RS0", 1, 1, 0);</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B130">
+        <v>2</v>
+      </c>
+      <c r="C130" t="s">
+        <v>126</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
+      </c>
+      <c r="E130">
+        <v>1</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+      <c r="I130" t="str">
+        <f t="shared" si="21"/>
+        <v>static constexpr u8 DE0 = 2;</v>
+      </c>
+      <c r="J130" t="str">
+        <f t="shared" si="22"/>
+        <v>registerField(Fields::DE0, "DE0", 2, 1, 0);</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B131">
+        <v>3</v>
+      </c>
+      <c r="C131" t="s">
+        <v>127</v>
+      </c>
+      <c r="D131">
+        <v>3</v>
+      </c>
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <v>0</v>
+      </c>
+      <c r="I131" t="str">
+        <f t="shared" si="21"/>
+        <v>static constexpr u8 TE0 = 3;</v>
+      </c>
+      <c r="J131" t="str">
+        <f t="shared" si="22"/>
+        <v>registerField(Fields::TE0, "TE0", 3, 1, 0);</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B132">
+        <v>4</v>
+      </c>
+      <c r="C132" t="s">
+        <v>128</v>
+      </c>
+      <c r="D132">
+        <v>8</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="F132">
+        <v>0</v>
+      </c>
+      <c r="I132" t="str">
+        <f t="shared" si="21"/>
+        <v>static constexpr u8 FB1 = 4;</v>
+      </c>
+      <c r="J132" t="str">
+        <f t="shared" si="22"/>
+        <v>registerField(Fields::FB1, "FB1", 8, 1, 0);</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B133">
+        <v>5</v>
+      </c>
+      <c r="C133" t="s">
+        <v>129</v>
+      </c>
+      <c r="D133">
+        <v>9</v>
+      </c>
+      <c r="E133">
+        <v>1</v>
+      </c>
+      <c r="F133">
+        <v>0</v>
+      </c>
+      <c r="I133" t="str">
+        <f t="shared" si="21"/>
+        <v>static constexpr u8 RS1 = 5;</v>
+      </c>
+      <c r="J133" t="str">
+        <f t="shared" si="22"/>
+        <v>registerField(Fields::RS1, "RS1", 9, 1, 0);</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B134">
+        <v>6</v>
+      </c>
+      <c r="C134" t="s">
+        <v>130</v>
+      </c>
+      <c r="D134">
+        <v>10</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="F134">
+        <v>0</v>
+      </c>
+      <c r="I134" t="str">
+        <f t="shared" si="21"/>
+        <v>static constexpr u8 DE1 = 6;</v>
+      </c>
+      <c r="J134" t="str">
+        <f t="shared" si="22"/>
+        <v>registerField(Fields::DE1, "DE1", 10, 1, 0);</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B135">
+        <v>7</v>
+      </c>
+      <c r="C135" t="s">
+        <v>131</v>
+      </c>
+      <c r="D135">
+        <v>11</v>
+      </c>
+      <c r="E135">
+        <v>1</v>
+      </c>
+      <c r="F135">
+        <v>0</v>
+      </c>
+      <c r="I135" t="str">
+        <f t="shared" si="21"/>
+        <v>static constexpr u8 TE1 = 7;</v>
+      </c>
+      <c r="J135" t="str">
+        <f t="shared" si="22"/>
+        <v>registerField(Fields::TE1, "TE1", 11, 1, 0);</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>44</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+      <c r="C137" t="s">
+        <v>132</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>1</v>
+      </c>
+      <c r="F137">
+        <v>0</v>
+      </c>
+      <c r="H137" t="str">
+        <f>"class VPURegister_"&amp;A137&amp;"_t;"</f>
+        <v>class VPURegister_STAT_t;</v>
+      </c>
+      <c r="I137" t="str">
+        <f t="shared" ref="I137" si="23">"static constexpr u8 "&amp;C137&amp;" = "&amp;B137&amp;";"</f>
+        <v>static constexpr u8 VBS0 = 0;</v>
+      </c>
+      <c r="J137" t="str">
+        <f t="shared" ref="J137" si="24">"registerField(Fields::"&amp;C137&amp;", """&amp;C137&amp;""", "&amp;D137&amp;", "&amp;E137&amp;", "&amp;F137&amp;");"</f>
+        <v>registerField(Fields::VBS0, "VBS0", 0, 1, 0);</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B138">
+        <v>1</v>
+      </c>
+      <c r="C138" t="s">
+        <v>134</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+      <c r="F138">
+        <v>0</v>
+      </c>
+      <c r="I138" t="str">
+        <f t="shared" ref="I138:I149" si="25">"static constexpr u8 "&amp;C138&amp;" = "&amp;B138&amp;";"</f>
+        <v>static constexpr u8 VDS0 = 1;</v>
+      </c>
+      <c r="J138" t="str">
+        <f t="shared" ref="J138:J149" si="26">"registerField(Fields::"&amp;C138&amp;", """&amp;C138&amp;""", "&amp;D138&amp;", "&amp;E138&amp;", "&amp;F138&amp;");"</f>
+        <v>registerField(Fields::VDS0, "VDS0", 1, 1, 0);</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B139">
+        <v>2</v>
+      </c>
+      <c r="C139" t="s">
+        <v>135</v>
+      </c>
+      <c r="D139">
+        <v>2</v>
+      </c>
+      <c r="E139">
+        <v>1</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+      <c r="I139" t="str">
+        <f t="shared" si="25"/>
+        <v>static constexpr u8 VTS0 = 2;</v>
+      </c>
+      <c r="J139" t="str">
+        <f t="shared" si="26"/>
+        <v>registerField(Fields::VTS0, "VTS0", 2, 1, 0);</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B140">
+        <v>3</v>
+      </c>
+      <c r="C140" t="s">
+        <v>136</v>
+      </c>
+      <c r="D140">
+        <v>3</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+      <c r="I140" t="str">
+        <f t="shared" si="25"/>
+        <v>static constexpr u8 VFS0 = 3;</v>
+      </c>
+      <c r="J140" t="str">
+        <f t="shared" si="26"/>
+        <v>registerField(Fields::VFS0, "VFS0", 3, 1, 0);</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B141">
+        <v>4</v>
+      </c>
+      <c r="C141" t="s">
+        <v>137</v>
+      </c>
+      <c r="D141">
+        <v>5</v>
+      </c>
+      <c r="E141">
+        <v>1</v>
+      </c>
+      <c r="F141">
+        <v>0</v>
+      </c>
+      <c r="I141" t="str">
+        <f t="shared" si="25"/>
+        <v>static constexpr u8 DIV0 = 4;</v>
+      </c>
+      <c r="J141" t="str">
+        <f t="shared" si="26"/>
+        <v>registerField(Fields::DIV0, "DIV0", 5, 1, 0);</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B142">
+        <v>5</v>
+      </c>
+      <c r="C142" t="s">
+        <v>138</v>
+      </c>
+      <c r="D142">
+        <v>7</v>
+      </c>
+      <c r="E142">
+        <v>1</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+      <c r="I142" t="str">
+        <f t="shared" si="25"/>
+        <v>static constexpr u8 IBS0 = 5;</v>
+      </c>
+      <c r="J142" t="str">
+        <f t="shared" si="26"/>
+        <v>registerField(Fields::IBS0, "IBS0", 7, 1, 0);</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B143">
+        <v>6</v>
+      </c>
+      <c r="C143" t="s">
+        <v>133</v>
+      </c>
+      <c r="D143">
+        <v>8</v>
+      </c>
+      <c r="E143">
+        <v>1</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+      <c r="I143" t="str">
+        <f t="shared" si="25"/>
+        <v>static constexpr u8 VBS1 = 6;</v>
+      </c>
+      <c r="J143" t="str">
+        <f t="shared" si="26"/>
+        <v>registerField(Fields::VBS1, "VBS1", 8, 1, 0);</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B144">
+        <v>7</v>
+      </c>
+      <c r="C144" t="s">
+        <v>139</v>
+      </c>
+      <c r="D144">
+        <v>9</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+      <c r="I144" t="str">
+        <f t="shared" si="25"/>
+        <v>static constexpr u8 VDS1 = 7;</v>
+      </c>
+      <c r="J144" t="str">
+        <f t="shared" si="26"/>
+        <v>registerField(Fields::VDS1, "VDS1", 9, 1, 0);</v>
+      </c>
+    </row>
+    <row r="145" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B145">
+        <v>8</v>
+      </c>
+      <c r="C145" t="s">
+        <v>140</v>
+      </c>
+      <c r="D145">
+        <v>10</v>
+      </c>
+      <c r="E145">
+        <v>1</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+      <c r="I145" t="str">
+        <f t="shared" si="25"/>
+        <v>static constexpr u8 VTS1 = 8;</v>
+      </c>
+      <c r="J145" t="str">
+        <f t="shared" si="26"/>
+        <v>registerField(Fields::VTS1, "VTS1", 10, 1, 0);</v>
+      </c>
+    </row>
+    <row r="146" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B146">
+        <v>9</v>
+      </c>
+      <c r="C146" t="s">
+        <v>141</v>
+      </c>
+      <c r="D146">
+        <v>11</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
+      <c r="F146">
+        <v>0</v>
+      </c>
+      <c r="I146" t="str">
+        <f t="shared" si="25"/>
+        <v>static constexpr u8 VFS1 = 9;</v>
+      </c>
+      <c r="J146" t="str">
+        <f t="shared" si="26"/>
+        <v>registerField(Fields::VFS1, "VFS1", 11, 1, 0);</v>
+      </c>
+    </row>
+    <row r="147" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B147">
+        <v>10</v>
+      </c>
+      <c r="C147" t="s">
+        <v>142</v>
+      </c>
+      <c r="D147">
+        <v>12</v>
+      </c>
+      <c r="E147">
+        <v>1</v>
+      </c>
+      <c r="F147">
+        <v>0</v>
+      </c>
+      <c r="I147" t="str">
+        <f t="shared" si="25"/>
+        <v>static constexpr u8 VGW1 = 10;</v>
+      </c>
+      <c r="J147" t="str">
+        <f t="shared" si="26"/>
+        <v>registerField(Fields::VGW1, "VGW1", 12, 1, 0);</v>
+      </c>
+    </row>
+    <row r="148" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B148">
+        <v>11</v>
+      </c>
+      <c r="C148" t="s">
+        <v>143</v>
+      </c>
+      <c r="D148">
+        <v>13</v>
+      </c>
+      <c r="E148">
+        <v>1</v>
+      </c>
+      <c r="F148">
+        <v>0</v>
+      </c>
+      <c r="I148" t="str">
+        <f t="shared" si="25"/>
+        <v>static constexpr u8 DIV1 = 11;</v>
+      </c>
+      <c r="J148" t="str">
+        <f t="shared" si="26"/>
+        <v>registerField(Fields::DIV1, "DIV1", 13, 1, 0);</v>
+      </c>
+    </row>
+    <row r="149" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B149">
+        <v>12</v>
+      </c>
+      <c r="C149" t="s">
+        <v>144</v>
+      </c>
+      <c r="D149">
+        <v>14</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+      <c r="F149">
+        <v>0</v>
+      </c>
+      <c r="I149" t="str">
+        <f t="shared" si="25"/>
+        <v>static constexpr u8 EFU1 = 12;</v>
+      </c>
+      <c r="J149" t="str">
+        <f t="shared" si="26"/>
+        <v>registerField(Fields::EFU1, "EFU1", 14, 1, 0);</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
WIP on IOP DMAC registers. Changed FIFO queue to use u32 as base type, since the IOP needs to read from it.
</commit_message>
<xml_diff>
--- a/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
+++ b/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="153">
   <si>
     <t>Field Name</t>
   </si>
@@ -459,6 +459,30 @@
   </si>
   <si>
     <t>EFU1</t>
+  </si>
+  <si>
+    <t>BCR</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>CHCR</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>LI</t>
+  </si>
+  <si>
+    <t>TR</t>
   </si>
 </sst>
 </file>
@@ -776,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J149"/>
+  <dimension ref="A1:J157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="I137" workbookViewId="0">
+      <selection activeCell="J154" sqref="J154:J157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4010,7 +4034,7 @@
         <v>registerField(Fields::VDS1, "VDS1", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="145" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B145">
         <v>8</v>
       </c>
@@ -4035,7 +4059,7 @@
         <v>registerField(Fields::VTS1, "VTS1", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="146" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B146">
         <v>9</v>
       </c>
@@ -4060,7 +4084,7 @@
         <v>registerField(Fields::VFS1, "VFS1", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="147" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B147">
         <v>10</v>
       </c>
@@ -4085,7 +4109,7 @@
         <v>registerField(Fields::VGW1, "VGW1", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="148" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B148">
         <v>11</v>
       </c>
@@ -4110,7 +4134,7 @@
         <v>registerField(Fields::DIV1, "DIV1", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="149" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B149">
         <v>12</v>
       </c>
@@ -4133,6 +4157,170 @@
       <c r="J149" t="str">
         <f t="shared" si="26"/>
         <v>registerField(Fields::EFU1, "EFU1", 14, 1, 0);</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>145</v>
+      </c>
+      <c r="B151">
+        <v>0</v>
+      </c>
+      <c r="C151" t="s">
+        <v>146</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>16</v>
+      </c>
+      <c r="F151">
+        <v>0</v>
+      </c>
+      <c r="H151" t="str">
+        <f>"class IOPDmacChannelRegister_"&amp;A151&amp;"_t;"</f>
+        <v>class IOPDmacChannelRegister_BCR_t;</v>
+      </c>
+      <c r="I151" t="str">
+        <f t="shared" ref="I151" si="27">"static constexpr u8 "&amp;C151&amp;" = "&amp;B151&amp;";"</f>
+        <v>static constexpr u8 BS = 0;</v>
+      </c>
+      <c r="J151" t="str">
+        <f t="shared" ref="J151" si="28">"registerField(Fields::"&amp;C151&amp;", """&amp;C151&amp;""", "&amp;D151&amp;", "&amp;E151&amp;", "&amp;F151&amp;");"</f>
+        <v>registerField(Fields::BS, "BS", 0, 16, 0);</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B152">
+        <v>1</v>
+      </c>
+      <c r="C152" t="s">
+        <v>147</v>
+      </c>
+      <c r="D152">
+        <v>16</v>
+      </c>
+      <c r="E152">
+        <v>16</v>
+      </c>
+      <c r="F152">
+        <v>0</v>
+      </c>
+      <c r="I152" t="str">
+        <f t="shared" ref="I152" si="29">"static constexpr u8 "&amp;C152&amp;" = "&amp;B152&amp;";"</f>
+        <v>static constexpr u8 BA = 1;</v>
+      </c>
+      <c r="J152" t="str">
+        <f t="shared" ref="J152" si="30">"registerField(Fields::"&amp;C152&amp;", """&amp;C152&amp;""", "&amp;D152&amp;", "&amp;E152&amp;", "&amp;F152&amp;");"</f>
+        <v>registerField(Fields::BA, "BA", 16, 16, 0);</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>148</v>
+      </c>
+      <c r="B154">
+        <v>0</v>
+      </c>
+      <c r="C154" t="s">
+        <v>149</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+      <c r="E154">
+        <v>1</v>
+      </c>
+      <c r="F154">
+        <v>0</v>
+      </c>
+      <c r="H154" t="str">
+        <f>"class IOPDmacChannelRegister_"&amp;A154&amp;"_t;"</f>
+        <v>class IOPDmacChannelRegister_CHCR_t;</v>
+      </c>
+      <c r="I154" t="str">
+        <f t="shared" ref="I154" si="31">"static constexpr u8 "&amp;C154&amp;" = "&amp;B154&amp;";"</f>
+        <v>static constexpr u8 DR = 0;</v>
+      </c>
+      <c r="J154" t="str">
+        <f t="shared" ref="J154" si="32">"registerField(Fields::"&amp;C154&amp;", """&amp;C154&amp;""", "&amp;D154&amp;", "&amp;E154&amp;", "&amp;F154&amp;");"</f>
+        <v>registerField(Fields::DR, "DR", 0, 1, 0);</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B155">
+        <v>1</v>
+      </c>
+      <c r="C155" t="s">
+        <v>150</v>
+      </c>
+      <c r="D155">
+        <v>9</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+      <c r="F155">
+        <v>0</v>
+      </c>
+      <c r="I155" t="str">
+        <f t="shared" ref="I155:I158" si="33">"static constexpr u8 "&amp;C155&amp;" = "&amp;B155&amp;";"</f>
+        <v>static constexpr u8 CO = 1;</v>
+      </c>
+      <c r="J155" t="str">
+        <f t="shared" ref="J155:J158" si="34">"registerField(Fields::"&amp;C155&amp;", """&amp;C155&amp;""", "&amp;D155&amp;", "&amp;E155&amp;", "&amp;F155&amp;");"</f>
+        <v>registerField(Fields::CO, "CO", 9, 1, 0);</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B156">
+        <v>2</v>
+      </c>
+      <c r="C156" t="s">
+        <v>151</v>
+      </c>
+      <c r="D156">
+        <v>10</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+      <c r="F156">
+        <v>0</v>
+      </c>
+      <c r="I156" t="str">
+        <f t="shared" si="33"/>
+        <v>static constexpr u8 LI = 2;</v>
+      </c>
+      <c r="J156" t="str">
+        <f t="shared" si="34"/>
+        <v>registerField(Fields::LI, "LI", 10, 1, 0);</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B157">
+        <v>3</v>
+      </c>
+      <c r="C157" t="s">
+        <v>152</v>
+      </c>
+      <c r="D157">
+        <v>24</v>
+      </c>
+      <c r="E157">
+        <v>1</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+      <c r="I157" t="str">
+        <f t="shared" si="33"/>
+        <v>static constexpr u8 TR = 3;</v>
+      </c>
+      <c r="J157" t="str">
+        <f t="shared" si="34"/>
+        <v>registerField(Fields::TR, "TR", 24, 1, 0);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial IOP INTC (INTR?) commit - still to decypher bitfields within the registers.
</commit_message>
<xml_diff>
--- a/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
+++ b/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="164">
   <si>
     <t>Field Name</t>
   </si>
@@ -483,6 +483,39 @@
   </si>
   <si>
     <t>TR</t>
+  </si>
+  <si>
+    <t>VBLNK</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>CDROM</t>
+  </si>
+  <si>
+    <t>DMA</t>
+  </si>
+  <si>
+    <t>TMR0</t>
+  </si>
+  <si>
+    <t>TMR1</t>
+  </si>
+  <si>
+    <t>TMR2</t>
+  </si>
+  <si>
+    <t>SIO</t>
+  </si>
+  <si>
+    <t>SPU</t>
+  </si>
+  <si>
+    <t>PIO</t>
+  </si>
+  <si>
+    <t>CON_MC</t>
   </si>
 </sst>
 </file>
@@ -800,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J157"/>
+  <dimension ref="A1:J181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I137" workbookViewId="0">
-      <selection activeCell="J154" sqref="J154:J157"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="B171" sqref="B171:J182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4265,11 +4298,11 @@
         <v>0</v>
       </c>
       <c r="I155" t="str">
-        <f t="shared" ref="I155:I158" si="33">"static constexpr u8 "&amp;C155&amp;" = "&amp;B155&amp;";"</f>
+        <f t="shared" ref="I155:I157" si="33">"static constexpr u8 "&amp;C155&amp;" = "&amp;B155&amp;";"</f>
         <v>static constexpr u8 CO = 1;</v>
       </c>
       <c r="J155" t="str">
-        <f t="shared" ref="J155:J158" si="34">"registerField(Fields::"&amp;C155&amp;", """&amp;C155&amp;""", "&amp;D155&amp;", "&amp;E155&amp;", "&amp;F155&amp;");"</f>
+        <f t="shared" ref="J155:J157" si="34">"registerField(Fields::"&amp;C155&amp;", """&amp;C155&amp;""", "&amp;D155&amp;", "&amp;E155&amp;", "&amp;F155&amp;");"</f>
         <v>registerField(Fields::CO, "CO", 9, 1, 0);</v>
       </c>
     </row>
@@ -4321,6 +4354,570 @@
       <c r="J157" t="str">
         <f t="shared" si="34"/>
         <v>registerField(Fields::TR, "TR", 24, 1, 0);</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>44</v>
+      </c>
+      <c r="B159">
+        <v>0</v>
+      </c>
+      <c r="C159" t="s">
+        <v>153</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+      <c r="E159">
+        <v>1</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+      <c r="H159" t="str">
+        <f>"class IOPDmacChannelRegister_"&amp;A159&amp;"_t;"</f>
+        <v>class IOPDmacChannelRegister_STAT_t;</v>
+      </c>
+      <c r="I159" t="str">
+        <f t="shared" ref="I159" si="35">"static constexpr u8 "&amp;C159&amp;" = "&amp;B159&amp;";"</f>
+        <v>static constexpr u8 VBLNK = 0;</v>
+      </c>
+      <c r="J159" t="str">
+        <f t="shared" ref="J159" si="36">"registerField(Fields::"&amp;C159&amp;", """&amp;C159&amp;""", "&amp;D159&amp;", "&amp;E159&amp;", "&amp;F159&amp;");"</f>
+        <v>registerField(Fields::VBLNK, "VBLNK", 0, 1, 0);</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B160">
+        <v>1</v>
+      </c>
+      <c r="C160" t="s">
+        <v>154</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+      <c r="E160">
+        <v>1</v>
+      </c>
+      <c r="F160">
+        <v>0</v>
+      </c>
+      <c r="I160" t="str">
+        <f t="shared" ref="I160:I169" si="37">"static constexpr u8 "&amp;C160&amp;" = "&amp;B160&amp;";"</f>
+        <v>static constexpr u8 GPU = 1;</v>
+      </c>
+      <c r="J160" t="str">
+        <f t="shared" ref="J160:J169" si="38">"registerField(Fields::"&amp;C160&amp;", """&amp;C160&amp;""", "&amp;D160&amp;", "&amp;E160&amp;", "&amp;F160&amp;");"</f>
+        <v>registerField(Fields::GPU, "GPU", 1, 1, 0);</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B161">
+        <v>2</v>
+      </c>
+      <c r="C161" t="s">
+        <v>155</v>
+      </c>
+      <c r="D161">
+        <v>2</v>
+      </c>
+      <c r="E161">
+        <v>1</v>
+      </c>
+      <c r="F161">
+        <v>0</v>
+      </c>
+      <c r="I161" t="str">
+        <f t="shared" si="37"/>
+        <v>static constexpr u8 CDROM = 2;</v>
+      </c>
+      <c r="J161" t="str">
+        <f t="shared" si="38"/>
+        <v>registerField(Fields::CDROM, "CDROM", 2, 1, 0);</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B162">
+        <v>3</v>
+      </c>
+      <c r="C162" t="s">
+        <v>156</v>
+      </c>
+      <c r="D162">
+        <v>3</v>
+      </c>
+      <c r="E162">
+        <v>1</v>
+      </c>
+      <c r="F162">
+        <v>0</v>
+      </c>
+      <c r="I162" t="str">
+        <f t="shared" si="37"/>
+        <v>static constexpr u8 DMA = 3;</v>
+      </c>
+      <c r="J162" t="str">
+        <f t="shared" si="38"/>
+        <v>registerField(Fields::DMA, "DMA", 3, 1, 0);</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B163">
+        <v>4</v>
+      </c>
+      <c r="C163" t="s">
+        <v>157</v>
+      </c>
+      <c r="D163">
+        <v>4</v>
+      </c>
+      <c r="E163">
+        <v>1</v>
+      </c>
+      <c r="F163">
+        <v>0</v>
+      </c>
+      <c r="I163" t="str">
+        <f t="shared" si="37"/>
+        <v>static constexpr u8 TMR0 = 4;</v>
+      </c>
+      <c r="J163" t="str">
+        <f t="shared" si="38"/>
+        <v>registerField(Fields::TMR0, "TMR0", 4, 1, 0);</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B164">
+        <v>5</v>
+      </c>
+      <c r="C164" t="s">
+        <v>158</v>
+      </c>
+      <c r="D164">
+        <v>5</v>
+      </c>
+      <c r="E164">
+        <v>1</v>
+      </c>
+      <c r="F164">
+        <v>0</v>
+      </c>
+      <c r="I164" t="str">
+        <f t="shared" si="37"/>
+        <v>static constexpr u8 TMR1 = 5;</v>
+      </c>
+      <c r="J164" t="str">
+        <f t="shared" si="38"/>
+        <v>registerField(Fields::TMR1, "TMR1", 5, 1, 0);</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B165">
+        <v>6</v>
+      </c>
+      <c r="C165" t="s">
+        <v>159</v>
+      </c>
+      <c r="D165">
+        <v>6</v>
+      </c>
+      <c r="E165">
+        <v>1</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
+      </c>
+      <c r="I165" t="str">
+        <f t="shared" si="37"/>
+        <v>static constexpr u8 TMR2 = 6;</v>
+      </c>
+      <c r="J165" t="str">
+        <f t="shared" si="38"/>
+        <v>registerField(Fields::TMR2, "TMR2", 6, 1, 0);</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B166">
+        <v>7</v>
+      </c>
+      <c r="C166" t="s">
+        <v>163</v>
+      </c>
+      <c r="D166">
+        <v>7</v>
+      </c>
+      <c r="E166">
+        <v>1</v>
+      </c>
+      <c r="F166">
+        <v>0</v>
+      </c>
+      <c r="I166" t="str">
+        <f t="shared" si="37"/>
+        <v>static constexpr u8 CON_MC = 7;</v>
+      </c>
+      <c r="J166" t="str">
+        <f t="shared" si="38"/>
+        <v>registerField(Fields::CON_MC, "CON_MC", 7, 1, 0);</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B167">
+        <v>8</v>
+      </c>
+      <c r="C167" t="s">
+        <v>160</v>
+      </c>
+      <c r="D167">
+        <v>8</v>
+      </c>
+      <c r="E167">
+        <v>1</v>
+      </c>
+      <c r="F167">
+        <v>0</v>
+      </c>
+      <c r="I167" t="str">
+        <f t="shared" si="37"/>
+        <v>static constexpr u8 SIO = 8;</v>
+      </c>
+      <c r="J167" t="str">
+        <f t="shared" si="38"/>
+        <v>registerField(Fields::SIO, "SIO", 8, 1, 0);</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B168">
+        <v>9</v>
+      </c>
+      <c r="C168" t="s">
+        <v>161</v>
+      </c>
+      <c r="D168">
+        <v>9</v>
+      </c>
+      <c r="E168">
+        <v>1</v>
+      </c>
+      <c r="F168">
+        <v>0</v>
+      </c>
+      <c r="I168" t="str">
+        <f t="shared" si="37"/>
+        <v>static constexpr u8 SPU = 9;</v>
+      </c>
+      <c r="J168" t="str">
+        <f t="shared" si="38"/>
+        <v>registerField(Fields::SPU, "SPU", 9, 1, 0);</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B169">
+        <v>10</v>
+      </c>
+      <c r="C169" t="s">
+        <v>162</v>
+      </c>
+      <c r="D169">
+        <v>10</v>
+      </c>
+      <c r="E169">
+        <v>1</v>
+      </c>
+      <c r="F169">
+        <v>0</v>
+      </c>
+      <c r="I169" t="str">
+        <f t="shared" si="37"/>
+        <v>static constexpr u8 PIO = 10;</v>
+      </c>
+      <c r="J169" t="str">
+        <f t="shared" si="38"/>
+        <v>registerField(Fields::PIO, "PIO", 10, 1, 0);</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>13</v>
+      </c>
+      <c r="B171">
+        <v>0</v>
+      </c>
+      <c r="C171" t="s">
+        <v>153</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171">
+        <v>1</v>
+      </c>
+      <c r="F171">
+        <v>0</v>
+      </c>
+      <c r="H171" t="str">
+        <f>"class IOPDmacChannelRegister_"&amp;A171&amp;"_t;"</f>
+        <v>class IOPDmacChannelRegister_MASK_t;</v>
+      </c>
+      <c r="I171" t="str">
+        <f t="shared" ref="I171:I181" si="39">"static constexpr u8 "&amp;C171&amp;" = "&amp;B171&amp;";"</f>
+        <v>static constexpr u8 VBLNK = 0;</v>
+      </c>
+      <c r="J171" t="str">
+        <f t="shared" ref="J171:J181" si="40">"registerField(Fields::"&amp;C171&amp;", """&amp;C171&amp;""", "&amp;D171&amp;", "&amp;E171&amp;", "&amp;F171&amp;");"</f>
+        <v>registerField(Fields::VBLNK, "VBLNK", 0, 1, 0);</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B172">
+        <v>1</v>
+      </c>
+      <c r="C172" t="s">
+        <v>154</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+      <c r="E172">
+        <v>1</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+      <c r="I172" t="str">
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 GPU = 1;</v>
+      </c>
+      <c r="J172" t="str">
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::GPU, "GPU", 1, 1, 0);</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B173">
+        <v>2</v>
+      </c>
+      <c r="C173" t="s">
+        <v>155</v>
+      </c>
+      <c r="D173">
+        <v>2</v>
+      </c>
+      <c r="E173">
+        <v>1</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+      <c r="I173" t="str">
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 CDROM = 2;</v>
+      </c>
+      <c r="J173" t="str">
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::CDROM, "CDROM", 2, 1, 0);</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B174">
+        <v>3</v>
+      </c>
+      <c r="C174" t="s">
+        <v>156</v>
+      </c>
+      <c r="D174">
+        <v>3</v>
+      </c>
+      <c r="E174">
+        <v>1</v>
+      </c>
+      <c r="F174">
+        <v>0</v>
+      </c>
+      <c r="I174" t="str">
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 DMA = 3;</v>
+      </c>
+      <c r="J174" t="str">
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::DMA, "DMA", 3, 1, 0);</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B175">
+        <v>4</v>
+      </c>
+      <c r="C175" t="s">
+        <v>157</v>
+      </c>
+      <c r="D175">
+        <v>4</v>
+      </c>
+      <c r="E175">
+        <v>1</v>
+      </c>
+      <c r="F175">
+        <v>0</v>
+      </c>
+      <c r="I175" t="str">
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 TMR0 = 4;</v>
+      </c>
+      <c r="J175" t="str">
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::TMR0, "TMR0", 4, 1, 0);</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B176">
+        <v>5</v>
+      </c>
+      <c r="C176" t="s">
+        <v>158</v>
+      </c>
+      <c r="D176">
+        <v>5</v>
+      </c>
+      <c r="E176">
+        <v>1</v>
+      </c>
+      <c r="F176">
+        <v>0</v>
+      </c>
+      <c r="I176" t="str">
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 TMR1 = 5;</v>
+      </c>
+      <c r="J176" t="str">
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::TMR1, "TMR1", 5, 1, 0);</v>
+      </c>
+    </row>
+    <row r="177" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B177">
+        <v>6</v>
+      </c>
+      <c r="C177" t="s">
+        <v>159</v>
+      </c>
+      <c r="D177">
+        <v>6</v>
+      </c>
+      <c r="E177">
+        <v>1</v>
+      </c>
+      <c r="F177">
+        <v>0</v>
+      </c>
+      <c r="I177" t="str">
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 TMR2 = 6;</v>
+      </c>
+      <c r="J177" t="str">
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::TMR2, "TMR2", 6, 1, 0);</v>
+      </c>
+    </row>
+    <row r="178" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B178">
+        <v>7</v>
+      </c>
+      <c r="C178" t="s">
+        <v>163</v>
+      </c>
+      <c r="D178">
+        <v>7</v>
+      </c>
+      <c r="E178">
+        <v>1</v>
+      </c>
+      <c r="F178">
+        <v>0</v>
+      </c>
+      <c r="I178" t="str">
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 CON_MC = 7;</v>
+      </c>
+      <c r="J178" t="str">
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::CON_MC, "CON_MC", 7, 1, 0);</v>
+      </c>
+    </row>
+    <row r="179" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B179">
+        <v>8</v>
+      </c>
+      <c r="C179" t="s">
+        <v>160</v>
+      </c>
+      <c r="D179">
+        <v>8</v>
+      </c>
+      <c r="E179">
+        <v>1</v>
+      </c>
+      <c r="F179">
+        <v>0</v>
+      </c>
+      <c r="I179" t="str">
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 SIO = 8;</v>
+      </c>
+      <c r="J179" t="str">
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::SIO, "SIO", 8, 1, 0);</v>
+      </c>
+    </row>
+    <row r="180" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B180">
+        <v>9</v>
+      </c>
+      <c r="C180" t="s">
+        <v>161</v>
+      </c>
+      <c r="D180">
+        <v>9</v>
+      </c>
+      <c r="E180">
+        <v>1</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+      <c r="I180" t="str">
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 SPU = 9;</v>
+      </c>
+      <c r="J180" t="str">
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::SPU, "SPU", 9, 1, 0);</v>
+      </c>
+    </row>
+    <row r="181" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B181">
+        <v>10</v>
+      </c>
+      <c r="C181" t="s">
+        <v>162</v>
+      </c>
+      <c r="D181">
+        <v>10</v>
+      </c>
+      <c r="E181">
+        <v>1</v>
+      </c>
+      <c r="F181">
+        <v>0</v>
+      </c>
+      <c r="I181" t="str">
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 PIO = 10;</v>
+      </c>
+      <c r="J181" t="str">
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::PIO, "PIO", 10, 1, 0);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP on the IOP Dmac
</commit_message>
<xml_diff>
--- a/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
+++ b/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="201">
   <si>
     <t>Field Name</t>
   </si>
@@ -473,15 +473,6 @@
     <t>CHCR</t>
   </si>
   <si>
-    <t>DR</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>LI</t>
-  </si>
-  <si>
     <t>TR</t>
   </si>
   <si>
@@ -516,6 +507,126 @@
   </si>
   <si>
     <t>CON_MC</t>
+  </si>
+  <si>
+    <t>PCR</t>
+  </si>
+  <si>
+    <t>PRI0</t>
+  </si>
+  <si>
+    <t>PRI1</t>
+  </si>
+  <si>
+    <t>PRI2</t>
+  </si>
+  <si>
+    <t>PRI3</t>
+  </si>
+  <si>
+    <t>PRI4</t>
+  </si>
+  <si>
+    <t>PRI5</t>
+  </si>
+  <si>
+    <t>PRI6</t>
+  </si>
+  <si>
+    <t>ENA0</t>
+  </si>
+  <si>
+    <t>ENA1</t>
+  </si>
+  <si>
+    <t>ENA2</t>
+  </si>
+  <si>
+    <t>ENA3</t>
+  </si>
+  <si>
+    <t>ENA4</t>
+  </si>
+  <si>
+    <t>ENA5</t>
+  </si>
+  <si>
+    <t>ENA6</t>
+  </si>
+  <si>
+    <t>ICR</t>
+  </si>
+  <si>
+    <t>IRQFORCE</t>
+  </si>
+  <si>
+    <t>IRQ0_EN</t>
+  </si>
+  <si>
+    <t>IRQ1_EN</t>
+  </si>
+  <si>
+    <t>IRQ2_EN</t>
+  </si>
+  <si>
+    <t>IRQ3_EN</t>
+  </si>
+  <si>
+    <t>IRQ4_EN</t>
+  </si>
+  <si>
+    <t>IRQ5_EN</t>
+  </si>
+  <si>
+    <t>IRQ6_EN</t>
+  </si>
+  <si>
+    <t>IRQ0_FL</t>
+  </si>
+  <si>
+    <t>IRQ1_FL</t>
+  </si>
+  <si>
+    <t>IRQ2_FL</t>
+  </si>
+  <si>
+    <t>IRQ3_FL</t>
+  </si>
+  <si>
+    <t>IRQ4_FL</t>
+  </si>
+  <si>
+    <t>IRQ5_FL</t>
+  </si>
+  <si>
+    <t>IRQ6_FL</t>
+  </si>
+  <si>
+    <t>IRQMASTER</t>
+  </si>
+  <si>
+    <t>IRQENABLE</t>
+  </si>
+  <si>
+    <t>MAS</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>C_DWS</t>
+  </si>
+  <si>
+    <t>C_CWS</t>
+  </si>
+  <si>
+    <t>START_B</t>
+  </si>
+  <si>
+    <t>START_T</t>
   </si>
 </sst>
 </file>
@@ -833,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J181"/>
+  <dimension ref="A1:J218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="B171" sqref="B171:J182"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="D159" sqref="D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4274,11 +4385,11 @@
       </c>
       <c r="I154" t="str">
         <f t="shared" ref="I154" si="31">"static constexpr u8 "&amp;C154&amp;" = "&amp;B154&amp;";"</f>
-        <v>static constexpr u8 DR = 0;</v>
+        <v>static constexpr u8 TR = 0;</v>
       </c>
       <c r="J154" t="str">
         <f t="shared" ref="J154" si="32">"registerField(Fields::"&amp;C154&amp;", """&amp;C154&amp;""", "&amp;D154&amp;", "&amp;E154&amp;", "&amp;F154&amp;");"</f>
-        <v>registerField(Fields::DR, "DR", 0, 1, 0);</v>
+        <v>registerField(Fields::TR, "TR", 0, 1, 0);</v>
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.3">
@@ -4286,24 +4397,7 @@
         <v>1</v>
       </c>
       <c r="C155" t="s">
-        <v>150</v>
-      </c>
-      <c r="D155">
-        <v>9</v>
-      </c>
-      <c r="E155">
-        <v>1</v>
-      </c>
-      <c r="F155">
-        <v>0</v>
-      </c>
-      <c r="I155" t="str">
-        <f t="shared" ref="I155:I157" si="33">"static constexpr u8 "&amp;C155&amp;" = "&amp;B155&amp;";"</f>
-        <v>static constexpr u8 CO = 1;</v>
-      </c>
-      <c r="J155" t="str">
-        <f t="shared" ref="J155:J157" si="34">"registerField(Fields::"&amp;C155&amp;", """&amp;C155&amp;""", "&amp;D155&amp;", "&amp;E155&amp;", "&amp;F155&amp;");"</f>
-        <v>registerField(Fields::CO, "CO", 9, 1, 0);</v>
+        <v>194</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.3">
@@ -4311,24 +4405,7 @@
         <v>2</v>
       </c>
       <c r="C156" t="s">
-        <v>151</v>
-      </c>
-      <c r="D156">
-        <v>10</v>
-      </c>
-      <c r="E156">
-        <v>1</v>
-      </c>
-      <c r="F156">
-        <v>0</v>
-      </c>
-      <c r="I156" t="str">
-        <f t="shared" si="33"/>
-        <v>static constexpr u8 LI = 2;</v>
-      </c>
-      <c r="J156" t="str">
-        <f t="shared" si="34"/>
-        <v>registerField(Fields::LI, "LI", 10, 1, 0);</v>
+        <v>195</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.3">
@@ -4336,67 +4413,34 @@
         <v>3</v>
       </c>
       <c r="C157" t="s">
-        <v>152</v>
-      </c>
-      <c r="D157">
-        <v>24</v>
-      </c>
-      <c r="E157">
-        <v>1</v>
-      </c>
-      <c r="F157">
-        <v>0</v>
-      </c>
-      <c r="I157" t="str">
-        <f t="shared" si="33"/>
-        <v>static constexpr u8 TR = 3;</v>
-      </c>
-      <c r="J157" t="str">
-        <f t="shared" si="34"/>
-        <v>registerField(Fields::TR, "TR", 24, 1, 0);</v>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B158">
+        <v>4</v>
+      </c>
+      <c r="C158" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
-        <v>44</v>
-      </c>
       <c r="B159">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C159" t="s">
-        <v>153</v>
-      </c>
-      <c r="D159">
-        <v>0</v>
-      </c>
-      <c r="E159">
-        <v>1</v>
-      </c>
-      <c r="F159">
-        <v>0</v>
-      </c>
-      <c r="H159" t="str">
-        <f>"class IOPDmacChannelRegister_"&amp;A159&amp;"_t;"</f>
-        <v>class IOPDmacChannelRegister_STAT_t;</v>
-      </c>
-      <c r="I159" t="str">
-        <f t="shared" ref="I159" si="35">"static constexpr u8 "&amp;C159&amp;" = "&amp;B159&amp;";"</f>
-        <v>static constexpr u8 VBLNK = 0;</v>
-      </c>
-      <c r="J159" t="str">
-        <f t="shared" ref="J159" si="36">"registerField(Fields::"&amp;C159&amp;", """&amp;C159&amp;""", "&amp;D159&amp;", "&amp;E159&amp;", "&amp;F159&amp;");"</f>
-        <v>registerField(Fields::VBLNK, "VBLNK", 0, 1, 0);</v>
+        <v>198</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B160">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>154</v>
+        <v>199</v>
       </c>
       <c r="D160">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E160">
         <v>1</v>
@@ -4404,520 +4448,1374 @@
       <c r="F160">
         <v>0</v>
       </c>
-      <c r="I160" t="str">
-        <f t="shared" ref="I160:I169" si="37">"static constexpr u8 "&amp;C160&amp;" = "&amp;B160&amp;";"</f>
-        <v>static constexpr u8 GPU = 1;</v>
-      </c>
-      <c r="J160" t="str">
-        <f t="shared" ref="J160:J169" si="38">"registerField(Fields::"&amp;C160&amp;", """&amp;C160&amp;""", "&amp;D160&amp;", "&amp;E160&amp;", "&amp;F160&amp;");"</f>
-        <v>registerField(Fields::GPU, "GPU", 1, 1, 0);</v>
+      <c r="I160" t="e">
+        <f>"static constexpr u8 "&amp;#REF!&amp;" = "&amp;#REF!&amp;";"</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J160" t="e">
+        <f>"registerField(Fields::"&amp;#REF!&amp;", """&amp;#REF!&amp;""", "&amp;D160&amp;", "&amp;E160&amp;", "&amp;F160&amp;");"</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B161">
+        <v>7</v>
+      </c>
+      <c r="C161" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>44</v>
+      </c>
+      <c r="B163">
+        <v>0</v>
+      </c>
+      <c r="C163" t="s">
+        <v>150</v>
+      </c>
+      <c r="D163">
+        <v>0</v>
+      </c>
+      <c r="E163">
+        <v>1</v>
+      </c>
+      <c r="F163">
+        <v>0</v>
+      </c>
+      <c r="H163" t="str">
+        <f>"class IOPDmacChannelRegister_"&amp;A163&amp;"_t;"</f>
+        <v>class IOPDmacChannelRegister_STAT_t;</v>
+      </c>
+      <c r="I163" t="str">
+        <f t="shared" ref="I163" si="33">"static constexpr u8 "&amp;C163&amp;" = "&amp;B163&amp;";"</f>
+        <v>static constexpr u8 VBLNK = 0;</v>
+      </c>
+      <c r="J163" t="str">
+        <f t="shared" ref="J163" si="34">"registerField(Fields::"&amp;C163&amp;", """&amp;C163&amp;""", "&amp;D163&amp;", "&amp;E163&amp;", "&amp;F163&amp;");"</f>
+        <v>registerField(Fields::VBLNK, "VBLNK", 0, 1, 0);</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B164">
+        <v>1</v>
+      </c>
+      <c r="C164" t="s">
+        <v>151</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+      <c r="E164">
+        <v>1</v>
+      </c>
+      <c r="F164">
+        <v>0</v>
+      </c>
+      <c r="I164" t="str">
+        <f t="shared" ref="I164:I173" si="35">"static constexpr u8 "&amp;C164&amp;" = "&amp;B164&amp;";"</f>
+        <v>static constexpr u8 GPU = 1;</v>
+      </c>
+      <c r="J164" t="str">
+        <f t="shared" ref="J164:J173" si="36">"registerField(Fields::"&amp;C164&amp;", """&amp;C164&amp;""", "&amp;D164&amp;", "&amp;E164&amp;", "&amp;F164&amp;");"</f>
+        <v>registerField(Fields::GPU, "GPU", 1, 1, 0);</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B165">
         <v>2</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C165" t="s">
+        <v>152</v>
+      </c>
+      <c r="D165">
+        <v>2</v>
+      </c>
+      <c r="E165">
+        <v>1</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
+      </c>
+      <c r="I165" t="str">
+        <f t="shared" si="35"/>
+        <v>static constexpr u8 CDROM = 2;</v>
+      </c>
+      <c r="J165" t="str">
+        <f t="shared" si="36"/>
+        <v>registerField(Fields::CDROM, "CDROM", 2, 1, 0);</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B166">
+        <v>3</v>
+      </c>
+      <c r="C166" t="s">
+        <v>153</v>
+      </c>
+      <c r="D166">
+        <v>3</v>
+      </c>
+      <c r="E166">
+        <v>1</v>
+      </c>
+      <c r="F166">
+        <v>0</v>
+      </c>
+      <c r="I166" t="str">
+        <f t="shared" si="35"/>
+        <v>static constexpr u8 DMA = 3;</v>
+      </c>
+      <c r="J166" t="str">
+        <f t="shared" si="36"/>
+        <v>registerField(Fields::DMA, "DMA", 3, 1, 0);</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B167">
+        <v>4</v>
+      </c>
+      <c r="C167" t="s">
+        <v>154</v>
+      </c>
+      <c r="D167">
+        <v>4</v>
+      </c>
+      <c r="E167">
+        <v>1</v>
+      </c>
+      <c r="F167">
+        <v>0</v>
+      </c>
+      <c r="I167" t="str">
+        <f t="shared" si="35"/>
+        <v>static constexpr u8 TMR0 = 4;</v>
+      </c>
+      <c r="J167" t="str">
+        <f t="shared" si="36"/>
+        <v>registerField(Fields::TMR0, "TMR0", 4, 1, 0);</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B168">
+        <v>5</v>
+      </c>
+      <c r="C168" t="s">
         <v>155</v>
       </c>
-      <c r="D161">
+      <c r="D168">
+        <v>5</v>
+      </c>
+      <c r="E168">
+        <v>1</v>
+      </c>
+      <c r="F168">
+        <v>0</v>
+      </c>
+      <c r="I168" t="str">
+        <f t="shared" si="35"/>
+        <v>static constexpr u8 TMR1 = 5;</v>
+      </c>
+      <c r="J168" t="str">
+        <f t="shared" si="36"/>
+        <v>registerField(Fields::TMR1, "TMR1", 5, 1, 0);</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B169">
+        <v>6</v>
+      </c>
+      <c r="C169" t="s">
+        <v>156</v>
+      </c>
+      <c r="D169">
+        <v>6</v>
+      </c>
+      <c r="E169">
+        <v>1</v>
+      </c>
+      <c r="F169">
+        <v>0</v>
+      </c>
+      <c r="I169" t="str">
+        <f t="shared" si="35"/>
+        <v>static constexpr u8 TMR2 = 6;</v>
+      </c>
+      <c r="J169" t="str">
+        <f t="shared" si="36"/>
+        <v>registerField(Fields::TMR2, "TMR2", 6, 1, 0);</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B170">
+        <v>7</v>
+      </c>
+      <c r="C170" t="s">
+        <v>160</v>
+      </c>
+      <c r="D170">
+        <v>7</v>
+      </c>
+      <c r="E170">
+        <v>1</v>
+      </c>
+      <c r="F170">
+        <v>0</v>
+      </c>
+      <c r="I170" t="str">
+        <f t="shared" si="35"/>
+        <v>static constexpr u8 CON_MC = 7;</v>
+      </c>
+      <c r="J170" t="str">
+        <f t="shared" si="36"/>
+        <v>registerField(Fields::CON_MC, "CON_MC", 7, 1, 0);</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B171">
+        <v>8</v>
+      </c>
+      <c r="C171" t="s">
+        <v>157</v>
+      </c>
+      <c r="D171">
+        <v>8</v>
+      </c>
+      <c r="E171">
+        <v>1</v>
+      </c>
+      <c r="F171">
+        <v>0</v>
+      </c>
+      <c r="I171" t="str">
+        <f t="shared" si="35"/>
+        <v>static constexpr u8 SIO = 8;</v>
+      </c>
+      <c r="J171" t="str">
+        <f t="shared" si="36"/>
+        <v>registerField(Fields::SIO, "SIO", 8, 1, 0);</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B172">
+        <v>9</v>
+      </c>
+      <c r="C172" t="s">
+        <v>158</v>
+      </c>
+      <c r="D172">
+        <v>9</v>
+      </c>
+      <c r="E172">
+        <v>1</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+      <c r="I172" t="str">
+        <f t="shared" si="35"/>
+        <v>static constexpr u8 SPU = 9;</v>
+      </c>
+      <c r="J172" t="str">
+        <f t="shared" si="36"/>
+        <v>registerField(Fields::SPU, "SPU", 9, 1, 0);</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B173">
+        <v>10</v>
+      </c>
+      <c r="C173" t="s">
+        <v>159</v>
+      </c>
+      <c r="D173">
+        <v>10</v>
+      </c>
+      <c r="E173">
+        <v>1</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+      <c r="I173" t="str">
+        <f t="shared" si="35"/>
+        <v>static constexpr u8 PIO = 10;</v>
+      </c>
+      <c r="J173" t="str">
+        <f t="shared" si="36"/>
+        <v>registerField(Fields::PIO, "PIO", 10, 1, 0);</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>13</v>
+      </c>
+      <c r="B175">
+        <v>0</v>
+      </c>
+      <c r="C175" t="s">
+        <v>150</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175">
+        <v>1</v>
+      </c>
+      <c r="F175">
+        <v>0</v>
+      </c>
+      <c r="H175" t="str">
+        <f>"class IOPDmacChannelRegister_"&amp;A175&amp;"_t;"</f>
+        <v>class IOPDmacChannelRegister_MASK_t;</v>
+      </c>
+      <c r="I175" t="str">
+        <f t="shared" ref="I175:I185" si="37">"static constexpr u8 "&amp;C175&amp;" = "&amp;B175&amp;";"</f>
+        <v>static constexpr u8 VBLNK = 0;</v>
+      </c>
+      <c r="J175" t="str">
+        <f t="shared" ref="J175:J185" si="38">"registerField(Fields::"&amp;C175&amp;", """&amp;C175&amp;""", "&amp;D175&amp;", "&amp;E175&amp;", "&amp;F175&amp;");"</f>
+        <v>registerField(Fields::VBLNK, "VBLNK", 0, 1, 0);</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B176">
+        <v>1</v>
+      </c>
+      <c r="C176" t="s">
+        <v>151</v>
+      </c>
+      <c r="D176">
+        <v>1</v>
+      </c>
+      <c r="E176">
+        <v>1</v>
+      </c>
+      <c r="F176">
+        <v>0</v>
+      </c>
+      <c r="I176" t="str">
+        <f t="shared" si="37"/>
+        <v>static constexpr u8 GPU = 1;</v>
+      </c>
+      <c r="J176" t="str">
+        <f t="shared" si="38"/>
+        <v>registerField(Fields::GPU, "GPU", 1, 1, 0);</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B177">
         <v>2</v>
       </c>
-      <c r="E161">
-        <v>1</v>
-      </c>
-      <c r="F161">
-        <v>0</v>
-      </c>
-      <c r="I161" t="str">
+      <c r="C177" t="s">
+        <v>152</v>
+      </c>
+      <c r="D177">
+        <v>2</v>
+      </c>
+      <c r="E177">
+        <v>1</v>
+      </c>
+      <c r="F177">
+        <v>0</v>
+      </c>
+      <c r="I177" t="str">
         <f t="shared" si="37"/>
         <v>static constexpr u8 CDROM = 2;</v>
       </c>
-      <c r="J161" t="str">
+      <c r="J177" t="str">
         <f t="shared" si="38"/>
         <v>registerField(Fields::CDROM, "CDROM", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B162">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B178">
         <v>3</v>
       </c>
-      <c r="C162" t="s">
-        <v>156</v>
-      </c>
-      <c r="D162">
+      <c r="C178" t="s">
+        <v>153</v>
+      </c>
+      <c r="D178">
         <v>3</v>
       </c>
-      <c r="E162">
-        <v>1</v>
-      </c>
-      <c r="F162">
-        <v>0</v>
-      </c>
-      <c r="I162" t="str">
+      <c r="E178">
+        <v>1</v>
+      </c>
+      <c r="F178">
+        <v>0</v>
+      </c>
+      <c r="I178" t="str">
         <f t="shared" si="37"/>
         <v>static constexpr u8 DMA = 3;</v>
       </c>
-      <c r="J162" t="str">
+      <c r="J178" t="str">
         <f t="shared" si="38"/>
         <v>registerField(Fields::DMA, "DMA", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B163">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B179">
         <v>4</v>
       </c>
-      <c r="C163" t="s">
-        <v>157</v>
-      </c>
-      <c r="D163">
+      <c r="C179" t="s">
+        <v>154</v>
+      </c>
+      <c r="D179">
         <v>4</v>
       </c>
-      <c r="E163">
-        <v>1</v>
-      </c>
-      <c r="F163">
-        <v>0</v>
-      </c>
-      <c r="I163" t="str">
+      <c r="E179">
+        <v>1</v>
+      </c>
+      <c r="F179">
+        <v>0</v>
+      </c>
+      <c r="I179" t="str">
         <f t="shared" si="37"/>
         <v>static constexpr u8 TMR0 = 4;</v>
       </c>
-      <c r="J163" t="str">
+      <c r="J179" t="str">
         <f t="shared" si="38"/>
         <v>registerField(Fields::TMR0, "TMR0", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B164">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B180">
         <v>5</v>
       </c>
-      <c r="C164" t="s">
-        <v>158</v>
-      </c>
-      <c r="D164">
+      <c r="C180" t="s">
+        <v>155</v>
+      </c>
+      <c r="D180">
         <v>5</v>
       </c>
-      <c r="E164">
-        <v>1</v>
-      </c>
-      <c r="F164">
-        <v>0</v>
-      </c>
-      <c r="I164" t="str">
+      <c r="E180">
+        <v>1</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+      <c r="I180" t="str">
         <f t="shared" si="37"/>
         <v>static constexpr u8 TMR1 = 5;</v>
       </c>
-      <c r="J164" t="str">
+      <c r="J180" t="str">
         <f t="shared" si="38"/>
         <v>registerField(Fields::TMR1, "TMR1", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B165">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B181">
         <v>6</v>
       </c>
-      <c r="C165" t="s">
-        <v>159</v>
-      </c>
-      <c r="D165">
+      <c r="C181" t="s">
+        <v>156</v>
+      </c>
+      <c r="D181">
         <v>6</v>
       </c>
-      <c r="E165">
-        <v>1</v>
-      </c>
-      <c r="F165">
-        <v>0</v>
-      </c>
-      <c r="I165" t="str">
+      <c r="E181">
+        <v>1</v>
+      </c>
+      <c r="F181">
+        <v>0</v>
+      </c>
+      <c r="I181" t="str">
         <f t="shared" si="37"/>
         <v>static constexpr u8 TMR2 = 6;</v>
       </c>
-      <c r="J165" t="str">
+      <c r="J181" t="str">
         <f t="shared" si="38"/>
         <v>registerField(Fields::TMR2, "TMR2", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B166">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B182">
         <v>7</v>
       </c>
-      <c r="C166" t="s">
-        <v>163</v>
-      </c>
-      <c r="D166">
+      <c r="C182" t="s">
+        <v>160</v>
+      </c>
+      <c r="D182">
         <v>7</v>
       </c>
-      <c r="E166">
-        <v>1</v>
-      </c>
-      <c r="F166">
-        <v>0</v>
-      </c>
-      <c r="I166" t="str">
+      <c r="E182">
+        <v>1</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+      <c r="I182" t="str">
         <f t="shared" si="37"/>
         <v>static constexpr u8 CON_MC = 7;</v>
       </c>
-      <c r="J166" t="str">
+      <c r="J182" t="str">
         <f t="shared" si="38"/>
         <v>registerField(Fields::CON_MC, "CON_MC", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B167">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B183">
         <v>8</v>
       </c>
-      <c r="C167" t="s">
-        <v>160</v>
-      </c>
-      <c r="D167">
+      <c r="C183" t="s">
+        <v>157</v>
+      </c>
+      <c r="D183">
         <v>8</v>
       </c>
-      <c r="E167">
-        <v>1</v>
-      </c>
-      <c r="F167">
-        <v>0</v>
-      </c>
-      <c r="I167" t="str">
+      <c r="E183">
+        <v>1</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+      <c r="I183" t="str">
         <f t="shared" si="37"/>
         <v>static constexpr u8 SIO = 8;</v>
       </c>
-      <c r="J167" t="str">
+      <c r="J183" t="str">
         <f t="shared" si="38"/>
         <v>registerField(Fields::SIO, "SIO", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B168">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B184">
         <v>9</v>
       </c>
-      <c r="C168" t="s">
-        <v>161</v>
-      </c>
-      <c r="D168">
+      <c r="C184" t="s">
+        <v>158</v>
+      </c>
+      <c r="D184">
         <v>9</v>
       </c>
-      <c r="E168">
-        <v>1</v>
-      </c>
-      <c r="F168">
-        <v>0</v>
-      </c>
-      <c r="I168" t="str">
+      <c r="E184">
+        <v>1</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+      <c r="I184" t="str">
         <f t="shared" si="37"/>
         <v>static constexpr u8 SPU = 9;</v>
       </c>
-      <c r="J168" t="str">
+      <c r="J184" t="str">
         <f t="shared" si="38"/>
         <v>registerField(Fields::SPU, "SPU", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B169">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B185">
         <v>10</v>
       </c>
-      <c r="C169" t="s">
-        <v>162</v>
-      </c>
-      <c r="D169">
+      <c r="C185" t="s">
+        <v>159</v>
+      </c>
+      <c r="D185">
         <v>10</v>
       </c>
-      <c r="E169">
-        <v>1</v>
-      </c>
-      <c r="F169">
-        <v>0</v>
-      </c>
-      <c r="I169" t="str">
+      <c r="E185">
+        <v>1</v>
+      </c>
+      <c r="F185">
+        <v>0</v>
+      </c>
+      <c r="I185" t="str">
         <f t="shared" si="37"/>
         <v>static constexpr u8 PIO = 10;</v>
       </c>
-      <c r="J169" t="str">
+      <c r="J185" t="str">
         <f t="shared" si="38"/>
         <v>registerField(Fields::PIO, "PIO", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>161</v>
+      </c>
+      <c r="B187">
+        <v>0</v>
+      </c>
+      <c r="C187" t="s">
+        <v>162</v>
+      </c>
+      <c r="D187">
+        <v>0</v>
+      </c>
+      <c r="E187">
+        <v>3</v>
+      </c>
+      <c r="F187">
+        <v>0</v>
+      </c>
+      <c r="H187" t="str">
+        <f>"class IOPDmacRegister_"&amp;A187&amp;"_t;"</f>
+        <v>class IOPDmacRegister_PCR_t;</v>
+      </c>
+      <c r="I187" t="str">
+        <f t="shared" ref="I187" si="39">"static constexpr u8 "&amp;C187&amp;" = "&amp;B187&amp;";"</f>
+        <v>static constexpr u8 PRI0 = 0;</v>
+      </c>
+      <c r="J187" t="str">
+        <f t="shared" ref="J187" si="40">"registerField(Fields::"&amp;C187&amp;", """&amp;C187&amp;""", "&amp;D187&amp;", "&amp;E187&amp;", "&amp;F187&amp;");"</f>
+        <v>registerField(Fields::PRI0, "PRI0", 0, 3, 0);</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B188">
+        <v>1</v>
+      </c>
+      <c r="C188" t="s">
+        <v>169</v>
+      </c>
+      <c r="D188">
+        <v>3</v>
+      </c>
+      <c r="E188">
+        <v>1</v>
+      </c>
+      <c r="F188">
+        <v>0</v>
+      </c>
+      <c r="I188" t="str">
+        <f t="shared" ref="I188:I200" si="41">"static constexpr u8 "&amp;C188&amp;" = "&amp;B188&amp;";"</f>
+        <v>static constexpr u8 ENA0 = 1;</v>
+      </c>
+      <c r="J188" t="str">
+        <f t="shared" ref="J188:J200" si="42">"registerField(Fields::"&amp;C188&amp;", """&amp;C188&amp;""", "&amp;D188&amp;", "&amp;E188&amp;", "&amp;F188&amp;");"</f>
+        <v>registerField(Fields::ENA0, "ENA0", 3, 1, 0);</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B189">
+        <v>2</v>
+      </c>
+      <c r="C189" t="s">
+        <v>163</v>
+      </c>
+      <c r="D189">
+        <v>4</v>
+      </c>
+      <c r="E189">
+        <v>3</v>
+      </c>
+      <c r="F189">
+        <v>0</v>
+      </c>
+      <c r="I189" t="str">
+        <f t="shared" si="41"/>
+        <v>static constexpr u8 PRI1 = 2;</v>
+      </c>
+      <c r="J189" t="str">
+        <f t="shared" si="42"/>
+        <v>registerField(Fields::PRI1, "PRI1", 4, 3, 0);</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B190">
+        <v>3</v>
+      </c>
+      <c r="C190" t="s">
+        <v>170</v>
+      </c>
+      <c r="D190">
+        <v>7</v>
+      </c>
+      <c r="E190">
+        <v>1</v>
+      </c>
+      <c r="F190">
+        <v>0</v>
+      </c>
+      <c r="I190" t="str">
+        <f t="shared" si="41"/>
+        <v>static constexpr u8 ENA1 = 3;</v>
+      </c>
+      <c r="J190" t="str">
+        <f t="shared" si="42"/>
+        <v>registerField(Fields::ENA1, "ENA1", 7, 1, 0);</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B191">
+        <v>4</v>
+      </c>
+      <c r="C191" t="s">
+        <v>164</v>
+      </c>
+      <c r="D191">
+        <v>8</v>
+      </c>
+      <c r="E191">
+        <v>3</v>
+      </c>
+      <c r="F191">
+        <v>0</v>
+      </c>
+      <c r="I191" t="str">
+        <f t="shared" si="41"/>
+        <v>static constexpr u8 PRI2 = 4;</v>
+      </c>
+      <c r="J191" t="str">
+        <f t="shared" si="42"/>
+        <v>registerField(Fields::PRI2, "PRI2", 8, 3, 0);</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B192">
+        <v>5</v>
+      </c>
+      <c r="C192" t="s">
+        <v>171</v>
+      </c>
+      <c r="D192">
+        <v>11</v>
+      </c>
+      <c r="E192">
+        <v>1</v>
+      </c>
+      <c r="F192">
+        <v>0</v>
+      </c>
+      <c r="I192" t="str">
+        <f t="shared" si="41"/>
+        <v>static constexpr u8 ENA2 = 5;</v>
+      </c>
+      <c r="J192" t="str">
+        <f t="shared" si="42"/>
+        <v>registerField(Fields::ENA2, "ENA2", 11, 1, 0);</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B193">
+        <v>6</v>
+      </c>
+      <c r="C193" t="s">
+        <v>165</v>
+      </c>
+      <c r="D193">
+        <v>12</v>
+      </c>
+      <c r="E193">
+        <v>3</v>
+      </c>
+      <c r="F193">
+        <v>0</v>
+      </c>
+      <c r="I193" t="str">
+        <f t="shared" si="41"/>
+        <v>static constexpr u8 PRI3 = 6;</v>
+      </c>
+      <c r="J193" t="str">
+        <f t="shared" si="42"/>
+        <v>registerField(Fields::PRI3, "PRI3", 12, 3, 0);</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B194">
+        <v>7</v>
+      </c>
+      <c r="C194" t="s">
+        <v>172</v>
+      </c>
+      <c r="D194">
+        <v>15</v>
+      </c>
+      <c r="E194">
+        <v>1</v>
+      </c>
+      <c r="F194">
+        <v>0</v>
+      </c>
+      <c r="I194" t="str">
+        <f t="shared" si="41"/>
+        <v>static constexpr u8 ENA3 = 7;</v>
+      </c>
+      <c r="J194" t="str">
+        <f t="shared" si="42"/>
+        <v>registerField(Fields::ENA3, "ENA3", 15, 1, 0);</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B195">
+        <v>8</v>
+      </c>
+      <c r="C195" t="s">
+        <v>166</v>
+      </c>
+      <c r="D195">
+        <v>16</v>
+      </c>
+      <c r="E195">
+        <v>3</v>
+      </c>
+      <c r="F195">
+        <v>0</v>
+      </c>
+      <c r="I195" t="str">
+        <f t="shared" si="41"/>
+        <v>static constexpr u8 PRI4 = 8;</v>
+      </c>
+      <c r="J195" t="str">
+        <f t="shared" si="42"/>
+        <v>registerField(Fields::PRI4, "PRI4", 16, 3, 0);</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B196">
+        <v>9</v>
+      </c>
+      <c r="C196" t="s">
+        <v>173</v>
+      </c>
+      <c r="D196">
+        <v>19</v>
+      </c>
+      <c r="E196">
+        <v>1</v>
+      </c>
+      <c r="F196">
+        <v>0</v>
+      </c>
+      <c r="I196" t="str">
+        <f t="shared" si="41"/>
+        <v>static constexpr u8 ENA4 = 9;</v>
+      </c>
+      <c r="J196" t="str">
+        <f t="shared" si="42"/>
+        <v>registerField(Fields::ENA4, "ENA4", 19, 1, 0);</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B197">
+        <v>10</v>
+      </c>
+      <c r="C197" t="s">
+        <v>167</v>
+      </c>
+      <c r="D197">
+        <v>20</v>
+      </c>
+      <c r="E197">
+        <v>3</v>
+      </c>
+      <c r="F197">
+        <v>0</v>
+      </c>
+      <c r="I197" t="str">
+        <f t="shared" si="41"/>
+        <v>static constexpr u8 PRI5 = 10;</v>
+      </c>
+      <c r="J197" t="str">
+        <f t="shared" si="42"/>
+        <v>registerField(Fields::PRI5, "PRI5", 20, 3, 0);</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B198">
+        <v>11</v>
+      </c>
+      <c r="C198" t="s">
+        <v>174</v>
+      </c>
+      <c r="D198">
+        <v>23</v>
+      </c>
+      <c r="E198">
+        <v>1</v>
+      </c>
+      <c r="F198">
+        <v>0</v>
+      </c>
+      <c r="I198" t="str">
+        <f t="shared" si="41"/>
+        <v>static constexpr u8 ENA5 = 11;</v>
+      </c>
+      <c r="J198" t="str">
+        <f t="shared" si="42"/>
+        <v>registerField(Fields::ENA5, "ENA5", 23, 1, 0);</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B199">
+        <v>12</v>
+      </c>
+      <c r="C199" t="s">
+        <v>168</v>
+      </c>
+      <c r="D199">
+        <v>24</v>
+      </c>
+      <c r="E199">
+        <v>3</v>
+      </c>
+      <c r="F199">
+        <v>0</v>
+      </c>
+      <c r="I199" t="str">
+        <f t="shared" si="41"/>
+        <v>static constexpr u8 PRI6 = 12;</v>
+      </c>
+      <c r="J199" t="str">
+        <f t="shared" si="42"/>
+        <v>registerField(Fields::PRI6, "PRI6", 24, 3, 0);</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B200">
         <v>13</v>
       </c>
-      <c r="B171">
-        <v>0</v>
-      </c>
-      <c r="C171" t="s">
-        <v>153</v>
-      </c>
-      <c r="D171">
-        <v>0</v>
-      </c>
-      <c r="E171">
-        <v>1</v>
-      </c>
-      <c r="F171">
-        <v>0</v>
-      </c>
-      <c r="H171" t="str">
-        <f>"class IOPDmacChannelRegister_"&amp;A171&amp;"_t;"</f>
-        <v>class IOPDmacChannelRegister_MASK_t;</v>
-      </c>
-      <c r="I171" t="str">
-        <f t="shared" ref="I171:I181" si="39">"static constexpr u8 "&amp;C171&amp;" = "&amp;B171&amp;";"</f>
-        <v>static constexpr u8 VBLNK = 0;</v>
-      </c>
-      <c r="J171" t="str">
-        <f t="shared" ref="J171:J181" si="40">"registerField(Fields::"&amp;C171&amp;", """&amp;C171&amp;""", "&amp;D171&amp;", "&amp;E171&amp;", "&amp;F171&amp;");"</f>
-        <v>registerField(Fields::VBLNK, "VBLNK", 0, 1, 0);</v>
-      </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B172">
-        <v>1</v>
-      </c>
-      <c r="C172" t="s">
-        <v>154</v>
-      </c>
-      <c r="D172">
-        <v>1</v>
-      </c>
-      <c r="E172">
-        <v>1</v>
-      </c>
-      <c r="F172">
-        <v>0</v>
-      </c>
-      <c r="I172" t="str">
-        <f t="shared" si="39"/>
-        <v>static constexpr u8 GPU = 1;</v>
-      </c>
-      <c r="J172" t="str">
-        <f t="shared" si="40"/>
-        <v>registerField(Fields::GPU, "GPU", 1, 1, 0);</v>
-      </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B173">
+      <c r="C200" t="s">
+        <v>175</v>
+      </c>
+      <c r="D200">
+        <v>27</v>
+      </c>
+      <c r="E200">
+        <v>1</v>
+      </c>
+      <c r="F200">
+        <v>0</v>
+      </c>
+      <c r="I200" t="str">
+        <f t="shared" si="41"/>
+        <v>static constexpr u8 ENA6 = 13;</v>
+      </c>
+      <c r="J200" t="str">
+        <f t="shared" si="42"/>
+        <v>registerField(Fields::ENA6, "ENA6", 27, 1, 0);</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>176</v>
+      </c>
+      <c r="B202">
+        <v>0</v>
+      </c>
+      <c r="C202" t="s">
+        <v>177</v>
+      </c>
+      <c r="D202">
+        <v>15</v>
+      </c>
+      <c r="E202">
+        <v>1</v>
+      </c>
+      <c r="F202">
+        <v>0</v>
+      </c>
+      <c r="H202" t="str">
+        <f>"class IOPDmacRegister_"&amp;A202&amp;"_t;"</f>
+        <v>class IOPDmacRegister_ICR_t;</v>
+      </c>
+      <c r="I202" t="str">
+        <f t="shared" ref="I202" si="43">"static constexpr u8 "&amp;C202&amp;" = "&amp;B202&amp;";"</f>
+        <v>static constexpr u8 IRQFORCE = 0;</v>
+      </c>
+      <c r="J202" t="str">
+        <f t="shared" ref="J202" si="44">"registerField(Fields::"&amp;C202&amp;", """&amp;C202&amp;""", "&amp;D202&amp;", "&amp;E202&amp;", "&amp;F202&amp;");"</f>
+        <v>registerField(Fields::IRQFORCE, "IRQFORCE", 15, 1, 0);</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B203">
+        <v>1</v>
+      </c>
+      <c r="C203" t="s">
+        <v>178</v>
+      </c>
+      <c r="D203">
+        <v>16</v>
+      </c>
+      <c r="E203">
+        <v>1</v>
+      </c>
+      <c r="F203">
+        <v>0</v>
+      </c>
+      <c r="I203" t="str">
+        <f t="shared" ref="I203:I218" si="45">"static constexpr u8 "&amp;C203&amp;" = "&amp;B203&amp;";"</f>
+        <v>static constexpr u8 IRQ0_EN = 1;</v>
+      </c>
+      <c r="J203" t="str">
+        <f t="shared" ref="J203:J218" si="46">"registerField(Fields::"&amp;C203&amp;", """&amp;C203&amp;""", "&amp;D203&amp;", "&amp;E203&amp;", "&amp;F203&amp;");"</f>
+        <v>registerField(Fields::IRQ0_EN, "IRQ0_EN", 16, 1, 0);</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B204">
         <v>2</v>
       </c>
-      <c r="C173" t="s">
-        <v>155</v>
-      </c>
-      <c r="D173">
-        <v>2</v>
-      </c>
-      <c r="E173">
-        <v>1</v>
-      </c>
-      <c r="F173">
-        <v>0</v>
-      </c>
-      <c r="I173" t="str">
-        <f t="shared" si="39"/>
-        <v>static constexpr u8 CDROM = 2;</v>
-      </c>
-      <c r="J173" t="str">
-        <f t="shared" si="40"/>
-        <v>registerField(Fields::CDROM, "CDROM", 2, 1, 0);</v>
-      </c>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B174">
+      <c r="C204" t="s">
+        <v>179</v>
+      </c>
+      <c r="D204">
+        <v>17</v>
+      </c>
+      <c r="E204">
+        <v>1</v>
+      </c>
+      <c r="F204">
+        <v>0</v>
+      </c>
+      <c r="I204" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQ1_EN = 2;</v>
+      </c>
+      <c r="J204" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQ1_EN, "IRQ1_EN", 17, 1, 0);</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B205">
         <v>3</v>
       </c>
-      <c r="C174" t="s">
-        <v>156</v>
-      </c>
-      <c r="D174">
-        <v>3</v>
-      </c>
-      <c r="E174">
-        <v>1</v>
-      </c>
-      <c r="F174">
-        <v>0</v>
-      </c>
-      <c r="I174" t="str">
-        <f t="shared" si="39"/>
-        <v>static constexpr u8 DMA = 3;</v>
-      </c>
-      <c r="J174" t="str">
-        <f t="shared" si="40"/>
-        <v>registerField(Fields::DMA, "DMA", 3, 1, 0);</v>
-      </c>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B175">
+      <c r="C205" t="s">
+        <v>180</v>
+      </c>
+      <c r="D205">
+        <v>18</v>
+      </c>
+      <c r="E205">
+        <v>1</v>
+      </c>
+      <c r="F205">
+        <v>0</v>
+      </c>
+      <c r="I205" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQ2_EN = 3;</v>
+      </c>
+      <c r="J205" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQ2_EN, "IRQ2_EN", 18, 1, 0);</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B206">
         <v>4</v>
       </c>
-      <c r="C175" t="s">
-        <v>157</v>
-      </c>
-      <c r="D175">
-        <v>4</v>
-      </c>
-      <c r="E175">
-        <v>1</v>
-      </c>
-      <c r="F175">
-        <v>0</v>
-      </c>
-      <c r="I175" t="str">
-        <f t="shared" si="39"/>
-        <v>static constexpr u8 TMR0 = 4;</v>
-      </c>
-      <c r="J175" t="str">
-        <f t="shared" si="40"/>
-        <v>registerField(Fields::TMR0, "TMR0", 4, 1, 0);</v>
-      </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B176">
+      <c r="C206" t="s">
+        <v>181</v>
+      </c>
+      <c r="D206">
+        <v>19</v>
+      </c>
+      <c r="E206">
+        <v>1</v>
+      </c>
+      <c r="F206">
+        <v>0</v>
+      </c>
+      <c r="I206" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQ3_EN = 4;</v>
+      </c>
+      <c r="J206" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQ3_EN, "IRQ3_EN", 19, 1, 0);</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B207">
         <v>5</v>
       </c>
-      <c r="C176" t="s">
-        <v>158</v>
-      </c>
-      <c r="D176">
-        <v>5</v>
-      </c>
-      <c r="E176">
-        <v>1</v>
-      </c>
-      <c r="F176">
-        <v>0</v>
-      </c>
-      <c r="I176" t="str">
-        <f t="shared" si="39"/>
-        <v>static constexpr u8 TMR1 = 5;</v>
-      </c>
-      <c r="J176" t="str">
-        <f t="shared" si="40"/>
-        <v>registerField(Fields::TMR1, "TMR1", 5, 1, 0);</v>
-      </c>
-    </row>
-    <row r="177" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B177">
+      <c r="C207" t="s">
+        <v>182</v>
+      </c>
+      <c r="D207">
+        <v>20</v>
+      </c>
+      <c r="E207">
+        <v>1</v>
+      </c>
+      <c r="F207">
+        <v>0</v>
+      </c>
+      <c r="I207" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQ4_EN = 5;</v>
+      </c>
+      <c r="J207" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQ4_EN, "IRQ4_EN", 20, 1, 0);</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B208">
         <v>6</v>
       </c>
-      <c r="C177" t="s">
-        <v>159</v>
-      </c>
-      <c r="D177">
-        <v>6</v>
-      </c>
-      <c r="E177">
-        <v>1</v>
-      </c>
-      <c r="F177">
-        <v>0</v>
-      </c>
-      <c r="I177" t="str">
-        <f t="shared" si="39"/>
-        <v>static constexpr u8 TMR2 = 6;</v>
-      </c>
-      <c r="J177" t="str">
-        <f t="shared" si="40"/>
-        <v>registerField(Fields::TMR2, "TMR2", 6, 1, 0);</v>
-      </c>
-    </row>
-    <row r="178" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B178">
+      <c r="C208" t="s">
+        <v>183</v>
+      </c>
+      <c r="D208">
+        <v>21</v>
+      </c>
+      <c r="E208">
+        <v>1</v>
+      </c>
+      <c r="F208">
+        <v>0</v>
+      </c>
+      <c r="I208" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQ5_EN = 6;</v>
+      </c>
+      <c r="J208" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQ5_EN, "IRQ5_EN", 21, 1, 0);</v>
+      </c>
+    </row>
+    <row r="209" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B209">
         <v>7</v>
       </c>
-      <c r="C178" t="s">
-        <v>163</v>
-      </c>
-      <c r="D178">
-        <v>7</v>
-      </c>
-      <c r="E178">
-        <v>1</v>
-      </c>
-      <c r="F178">
-        <v>0</v>
-      </c>
-      <c r="I178" t="str">
-        <f t="shared" si="39"/>
-        <v>static constexpr u8 CON_MC = 7;</v>
-      </c>
-      <c r="J178" t="str">
-        <f t="shared" si="40"/>
-        <v>registerField(Fields::CON_MC, "CON_MC", 7, 1, 0);</v>
-      </c>
-    </row>
-    <row r="179" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B179">
+      <c r="C209" t="s">
+        <v>184</v>
+      </c>
+      <c r="D209">
+        <v>22</v>
+      </c>
+      <c r="E209">
+        <v>1</v>
+      </c>
+      <c r="F209">
+        <v>0</v>
+      </c>
+      <c r="I209" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQ6_EN = 7;</v>
+      </c>
+      <c r="J209" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQ6_EN, "IRQ6_EN", 22, 1, 0);</v>
+      </c>
+    </row>
+    <row r="210" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B210">
         <v>8</v>
       </c>
-      <c r="C179" t="s">
-        <v>160</v>
-      </c>
-      <c r="D179">
-        <v>8</v>
-      </c>
-      <c r="E179">
-        <v>1</v>
-      </c>
-      <c r="F179">
-        <v>0</v>
-      </c>
-      <c r="I179" t="str">
-        <f t="shared" si="39"/>
-        <v>static constexpr u8 SIO = 8;</v>
-      </c>
-      <c r="J179" t="str">
-        <f t="shared" si="40"/>
-        <v>registerField(Fields::SIO, "SIO", 8, 1, 0);</v>
-      </c>
-    </row>
-    <row r="180" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B180">
+      <c r="C210" t="s">
+        <v>193</v>
+      </c>
+      <c r="D210">
+        <v>23</v>
+      </c>
+      <c r="E210">
+        <v>1</v>
+      </c>
+      <c r="F210">
+        <v>0</v>
+      </c>
+      <c r="I210" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQENABLE = 8;</v>
+      </c>
+      <c r="J210" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQENABLE, "IRQENABLE", 23, 1, 0);</v>
+      </c>
+    </row>
+    <row r="211" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B211">
         <v>9</v>
       </c>
-      <c r="C180" t="s">
-        <v>161</v>
-      </c>
-      <c r="D180">
-        <v>9</v>
-      </c>
-      <c r="E180">
-        <v>1</v>
-      </c>
-      <c r="F180">
-        <v>0</v>
-      </c>
-      <c r="I180" t="str">
-        <f t="shared" si="39"/>
-        <v>static constexpr u8 SPU = 9;</v>
-      </c>
-      <c r="J180" t="str">
-        <f t="shared" si="40"/>
-        <v>registerField(Fields::SPU, "SPU", 9, 1, 0);</v>
-      </c>
-    </row>
-    <row r="181" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B181">
+      <c r="C211" t="s">
+        <v>185</v>
+      </c>
+      <c r="D211">
+        <v>24</v>
+      </c>
+      <c r="E211">
+        <v>1</v>
+      </c>
+      <c r="F211">
+        <v>0</v>
+      </c>
+      <c r="I211" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQ0_FL = 9;</v>
+      </c>
+      <c r="J211" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQ0_FL, "IRQ0_FL", 24, 1, 0);</v>
+      </c>
+    </row>
+    <row r="212" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B212">
         <v>10</v>
       </c>
-      <c r="C181" t="s">
-        <v>162</v>
-      </c>
-      <c r="D181">
-        <v>10</v>
-      </c>
-      <c r="E181">
-        <v>1</v>
-      </c>
-      <c r="F181">
-        <v>0</v>
-      </c>
-      <c r="I181" t="str">
-        <f t="shared" si="39"/>
-        <v>static constexpr u8 PIO = 10;</v>
-      </c>
-      <c r="J181" t="str">
-        <f t="shared" si="40"/>
-        <v>registerField(Fields::PIO, "PIO", 10, 1, 0);</v>
+      <c r="C212" t="s">
+        <v>186</v>
+      </c>
+      <c r="D212">
+        <v>25</v>
+      </c>
+      <c r="E212">
+        <v>1</v>
+      </c>
+      <c r="F212">
+        <v>0</v>
+      </c>
+      <c r="I212" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQ1_FL = 10;</v>
+      </c>
+      <c r="J212" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQ1_FL, "IRQ1_FL", 25, 1, 0);</v>
+      </c>
+    </row>
+    <row r="213" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B213">
+        <v>11</v>
+      </c>
+      <c r="C213" t="s">
+        <v>187</v>
+      </c>
+      <c r="D213">
+        <v>26</v>
+      </c>
+      <c r="E213">
+        <v>1</v>
+      </c>
+      <c r="F213">
+        <v>0</v>
+      </c>
+      <c r="I213" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQ2_FL = 11;</v>
+      </c>
+      <c r="J213" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQ2_FL, "IRQ2_FL", 26, 1, 0);</v>
+      </c>
+    </row>
+    <row r="214" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B214">
+        <v>12</v>
+      </c>
+      <c r="C214" t="s">
+        <v>188</v>
+      </c>
+      <c r="D214">
+        <v>27</v>
+      </c>
+      <c r="E214">
+        <v>1</v>
+      </c>
+      <c r="F214">
+        <v>0</v>
+      </c>
+      <c r="I214" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQ3_FL = 12;</v>
+      </c>
+      <c r="J214" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQ3_FL, "IRQ3_FL", 27, 1, 0);</v>
+      </c>
+    </row>
+    <row r="215" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B215">
+        <v>13</v>
+      </c>
+      <c r="C215" t="s">
+        <v>189</v>
+      </c>
+      <c r="D215">
+        <v>28</v>
+      </c>
+      <c r="E215">
+        <v>1</v>
+      </c>
+      <c r="F215">
+        <v>0</v>
+      </c>
+      <c r="I215" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQ4_FL = 13;</v>
+      </c>
+      <c r="J215" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQ4_FL, "IRQ4_FL", 28, 1, 0);</v>
+      </c>
+    </row>
+    <row r="216" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B216">
+        <v>14</v>
+      </c>
+      <c r="C216" t="s">
+        <v>190</v>
+      </c>
+      <c r="D216">
+        <v>29</v>
+      </c>
+      <c r="E216">
+        <v>1</v>
+      </c>
+      <c r="F216">
+        <v>0</v>
+      </c>
+      <c r="I216" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQ5_FL = 14;</v>
+      </c>
+      <c r="J216" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQ5_FL, "IRQ5_FL", 29, 1, 0);</v>
+      </c>
+    </row>
+    <row r="217" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B217">
+        <v>15</v>
+      </c>
+      <c r="C217" t="s">
+        <v>191</v>
+      </c>
+      <c r="D217">
+        <v>30</v>
+      </c>
+      <c r="E217">
+        <v>1</v>
+      </c>
+      <c r="F217">
+        <v>0</v>
+      </c>
+      <c r="I217" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQ6_FL = 15;</v>
+      </c>
+      <c r="J217" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQ6_FL, "IRQ6_FL", 30, 1, 0);</v>
+      </c>
+    </row>
+    <row r="218" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B218">
+        <v>16</v>
+      </c>
+      <c r="C218" t="s">
+        <v>192</v>
+      </c>
+      <c r="D218">
+        <v>31</v>
+      </c>
+      <c r="E218">
+        <v>1</v>
+      </c>
+      <c r="F218">
+        <v>0</v>
+      </c>
+      <c r="I218" t="str">
+        <f t="shared" si="45"/>
+        <v>static constexpr u8 IRQMASTER = 16;</v>
+      </c>
+      <c r="J218" t="str">
+        <f t="shared" si="46"/>
+        <v>registerField(Fields::IRQMASTER, "IRQMASTER", 31, 1, 0);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FeelsReallyGoodMan - EE and IOP are beginning to communicate through the SBUS (DMA transfers)! IOP now interrupting on SIF1 completing. Will need to change the way interrupt exceptions are generated as currently the IOP INTC is sending one every tick (and getting handled meaning no progression in the IOP Core). Reworked some COP0 BitfieldRegister32's that were basically equivilant to a Register32 (simplified). Added in an initalise virtual function to the registers. General reorganisation.
</commit_message>
<xml_diff>
--- a/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
+++ b/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="216">
   <si>
     <t>Field Name</t>
   </si>
@@ -473,9 +473,6 @@
     <t>CHCR</t>
   </si>
   <si>
-    <t>TR</t>
-  </si>
-  <si>
     <t>VBLNK</t>
   </si>
   <si>
@@ -497,18 +494,12 @@
     <t>TMR2</t>
   </si>
   <si>
-    <t>SIO</t>
-  </si>
-  <si>
     <t>SPU</t>
   </si>
   <si>
     <t>PIO</t>
   </si>
   <si>
-    <t>CON_MC</t>
-  </si>
-  <si>
     <t>PCR</t>
   </si>
   <si>
@@ -627,6 +618,60 @@
   </si>
   <si>
     <t>START_T</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>SIO1</t>
+  </si>
+  <si>
+    <t>SIO2</t>
+  </si>
+  <si>
+    <t>SIO0</t>
+  </si>
+  <si>
+    <t>EVBLANK</t>
+  </si>
+  <si>
+    <t>DVD</t>
+  </si>
+  <si>
+    <t>PCMCIA</t>
+  </si>
+  <si>
+    <t>TMR3</t>
+  </si>
+  <si>
+    <t>TMR4</t>
+  </si>
+  <si>
+    <t>TMR5</t>
+  </si>
+  <si>
+    <t>HTR0</t>
+  </si>
+  <si>
+    <t>HTR1</t>
+  </si>
+  <si>
+    <t>HTR2</t>
+  </si>
+  <si>
+    <t>HTR3</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>EXTR</t>
+  </si>
+  <si>
+    <t>FWRE</t>
+  </si>
+  <si>
+    <t>FDMA</t>
   </si>
 </sst>
 </file>
@@ -944,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J218"/>
+  <dimension ref="A1:J248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="D159" sqref="D159"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="I186" sqref="I186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4368,7 +4413,7 @@
         <v>0</v>
       </c>
       <c r="C154" t="s">
-        <v>149</v>
+        <v>198</v>
       </c>
       <c r="D154">
         <v>0</v>
@@ -4385,11 +4430,11 @@
       </c>
       <c r="I154" t="str">
         <f t="shared" ref="I154" si="31">"static constexpr u8 "&amp;C154&amp;" = "&amp;B154&amp;";"</f>
-        <v>static constexpr u8 TR = 0;</v>
+        <v>static constexpr u8 TD = 0;</v>
       </c>
       <c r="J154" t="str">
         <f t="shared" ref="J154" si="32">"registerField(Fields::"&amp;C154&amp;", """&amp;C154&amp;""", "&amp;D154&amp;", "&amp;E154&amp;", "&amp;F154&amp;");"</f>
-        <v>registerField(Fields::TR, "TR", 0, 1, 0);</v>
+        <v>registerField(Fields::TD, "TD", 0, 1, 0);</v>
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.3">
@@ -4397,7 +4442,24 @@
         <v>1</v>
       </c>
       <c r="C155" t="s">
-        <v>194</v>
+        <v>191</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+      <c r="F155">
+        <v>0</v>
+      </c>
+      <c r="I155" t="str">
+        <f t="shared" ref="I155:I161" si="33">"static constexpr u8 "&amp;C155&amp;" = "&amp;B155&amp;";"</f>
+        <v>static constexpr u8 MAS = 1;</v>
+      </c>
+      <c r="J155" t="str">
+        <f t="shared" ref="J155:J161" si="34">"registerField(Fields::"&amp;C155&amp;", """&amp;C155&amp;""", "&amp;D155&amp;", "&amp;E155&amp;", "&amp;F155&amp;");"</f>
+        <v>registerField(Fields::MAS, "MAS", 1, 1, 0);</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.3">
@@ -4405,7 +4467,24 @@
         <v>2</v>
       </c>
       <c r="C156" t="s">
-        <v>195</v>
+        <v>192</v>
+      </c>
+      <c r="D156">
+        <v>8</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+      <c r="F156">
+        <v>0</v>
+      </c>
+      <c r="I156" t="str">
+        <f t="shared" si="33"/>
+        <v>static constexpr u8 CE = 2;</v>
+      </c>
+      <c r="J156" t="str">
+        <f t="shared" si="34"/>
+        <v>registerField(Fields::CE, "CE", 8, 1, 0);</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.3">
@@ -4413,7 +4492,24 @@
         <v>3</v>
       </c>
       <c r="C157" t="s">
-        <v>196</v>
+        <v>193</v>
+      </c>
+      <c r="D157">
+        <v>9</v>
+      </c>
+      <c r="E157">
+        <v>2</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+      <c r="I157" t="str">
+        <f t="shared" si="33"/>
+        <v>static constexpr u8 SM = 3;</v>
+      </c>
+      <c r="J157" t="str">
+        <f t="shared" si="34"/>
+        <v>registerField(Fields::SM, "SM", 9, 2, 0);</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.3">
@@ -4421,7 +4517,24 @@
         <v>4</v>
       </c>
       <c r="C158" t="s">
-        <v>197</v>
+        <v>194</v>
+      </c>
+      <c r="D158">
+        <v>16</v>
+      </c>
+      <c r="E158">
+        <v>3</v>
+      </c>
+      <c r="F158">
+        <v>0</v>
+      </c>
+      <c r="I158" t="str">
+        <f t="shared" si="33"/>
+        <v>static constexpr u8 C_DWS = 4;</v>
+      </c>
+      <c r="J158" t="str">
+        <f t="shared" si="34"/>
+        <v>registerField(Fields::C_DWS, "C_DWS", 16, 3, 0);</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.3">
@@ -4429,7 +4542,24 @@
         <v>5</v>
       </c>
       <c r="C159" t="s">
-        <v>198</v>
+        <v>195</v>
+      </c>
+      <c r="D159">
+        <v>20</v>
+      </c>
+      <c r="E159">
+        <v>3</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+      <c r="I159" t="str">
+        <f t="shared" si="33"/>
+        <v>static constexpr u8 C_CWS = 5;</v>
+      </c>
+      <c r="J159" t="str">
+        <f t="shared" si="34"/>
+        <v>registerField(Fields::C_CWS, "C_CWS", 20, 3, 0);</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.3">
@@ -4437,7 +4567,7 @@
         <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D160">
         <v>24</v>
@@ -4448,13 +4578,13 @@
       <c r="F160">
         <v>0</v>
       </c>
-      <c r="I160" t="e">
-        <f>"static constexpr u8 "&amp;#REF!&amp;" = "&amp;#REF!&amp;";"</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J160" t="e">
-        <f>"registerField(Fields::"&amp;#REF!&amp;", """&amp;#REF!&amp;""", "&amp;D160&amp;", "&amp;E160&amp;", "&amp;F160&amp;");"</f>
-        <v>#REF!</v>
+      <c r="I160" t="str">
+        <f t="shared" si="33"/>
+        <v>static constexpr u8 START_B = 6;</v>
+      </c>
+      <c r="J160" t="str">
+        <f t="shared" si="34"/>
+        <v>registerField(Fields::START_B, "START_B", 24, 1, 0);</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.3">
@@ -4462,7 +4592,24 @@
         <v>7</v>
       </c>
       <c r="C161" t="s">
-        <v>200</v>
+        <v>197</v>
+      </c>
+      <c r="D161">
+        <v>28</v>
+      </c>
+      <c r="E161">
+        <v>1</v>
+      </c>
+      <c r="F161">
+        <v>0</v>
+      </c>
+      <c r="I161" t="str">
+        <f t="shared" si="33"/>
+        <v>static constexpr u8 START_T = 7;</v>
+      </c>
+      <c r="J161" t="str">
+        <f t="shared" si="34"/>
+        <v>registerField(Fields::START_T, "START_T", 28, 1, 0);</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.3">
@@ -4473,7 +4620,7 @@
         <v>0</v>
       </c>
       <c r="C163" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D163">
         <v>0</v>
@@ -4489,11 +4636,11 @@
         <v>class IOPDmacChannelRegister_STAT_t;</v>
       </c>
       <c r="I163" t="str">
-        <f t="shared" ref="I163" si="33">"static constexpr u8 "&amp;C163&amp;" = "&amp;B163&amp;";"</f>
+        <f t="shared" ref="I163" si="35">"static constexpr u8 "&amp;C163&amp;" = "&amp;B163&amp;";"</f>
         <v>static constexpr u8 VBLNK = 0;</v>
       </c>
       <c r="J163" t="str">
-        <f t="shared" ref="J163" si="34">"registerField(Fields::"&amp;C163&amp;", """&amp;C163&amp;""", "&amp;D163&amp;", "&amp;E163&amp;", "&amp;F163&amp;");"</f>
+        <f t="shared" ref="J163" si="36">"registerField(Fields::"&amp;C163&amp;", """&amp;C163&amp;""", "&amp;D163&amp;", "&amp;E163&amp;", "&amp;F163&amp;");"</f>
         <v>registerField(Fields::VBLNK, "VBLNK", 0, 1, 0);</v>
       </c>
     </row>
@@ -4502,7 +4649,7 @@
         <v>1</v>
       </c>
       <c r="C164" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D164">
         <v>1</v>
@@ -4514,11 +4661,11 @@
         <v>0</v>
       </c>
       <c r="I164" t="str">
-        <f t="shared" ref="I164:I173" si="35">"static constexpr u8 "&amp;C164&amp;" = "&amp;B164&amp;";"</f>
+        <f t="shared" ref="I164:I173" si="37">"static constexpr u8 "&amp;C164&amp;" = "&amp;B164&amp;";"</f>
         <v>static constexpr u8 GPU = 1;</v>
       </c>
       <c r="J164" t="str">
-        <f t="shared" ref="J164:J173" si="36">"registerField(Fields::"&amp;C164&amp;", """&amp;C164&amp;""", "&amp;D164&amp;", "&amp;E164&amp;", "&amp;F164&amp;");"</f>
+        <f t="shared" ref="J164:J173" si="38">"registerField(Fields::"&amp;C164&amp;", """&amp;C164&amp;""", "&amp;D164&amp;", "&amp;E164&amp;", "&amp;F164&amp;");"</f>
         <v>registerField(Fields::GPU, "GPU", 1, 1, 0);</v>
       </c>
     </row>
@@ -4527,7 +4674,7 @@
         <v>2</v>
       </c>
       <c r="C165" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D165">
         <v>2</v>
@@ -4539,11 +4686,11 @@
         <v>0</v>
       </c>
       <c r="I165" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>static constexpr u8 CDROM = 2;</v>
       </c>
       <c r="J165" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>registerField(Fields::CDROM, "CDROM", 2, 1, 0);</v>
       </c>
     </row>
@@ -4552,7 +4699,7 @@
         <v>3</v>
       </c>
       <c r="C166" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D166">
         <v>3</v>
@@ -4564,11 +4711,11 @@
         <v>0</v>
       </c>
       <c r="I166" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>static constexpr u8 DMA = 3;</v>
       </c>
       <c r="J166" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>registerField(Fields::DMA, "DMA", 3, 1, 0);</v>
       </c>
     </row>
@@ -4577,7 +4724,7 @@
         <v>4</v>
       </c>
       <c r="C167" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D167">
         <v>4</v>
@@ -4589,11 +4736,11 @@
         <v>0</v>
       </c>
       <c r="I167" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>static constexpr u8 TMR0 = 4;</v>
       </c>
       <c r="J167" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>registerField(Fields::TMR0, "TMR0", 4, 1, 0);</v>
       </c>
     </row>
@@ -4602,7 +4749,7 @@
         <v>5</v>
       </c>
       <c r="C168" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D168">
         <v>5</v>
@@ -4614,11 +4761,11 @@
         <v>0</v>
       </c>
       <c r="I168" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>static constexpr u8 TMR1 = 5;</v>
       </c>
       <c r="J168" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>registerField(Fields::TMR1, "TMR1", 5, 1, 0);</v>
       </c>
     </row>
@@ -4627,7 +4774,7 @@
         <v>6</v>
       </c>
       <c r="C169" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D169">
         <v>6</v>
@@ -4639,11 +4786,11 @@
         <v>0</v>
       </c>
       <c r="I169" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>static constexpr u8 TMR2 = 6;</v>
       </c>
       <c r="J169" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>registerField(Fields::TMR2, "TMR2", 6, 1, 0);</v>
       </c>
     </row>
@@ -4652,7 +4799,7 @@
         <v>7</v>
       </c>
       <c r="C170" t="s">
-        <v>160</v>
+        <v>201</v>
       </c>
       <c r="D170">
         <v>7</v>
@@ -4664,12 +4811,12 @@
         <v>0</v>
       </c>
       <c r="I170" t="str">
-        <f t="shared" si="35"/>
-        <v>static constexpr u8 CON_MC = 7;</v>
+        <f t="shared" si="37"/>
+        <v>static constexpr u8 SIO0 = 7;</v>
       </c>
       <c r="J170" t="str">
-        <f t="shared" si="36"/>
-        <v>registerField(Fields::CON_MC, "CON_MC", 7, 1, 0);</v>
+        <f t="shared" si="38"/>
+        <v>registerField(Fields::SIO0, "SIO0", 7, 1, 0);</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.3">
@@ -4677,7 +4824,7 @@
         <v>8</v>
       </c>
       <c r="C171" t="s">
-        <v>157</v>
+        <v>199</v>
       </c>
       <c r="D171">
         <v>8</v>
@@ -4689,12 +4836,12 @@
         <v>0</v>
       </c>
       <c r="I171" t="str">
-        <f t="shared" si="35"/>
-        <v>static constexpr u8 SIO = 8;</v>
+        <f t="shared" si="37"/>
+        <v>static constexpr u8 SIO1 = 8;</v>
       </c>
       <c r="J171" t="str">
-        <f t="shared" si="36"/>
-        <v>registerField(Fields::SIO, "SIO", 8, 1, 0);</v>
+        <f t="shared" si="38"/>
+        <v>registerField(Fields::SIO1, "SIO1", 8, 1, 0);</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.3">
@@ -4702,7 +4849,7 @@
         <v>9</v>
       </c>
       <c r="C172" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D172">
         <v>9</v>
@@ -4714,11 +4861,11 @@
         <v>0</v>
       </c>
       <c r="I172" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>static constexpr u8 SPU = 9;</v>
       </c>
       <c r="J172" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>registerField(Fields::SPU, "SPU", 9, 1, 0);</v>
       </c>
     </row>
@@ -4727,7 +4874,7 @@
         <v>10</v>
       </c>
       <c r="C173" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D173">
         <v>10</v>
@@ -4739,26 +4886,48 @@
         <v>0</v>
       </c>
       <c r="I173" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>static constexpr u8 PIO = 10;</v>
       </c>
       <c r="J173" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>registerField(Fields::PIO, "PIO", 10, 1, 0);</v>
       </c>
     </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B174">
+        <v>11</v>
+      </c>
+      <c r="C174" t="s">
+        <v>202</v>
+      </c>
+      <c r="D174">
+        <v>11</v>
+      </c>
+      <c r="E174">
+        <v>1</v>
+      </c>
+      <c r="F174">
+        <v>0</v>
+      </c>
+      <c r="I174" t="str">
+        <f t="shared" ref="I174:I188" si="39">"static constexpr u8 "&amp;C174&amp;" = "&amp;B174&amp;";"</f>
+        <v>static constexpr u8 EVBLANK = 11;</v>
+      </c>
+      <c r="J174" t="str">
+        <f t="shared" ref="J174:J188" si="40">"registerField(Fields::"&amp;C174&amp;", """&amp;C174&amp;""", "&amp;D174&amp;", "&amp;E174&amp;", "&amp;F174&amp;");"</f>
+        <v>registerField(Fields::EVBLANK, "EVBLANK", 11, 1, 0);</v>
+      </c>
+    </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A175" t="s">
-        <v>13</v>
-      </c>
       <c r="B175">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C175" t="s">
-        <v>150</v>
+        <v>203</v>
       </c>
       <c r="D175">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E175">
         <v>1</v>
@@ -4766,28 +4935,24 @@
       <c r="F175">
         <v>0</v>
       </c>
-      <c r="H175" t="str">
-        <f>"class IOPDmacChannelRegister_"&amp;A175&amp;"_t;"</f>
-        <v>class IOPDmacChannelRegister_MASK_t;</v>
-      </c>
       <c r="I175" t="str">
-        <f t="shared" ref="I175:I185" si="37">"static constexpr u8 "&amp;C175&amp;" = "&amp;B175&amp;";"</f>
-        <v>static constexpr u8 VBLNK = 0;</v>
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 DVD = 12;</v>
       </c>
       <c r="J175" t="str">
-        <f t="shared" ref="J175:J185" si="38">"registerField(Fields::"&amp;C175&amp;", """&amp;C175&amp;""", "&amp;D175&amp;", "&amp;E175&amp;", "&amp;F175&amp;");"</f>
-        <v>registerField(Fields::VBLNK, "VBLNK", 0, 1, 0);</v>
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::DVD, "DVD", 12, 1, 0);</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B176">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C176" t="s">
-        <v>151</v>
+        <v>204</v>
       </c>
       <c r="D176">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E176">
         <v>1</v>
@@ -4796,23 +4961,23 @@
         <v>0</v>
       </c>
       <c r="I176" t="str">
-        <f t="shared" si="37"/>
-        <v>static constexpr u8 GPU = 1;</v>
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 PCMCIA = 13;</v>
       </c>
       <c r="J176" t="str">
-        <f t="shared" si="38"/>
-        <v>registerField(Fields::GPU, "GPU", 1, 1, 0);</v>
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::PCMCIA, "PCMCIA", 13, 1, 0);</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B177">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C177" t="s">
-        <v>152</v>
+        <v>205</v>
       </c>
       <c r="D177">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E177">
         <v>1</v>
@@ -4821,23 +4986,23 @@
         <v>0</v>
       </c>
       <c r="I177" t="str">
-        <f t="shared" si="37"/>
-        <v>static constexpr u8 CDROM = 2;</v>
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 TMR3 = 14;</v>
       </c>
       <c r="J177" t="str">
-        <f t="shared" si="38"/>
-        <v>registerField(Fields::CDROM, "CDROM", 2, 1, 0);</v>
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::TMR3, "TMR3", 14, 1, 0);</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B178">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C178" t="s">
-        <v>153</v>
+        <v>206</v>
       </c>
       <c r="D178">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E178">
         <v>1</v>
@@ -4846,23 +5011,23 @@
         <v>0</v>
       </c>
       <c r="I178" t="str">
-        <f t="shared" si="37"/>
-        <v>static constexpr u8 DMA = 3;</v>
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 TMR4 = 15;</v>
       </c>
       <c r="J178" t="str">
-        <f t="shared" si="38"/>
-        <v>registerField(Fields::DMA, "DMA", 3, 1, 0);</v>
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::TMR4, "TMR4", 15, 1, 0);</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B179">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C179" t="s">
-        <v>154</v>
+        <v>207</v>
       </c>
       <c r="D179">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E179">
         <v>1</v>
@@ -4871,23 +5036,23 @@
         <v>0</v>
       </c>
       <c r="I179" t="str">
-        <f t="shared" si="37"/>
-        <v>static constexpr u8 TMR0 = 4;</v>
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 TMR5 = 16;</v>
       </c>
       <c r="J179" t="str">
-        <f t="shared" si="38"/>
-        <v>registerField(Fields::TMR0, "TMR0", 4, 1, 0);</v>
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::TMR5, "TMR5", 16, 1, 0);</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B180">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C180" t="s">
-        <v>155</v>
+        <v>200</v>
       </c>
       <c r="D180">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E180">
         <v>1</v>
@@ -4896,23 +5061,23 @@
         <v>0</v>
       </c>
       <c r="I180" t="str">
-        <f t="shared" si="37"/>
-        <v>static constexpr u8 TMR1 = 5;</v>
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 SIO2 = 17;</v>
       </c>
       <c r="J180" t="str">
-        <f t="shared" si="38"/>
-        <v>registerField(Fields::TMR1, "TMR1", 5, 1, 0);</v>
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::SIO2, "SIO2", 17, 1, 0);</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B181">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C181" t="s">
-        <v>156</v>
+        <v>208</v>
       </c>
       <c r="D181">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E181">
         <v>1</v>
@@ -4921,23 +5086,23 @@
         <v>0</v>
       </c>
       <c r="I181" t="str">
-        <f t="shared" si="37"/>
-        <v>static constexpr u8 TMR2 = 6;</v>
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 HTR0 = 18;</v>
       </c>
       <c r="J181" t="str">
-        <f t="shared" si="38"/>
-        <v>registerField(Fields::TMR2, "TMR2", 6, 1, 0);</v>
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::HTR0, "HTR0", 18, 1, 0);</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B182">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C182" t="s">
-        <v>160</v>
+        <v>209</v>
       </c>
       <c r="D182">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E182">
         <v>1</v>
@@ -4946,23 +5111,23 @@
         <v>0</v>
       </c>
       <c r="I182" t="str">
-        <f t="shared" si="37"/>
-        <v>static constexpr u8 CON_MC = 7;</v>
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 HTR1 = 19;</v>
       </c>
       <c r="J182" t="str">
-        <f t="shared" si="38"/>
-        <v>registerField(Fields::CON_MC, "CON_MC", 7, 1, 0);</v>
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::HTR1, "HTR1", 19, 1, 0);</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B183">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C183" t="s">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="D183">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E183">
         <v>1</v>
@@ -4971,23 +5136,23 @@
         <v>0</v>
       </c>
       <c r="I183" t="str">
-        <f t="shared" si="37"/>
-        <v>static constexpr u8 SIO = 8;</v>
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 HTR2 = 20;</v>
       </c>
       <c r="J183" t="str">
-        <f t="shared" si="38"/>
-        <v>registerField(Fields::SIO, "SIO", 8, 1, 0);</v>
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::HTR2, "HTR2", 20, 1, 0);</v>
       </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B184">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C184" t="s">
-        <v>158</v>
+        <v>211</v>
       </c>
       <c r="D184">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E184">
         <v>1</v>
@@ -4996,23 +5161,23 @@
         <v>0</v>
       </c>
       <c r="I184" t="str">
-        <f t="shared" si="37"/>
-        <v>static constexpr u8 SPU = 9;</v>
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 HTR3 = 21;</v>
       </c>
       <c r="J184" t="str">
-        <f t="shared" si="38"/>
-        <v>registerField(Fields::SPU, "SPU", 9, 1, 0);</v>
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::HTR3, "HTR3", 21, 1, 0);</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B185">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C185" t="s">
-        <v>159</v>
+        <v>212</v>
       </c>
       <c r="D185">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E185">
         <v>1</v>
@@ -5021,55 +5186,73 @@
         <v>0</v>
       </c>
       <c r="I185" t="str">
-        <f t="shared" si="37"/>
-        <v>static constexpr u8 PIO = 10;</v>
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 USB = 22;</v>
       </c>
       <c r="J185" t="str">
-        <f t="shared" si="38"/>
-        <v>registerField(Fields::PIO, "PIO", 10, 1, 0);</v>
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::USB, "USB", 22, 1, 0);</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B186">
+        <v>23</v>
+      </c>
+      <c r="C186" t="s">
+        <v>213</v>
+      </c>
+      <c r="D186">
+        <v>23</v>
+      </c>
+      <c r="E186">
+        <v>1</v>
+      </c>
+      <c r="F186">
+        <v>0</v>
+      </c>
+      <c r="I186" t="str">
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 EXTR = 23;</v>
+      </c>
+      <c r="J186" t="str">
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::EXTR, "EXTR", 23, 1, 0);</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A187" t="s">
-        <v>161</v>
-      </c>
       <c r="B187">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C187" t="s">
-        <v>162</v>
+        <v>214</v>
       </c>
       <c r="D187">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E187">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F187">
         <v>0</v>
       </c>
-      <c r="H187" t="str">
-        <f>"class IOPDmacRegister_"&amp;A187&amp;"_t;"</f>
-        <v>class IOPDmacRegister_PCR_t;</v>
-      </c>
       <c r="I187" t="str">
-        <f t="shared" ref="I187" si="39">"static constexpr u8 "&amp;C187&amp;" = "&amp;B187&amp;";"</f>
-        <v>static constexpr u8 PRI0 = 0;</v>
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 FWRE = 24;</v>
       </c>
       <c r="J187" t="str">
-        <f t="shared" ref="J187" si="40">"registerField(Fields::"&amp;C187&amp;", """&amp;C187&amp;""", "&amp;D187&amp;", "&amp;E187&amp;", "&amp;F187&amp;");"</f>
-        <v>registerField(Fields::PRI0, "PRI0", 0, 3, 0);</v>
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::FWRE, "FWRE", 24, 1, 0);</v>
       </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B188">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C188" t="s">
-        <v>169</v>
+        <v>215</v>
       </c>
       <c r="D188">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="E188">
         <v>1</v>
@@ -5078,48 +5261,26 @@
         <v>0</v>
       </c>
       <c r="I188" t="str">
-        <f t="shared" ref="I188:I200" si="41">"static constexpr u8 "&amp;C188&amp;" = "&amp;B188&amp;";"</f>
-        <v>static constexpr u8 ENA0 = 1;</v>
+        <f t="shared" si="39"/>
+        <v>static constexpr u8 FDMA = 25;</v>
       </c>
       <c r="J188" t="str">
-        <f t="shared" ref="J188:J200" si="42">"registerField(Fields::"&amp;C188&amp;", """&amp;C188&amp;""", "&amp;D188&amp;", "&amp;E188&amp;", "&amp;F188&amp;");"</f>
-        <v>registerField(Fields::ENA0, "ENA0", 3, 1, 0);</v>
-      </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B189">
-        <v>2</v>
-      </c>
-      <c r="C189" t="s">
-        <v>163</v>
-      </c>
-      <c r="D189">
-        <v>4</v>
-      </c>
-      <c r="E189">
-        <v>3</v>
-      </c>
-      <c r="F189">
-        <v>0</v>
-      </c>
-      <c r="I189" t="str">
-        <f t="shared" si="41"/>
-        <v>static constexpr u8 PRI1 = 2;</v>
-      </c>
-      <c r="J189" t="str">
-        <f t="shared" si="42"/>
-        <v>registerField(Fields::PRI1, "PRI1", 4, 3, 0);</v>
+        <f t="shared" si="40"/>
+        <v>registerField(Fields::FDMA, "FDMA", 25, 1, 0);</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>13</v>
+      </c>
       <c r="B190">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C190" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="D190">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E190">
         <v>1</v>
@@ -5127,49 +5288,53 @@
       <c r="F190">
         <v>0</v>
       </c>
+      <c r="H190" t="str">
+        <f>"class IOPDmacChannelRegister_"&amp;A190&amp;"_t;"</f>
+        <v>class IOPDmacChannelRegister_MASK_t;</v>
+      </c>
       <c r="I190" t="str">
-        <f t="shared" si="41"/>
-        <v>static constexpr u8 ENA1 = 3;</v>
+        <f t="shared" ref="I190:I200" si="41">"static constexpr u8 "&amp;C190&amp;" = "&amp;B190&amp;";"</f>
+        <v>static constexpr u8 VBLNK = 0;</v>
       </c>
       <c r="J190" t="str">
-        <f t="shared" si="42"/>
-        <v>registerField(Fields::ENA1, "ENA1", 7, 1, 0);</v>
+        <f t="shared" ref="J190:J200" si="42">"registerField(Fields::"&amp;C190&amp;", """&amp;C190&amp;""", "&amp;D190&amp;", "&amp;E190&amp;", "&amp;F190&amp;");"</f>
+        <v>registerField(Fields::VBLNK, "VBLNK", 0, 1, 0);</v>
       </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B191">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C191" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D191">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E191">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F191">
         <v>0</v>
       </c>
       <c r="I191" t="str">
         <f t="shared" si="41"/>
-        <v>static constexpr u8 PRI2 = 4;</v>
+        <v>static constexpr u8 GPU = 1;</v>
       </c>
       <c r="J191" t="str">
         <f t="shared" si="42"/>
-        <v>registerField(Fields::PRI2, "PRI2", 8, 3, 0);</v>
+        <v>registerField(Fields::GPU, "GPU", 1, 1, 0);</v>
       </c>
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B192">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C192" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="D192">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E192">
         <v>1</v>
@@ -5179,47 +5344,47 @@
       </c>
       <c r="I192" t="str">
         <f t="shared" si="41"/>
-        <v>static constexpr u8 ENA2 = 5;</v>
+        <v>static constexpr u8 CDROM = 2;</v>
       </c>
       <c r="J192" t="str">
         <f t="shared" si="42"/>
-        <v>registerField(Fields::ENA2, "ENA2", 11, 1, 0);</v>
-      </c>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
+        <v>registerField(Fields::CDROM, "CDROM", 2, 1, 0);</v>
+      </c>
+    </row>
+    <row r="193" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B193">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C193" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="D193">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E193">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F193">
         <v>0</v>
       </c>
       <c r="I193" t="str">
         <f t="shared" si="41"/>
-        <v>static constexpr u8 PRI3 = 6;</v>
+        <v>static constexpr u8 DMA = 3;</v>
       </c>
       <c r="J193" t="str">
         <f t="shared" si="42"/>
-        <v>registerField(Fields::PRI3, "PRI3", 12, 3, 0);</v>
-      </c>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
+        <v>registerField(Fields::DMA, "DMA", 3, 1, 0);</v>
+      </c>
+    </row>
+    <row r="194" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B194">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C194" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="D194">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E194">
         <v>1</v>
@@ -5229,47 +5394,47 @@
       </c>
       <c r="I194" t="str">
         <f t="shared" si="41"/>
-        <v>static constexpr u8 ENA3 = 7;</v>
+        <v>static constexpr u8 TMR0 = 4;</v>
       </c>
       <c r="J194" t="str">
         <f t="shared" si="42"/>
-        <v>registerField(Fields::ENA3, "ENA3", 15, 1, 0);</v>
-      </c>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
+        <v>registerField(Fields::TMR0, "TMR0", 4, 1, 0);</v>
+      </c>
+    </row>
+    <row r="195" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B195">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C195" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="D195">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E195">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F195">
         <v>0</v>
       </c>
       <c r="I195" t="str">
         <f t="shared" si="41"/>
-        <v>static constexpr u8 PRI4 = 8;</v>
+        <v>static constexpr u8 TMR1 = 5;</v>
       </c>
       <c r="J195" t="str">
         <f t="shared" si="42"/>
-        <v>registerField(Fields::PRI4, "PRI4", 16, 3, 0);</v>
-      </c>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
+        <v>registerField(Fields::TMR1, "TMR1", 5, 1, 0);</v>
+      </c>
+    </row>
+    <row r="196" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B196">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C196" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="D196">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E196">
         <v>1</v>
@@ -5279,47 +5444,47 @@
       </c>
       <c r="I196" t="str">
         <f t="shared" si="41"/>
-        <v>static constexpr u8 ENA4 = 9;</v>
+        <v>static constexpr u8 TMR2 = 6;</v>
       </c>
       <c r="J196" t="str">
         <f t="shared" si="42"/>
-        <v>registerField(Fields::ENA4, "ENA4", 19, 1, 0);</v>
-      </c>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
+        <v>registerField(Fields::TMR2, "TMR2", 6, 1, 0);</v>
+      </c>
+    </row>
+    <row r="197" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B197">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C197" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="D197">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E197">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F197">
         <v>0</v>
       </c>
       <c r="I197" t="str">
         <f t="shared" si="41"/>
-        <v>static constexpr u8 PRI5 = 10;</v>
+        <v>static constexpr u8 SIO0 = 7;</v>
       </c>
       <c r="J197" t="str">
         <f t="shared" si="42"/>
-        <v>registerField(Fields::PRI5, "PRI5", 20, 3, 0);</v>
-      </c>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
+        <v>registerField(Fields::SIO0, "SIO0", 7, 1, 0);</v>
+      </c>
+    </row>
+    <row r="198" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B198">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C198" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="D198">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E198">
         <v>1</v>
@@ -5329,47 +5494,47 @@
       </c>
       <c r="I198" t="str">
         <f t="shared" si="41"/>
-        <v>static constexpr u8 ENA5 = 11;</v>
+        <v>static constexpr u8 SIO1 = 8;</v>
       </c>
       <c r="J198" t="str">
         <f t="shared" si="42"/>
-        <v>registerField(Fields::ENA5, "ENA5", 23, 1, 0);</v>
-      </c>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
+        <v>registerField(Fields::SIO1, "SIO1", 8, 1, 0);</v>
+      </c>
+    </row>
+    <row r="199" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B199">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C199" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D199">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E199">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F199">
         <v>0</v>
       </c>
       <c r="I199" t="str">
         <f t="shared" si="41"/>
-        <v>static constexpr u8 PRI6 = 12;</v>
+        <v>static constexpr u8 SPU = 9;</v>
       </c>
       <c r="J199" t="str">
         <f t="shared" si="42"/>
-        <v>registerField(Fields::PRI6, "PRI6", 24, 3, 0);</v>
-      </c>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
+        <v>registerField(Fields::SPU, "SPU", 9, 1, 0);</v>
+      </c>
+    </row>
+    <row r="200" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B200">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C200" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="D200">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E200">
         <v>1</v>
@@ -5379,442 +5544,1174 @@
       </c>
       <c r="I200" t="str">
         <f t="shared" si="41"/>
-        <v>static constexpr u8 ENA6 = 13;</v>
+        <v>static constexpr u8 PIO = 10;</v>
       </c>
       <c r="J200" t="str">
         <f t="shared" si="42"/>
+        <v>registerField(Fields::PIO, "PIO", 10, 1, 0);</v>
+      </c>
+    </row>
+    <row r="201" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B201">
+        <v>11</v>
+      </c>
+      <c r="C201" t="s">
+        <v>202</v>
+      </c>
+      <c r="D201">
+        <v>11</v>
+      </c>
+      <c r="E201">
+        <v>1</v>
+      </c>
+      <c r="F201">
+        <v>0</v>
+      </c>
+      <c r="I201" t="str">
+        <f t="shared" ref="I201:I215" si="43">"static constexpr u8 "&amp;C201&amp;" = "&amp;B201&amp;";"</f>
+        <v>static constexpr u8 EVBLANK = 11;</v>
+      </c>
+      <c r="J201" t="str">
+        <f t="shared" ref="J201:J215" si="44">"registerField(Fields::"&amp;C201&amp;", """&amp;C201&amp;""", "&amp;D201&amp;", "&amp;E201&amp;", "&amp;F201&amp;");"</f>
+        <v>registerField(Fields::EVBLANK, "EVBLANK", 11, 1, 0);</v>
+      </c>
+    </row>
+    <row r="202" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B202">
+        <v>12</v>
+      </c>
+      <c r="C202" t="s">
+        <v>203</v>
+      </c>
+      <c r="D202">
+        <v>12</v>
+      </c>
+      <c r="E202">
+        <v>1</v>
+      </c>
+      <c r="F202">
+        <v>0</v>
+      </c>
+      <c r="I202" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 DVD = 12;</v>
+      </c>
+      <c r="J202" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::DVD, "DVD", 12, 1, 0);</v>
+      </c>
+    </row>
+    <row r="203" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B203">
+        <v>13</v>
+      </c>
+      <c r="C203" t="s">
+        <v>204</v>
+      </c>
+      <c r="D203">
+        <v>13</v>
+      </c>
+      <c r="E203">
+        <v>1</v>
+      </c>
+      <c r="F203">
+        <v>0</v>
+      </c>
+      <c r="I203" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 PCMCIA = 13;</v>
+      </c>
+      <c r="J203" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::PCMCIA, "PCMCIA", 13, 1, 0);</v>
+      </c>
+    </row>
+    <row r="204" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B204">
+        <v>14</v>
+      </c>
+      <c r="C204" t="s">
+        <v>205</v>
+      </c>
+      <c r="D204">
+        <v>14</v>
+      </c>
+      <c r="E204">
+        <v>1</v>
+      </c>
+      <c r="F204">
+        <v>0</v>
+      </c>
+      <c r="I204" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 TMR3 = 14;</v>
+      </c>
+      <c r="J204" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::TMR3, "TMR3", 14, 1, 0);</v>
+      </c>
+    </row>
+    <row r="205" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B205">
+        <v>15</v>
+      </c>
+      <c r="C205" t="s">
+        <v>206</v>
+      </c>
+      <c r="D205">
+        <v>15</v>
+      </c>
+      <c r="E205">
+        <v>1</v>
+      </c>
+      <c r="F205">
+        <v>0</v>
+      </c>
+      <c r="I205" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 TMR4 = 15;</v>
+      </c>
+      <c r="J205" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::TMR4, "TMR4", 15, 1, 0);</v>
+      </c>
+    </row>
+    <row r="206" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B206">
+        <v>16</v>
+      </c>
+      <c r="C206" t="s">
+        <v>207</v>
+      </c>
+      <c r="D206">
+        <v>16</v>
+      </c>
+      <c r="E206">
+        <v>1</v>
+      </c>
+      <c r="F206">
+        <v>0</v>
+      </c>
+      <c r="I206" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 TMR5 = 16;</v>
+      </c>
+      <c r="J206" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::TMR5, "TMR5", 16, 1, 0);</v>
+      </c>
+    </row>
+    <row r="207" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B207">
+        <v>17</v>
+      </c>
+      <c r="C207" t="s">
+        <v>200</v>
+      </c>
+      <c r="D207">
+        <v>17</v>
+      </c>
+      <c r="E207">
+        <v>1</v>
+      </c>
+      <c r="F207">
+        <v>0</v>
+      </c>
+      <c r="I207" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 SIO2 = 17;</v>
+      </c>
+      <c r="J207" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::SIO2, "SIO2", 17, 1, 0);</v>
+      </c>
+    </row>
+    <row r="208" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B208">
+        <v>18</v>
+      </c>
+      <c r="C208" t="s">
+        <v>208</v>
+      </c>
+      <c r="D208">
+        <v>18</v>
+      </c>
+      <c r="E208">
+        <v>1</v>
+      </c>
+      <c r="F208">
+        <v>0</v>
+      </c>
+      <c r="I208" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 HTR0 = 18;</v>
+      </c>
+      <c r="J208" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::HTR0, "HTR0", 18, 1, 0);</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B209">
+        <v>19</v>
+      </c>
+      <c r="C209" t="s">
+        <v>209</v>
+      </c>
+      <c r="D209">
+        <v>19</v>
+      </c>
+      <c r="E209">
+        <v>1</v>
+      </c>
+      <c r="F209">
+        <v>0</v>
+      </c>
+      <c r="I209" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 HTR1 = 19;</v>
+      </c>
+      <c r="J209" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::HTR1, "HTR1", 19, 1, 0);</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B210">
+        <v>20</v>
+      </c>
+      <c r="C210" t="s">
+        <v>210</v>
+      </c>
+      <c r="D210">
+        <v>20</v>
+      </c>
+      <c r="E210">
+        <v>1</v>
+      </c>
+      <c r="F210">
+        <v>0</v>
+      </c>
+      <c r="I210" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 HTR2 = 20;</v>
+      </c>
+      <c r="J210" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::HTR2, "HTR2", 20, 1, 0);</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B211">
+        <v>21</v>
+      </c>
+      <c r="C211" t="s">
+        <v>211</v>
+      </c>
+      <c r="D211">
+        <v>21</v>
+      </c>
+      <c r="E211">
+        <v>1</v>
+      </c>
+      <c r="F211">
+        <v>0</v>
+      </c>
+      <c r="I211" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 HTR3 = 21;</v>
+      </c>
+      <c r="J211" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::HTR3, "HTR3", 21, 1, 0);</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B212">
+        <v>22</v>
+      </c>
+      <c r="C212" t="s">
+        <v>212</v>
+      </c>
+      <c r="D212">
+        <v>22</v>
+      </c>
+      <c r="E212">
+        <v>1</v>
+      </c>
+      <c r="F212">
+        <v>0</v>
+      </c>
+      <c r="I212" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 USB = 22;</v>
+      </c>
+      <c r="J212" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::USB, "USB", 22, 1, 0);</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B213">
+        <v>23</v>
+      </c>
+      <c r="C213" t="s">
+        <v>213</v>
+      </c>
+      <c r="D213">
+        <v>23</v>
+      </c>
+      <c r="E213">
+        <v>1</v>
+      </c>
+      <c r="F213">
+        <v>0</v>
+      </c>
+      <c r="I213" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 EXTR = 23;</v>
+      </c>
+      <c r="J213" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::EXTR, "EXTR", 23, 1, 0);</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B214">
+        <v>24</v>
+      </c>
+      <c r="C214" t="s">
+        <v>214</v>
+      </c>
+      <c r="D214">
+        <v>24</v>
+      </c>
+      <c r="E214">
+        <v>1</v>
+      </c>
+      <c r="F214">
+        <v>0</v>
+      </c>
+      <c r="I214" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 FWRE = 24;</v>
+      </c>
+      <c r="J214" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::FWRE, "FWRE", 24, 1, 0);</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B215">
+        <v>25</v>
+      </c>
+      <c r="C215" t="s">
+        <v>215</v>
+      </c>
+      <c r="D215">
+        <v>25</v>
+      </c>
+      <c r="E215">
+        <v>1</v>
+      </c>
+      <c r="F215">
+        <v>0</v>
+      </c>
+      <c r="I215" t="str">
+        <f t="shared" si="43"/>
+        <v>static constexpr u8 FDMA = 25;</v>
+      </c>
+      <c r="J215" t="str">
+        <f t="shared" si="44"/>
+        <v>registerField(Fields::FDMA, "FDMA", 25, 1, 0);</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>158</v>
+      </c>
+      <c r="B217">
+        <v>0</v>
+      </c>
+      <c r="C217" t="s">
+        <v>159</v>
+      </c>
+      <c r="D217">
+        <v>0</v>
+      </c>
+      <c r="E217">
+        <v>3</v>
+      </c>
+      <c r="F217">
+        <v>0</v>
+      </c>
+      <c r="H217" t="str">
+        <f>"class IOPDmacRegister_"&amp;A217&amp;"_t;"</f>
+        <v>class IOPDmacRegister_PCR_t;</v>
+      </c>
+      <c r="I217" t="str">
+        <f t="shared" ref="I217" si="45">"static constexpr u8 "&amp;C217&amp;" = "&amp;B217&amp;";"</f>
+        <v>static constexpr u8 PRI0 = 0;</v>
+      </c>
+      <c r="J217" t="str">
+        <f t="shared" ref="J217" si="46">"registerField(Fields::"&amp;C217&amp;", """&amp;C217&amp;""", "&amp;D217&amp;", "&amp;E217&amp;", "&amp;F217&amp;");"</f>
+        <v>registerField(Fields::PRI0, "PRI0", 0, 3, 0);</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B218">
+        <v>1</v>
+      </c>
+      <c r="C218" t="s">
+        <v>166</v>
+      </c>
+      <c r="D218">
+        <v>3</v>
+      </c>
+      <c r="E218">
+        <v>1</v>
+      </c>
+      <c r="F218">
+        <v>0</v>
+      </c>
+      <c r="I218" t="str">
+        <f t="shared" ref="I218:I230" si="47">"static constexpr u8 "&amp;C218&amp;" = "&amp;B218&amp;";"</f>
+        <v>static constexpr u8 ENA0 = 1;</v>
+      </c>
+      <c r="J218" t="str">
+        <f t="shared" ref="J218:J230" si="48">"registerField(Fields::"&amp;C218&amp;", """&amp;C218&amp;""", "&amp;D218&amp;", "&amp;E218&amp;", "&amp;F218&amp;");"</f>
+        <v>registerField(Fields::ENA0, "ENA0", 3, 1, 0);</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B219">
+        <v>2</v>
+      </c>
+      <c r="C219" t="s">
+        <v>160</v>
+      </c>
+      <c r="D219">
+        <v>4</v>
+      </c>
+      <c r="E219">
+        <v>3</v>
+      </c>
+      <c r="F219">
+        <v>0</v>
+      </c>
+      <c r="I219" t="str">
+        <f t="shared" si="47"/>
+        <v>static constexpr u8 PRI1 = 2;</v>
+      </c>
+      <c r="J219" t="str">
+        <f t="shared" si="48"/>
+        <v>registerField(Fields::PRI1, "PRI1", 4, 3, 0);</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B220">
+        <v>3</v>
+      </c>
+      <c r="C220" t="s">
+        <v>167</v>
+      </c>
+      <c r="D220">
+        <v>7</v>
+      </c>
+      <c r="E220">
+        <v>1</v>
+      </c>
+      <c r="F220">
+        <v>0</v>
+      </c>
+      <c r="I220" t="str">
+        <f t="shared" si="47"/>
+        <v>static constexpr u8 ENA1 = 3;</v>
+      </c>
+      <c r="J220" t="str">
+        <f t="shared" si="48"/>
+        <v>registerField(Fields::ENA1, "ENA1", 7, 1, 0);</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B221">
+        <v>4</v>
+      </c>
+      <c r="C221" t="s">
+        <v>161</v>
+      </c>
+      <c r="D221">
+        <v>8</v>
+      </c>
+      <c r="E221">
+        <v>3</v>
+      </c>
+      <c r="F221">
+        <v>0</v>
+      </c>
+      <c r="I221" t="str">
+        <f t="shared" si="47"/>
+        <v>static constexpr u8 PRI2 = 4;</v>
+      </c>
+      <c r="J221" t="str">
+        <f t="shared" si="48"/>
+        <v>registerField(Fields::PRI2, "PRI2", 8, 3, 0);</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B222">
+        <v>5</v>
+      </c>
+      <c r="C222" t="s">
+        <v>168</v>
+      </c>
+      <c r="D222">
+        <v>11</v>
+      </c>
+      <c r="E222">
+        <v>1</v>
+      </c>
+      <c r="F222">
+        <v>0</v>
+      </c>
+      <c r="I222" t="str">
+        <f t="shared" si="47"/>
+        <v>static constexpr u8 ENA2 = 5;</v>
+      </c>
+      <c r="J222" t="str">
+        <f t="shared" si="48"/>
+        <v>registerField(Fields::ENA2, "ENA2", 11, 1, 0);</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B223">
+        <v>6</v>
+      </c>
+      <c r="C223" t="s">
+        <v>162</v>
+      </c>
+      <c r="D223">
+        <v>12</v>
+      </c>
+      <c r="E223">
+        <v>3</v>
+      </c>
+      <c r="F223">
+        <v>0</v>
+      </c>
+      <c r="I223" t="str">
+        <f t="shared" si="47"/>
+        <v>static constexpr u8 PRI3 = 6;</v>
+      </c>
+      <c r="J223" t="str">
+        <f t="shared" si="48"/>
+        <v>registerField(Fields::PRI3, "PRI3", 12, 3, 0);</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B224">
+        <v>7</v>
+      </c>
+      <c r="C224" t="s">
+        <v>169</v>
+      </c>
+      <c r="D224">
+        <v>15</v>
+      </c>
+      <c r="E224">
+        <v>1</v>
+      </c>
+      <c r="F224">
+        <v>0</v>
+      </c>
+      <c r="I224" t="str">
+        <f t="shared" si="47"/>
+        <v>static constexpr u8 ENA3 = 7;</v>
+      </c>
+      <c r="J224" t="str">
+        <f t="shared" si="48"/>
+        <v>registerField(Fields::ENA3, "ENA3", 15, 1, 0);</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B225">
+        <v>8</v>
+      </c>
+      <c r="C225" t="s">
+        <v>163</v>
+      </c>
+      <c r="D225">
+        <v>16</v>
+      </c>
+      <c r="E225">
+        <v>3</v>
+      </c>
+      <c r="F225">
+        <v>0</v>
+      </c>
+      <c r="I225" t="str">
+        <f t="shared" si="47"/>
+        <v>static constexpr u8 PRI4 = 8;</v>
+      </c>
+      <c r="J225" t="str">
+        <f t="shared" si="48"/>
+        <v>registerField(Fields::PRI4, "PRI4", 16, 3, 0);</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B226">
+        <v>9</v>
+      </c>
+      <c r="C226" t="s">
+        <v>170</v>
+      </c>
+      <c r="D226">
+        <v>19</v>
+      </c>
+      <c r="E226">
+        <v>1</v>
+      </c>
+      <c r="F226">
+        <v>0</v>
+      </c>
+      <c r="I226" t="str">
+        <f t="shared" si="47"/>
+        <v>static constexpr u8 ENA4 = 9;</v>
+      </c>
+      <c r="J226" t="str">
+        <f t="shared" si="48"/>
+        <v>registerField(Fields::ENA4, "ENA4", 19, 1, 0);</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B227">
+        <v>10</v>
+      </c>
+      <c r="C227" t="s">
+        <v>164</v>
+      </c>
+      <c r="D227">
+        <v>20</v>
+      </c>
+      <c r="E227">
+        <v>3</v>
+      </c>
+      <c r="F227">
+        <v>0</v>
+      </c>
+      <c r="I227" t="str">
+        <f t="shared" si="47"/>
+        <v>static constexpr u8 PRI5 = 10;</v>
+      </c>
+      <c r="J227" t="str">
+        <f t="shared" si="48"/>
+        <v>registerField(Fields::PRI5, "PRI5", 20, 3, 0);</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B228">
+        <v>11</v>
+      </c>
+      <c r="C228" t="s">
+        <v>171</v>
+      </c>
+      <c r="D228">
+        <v>23</v>
+      </c>
+      <c r="E228">
+        <v>1</v>
+      </c>
+      <c r="F228">
+        <v>0</v>
+      </c>
+      <c r="I228" t="str">
+        <f t="shared" si="47"/>
+        <v>static constexpr u8 ENA5 = 11;</v>
+      </c>
+      <c r="J228" t="str">
+        <f t="shared" si="48"/>
+        <v>registerField(Fields::ENA5, "ENA5", 23, 1, 0);</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B229">
+        <v>12</v>
+      </c>
+      <c r="C229" t="s">
+        <v>165</v>
+      </c>
+      <c r="D229">
+        <v>24</v>
+      </c>
+      <c r="E229">
+        <v>3</v>
+      </c>
+      <c r="F229">
+        <v>0</v>
+      </c>
+      <c r="I229" t="str">
+        <f t="shared" si="47"/>
+        <v>static constexpr u8 PRI6 = 12;</v>
+      </c>
+      <c r="J229" t="str">
+        <f t="shared" si="48"/>
+        <v>registerField(Fields::PRI6, "PRI6", 24, 3, 0);</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B230">
+        <v>13</v>
+      </c>
+      <c r="C230" t="s">
+        <v>172</v>
+      </c>
+      <c r="D230">
+        <v>27</v>
+      </c>
+      <c r="E230">
+        <v>1</v>
+      </c>
+      <c r="F230">
+        <v>0</v>
+      </c>
+      <c r="I230" t="str">
+        <f t="shared" si="47"/>
+        <v>static constexpr u8 ENA6 = 13;</v>
+      </c>
+      <c r="J230" t="str">
+        <f t="shared" si="48"/>
         <v>registerField(Fields::ENA6, "ENA6", 27, 1, 0);</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>173</v>
+      </c>
+      <c r="B232">
+        <v>0</v>
+      </c>
+      <c r="C232" t="s">
+        <v>174</v>
+      </c>
+      <c r="D232">
+        <v>15</v>
+      </c>
+      <c r="E232">
+        <v>1</v>
+      </c>
+      <c r="F232">
+        <v>0</v>
+      </c>
+      <c r="H232" t="str">
+        <f>"class IOPDmacRegister_"&amp;A232&amp;"_t;"</f>
+        <v>class IOPDmacRegister_ICR_t;</v>
+      </c>
+      <c r="I232" t="str">
+        <f t="shared" ref="I232" si="49">"static constexpr u8 "&amp;C232&amp;" = "&amp;B232&amp;";"</f>
+        <v>static constexpr u8 IRQFORCE = 0;</v>
+      </c>
+      <c r="J232" t="str">
+        <f t="shared" ref="J232" si="50">"registerField(Fields::"&amp;C232&amp;", """&amp;C232&amp;""", "&amp;D232&amp;", "&amp;E232&amp;", "&amp;F232&amp;");"</f>
+        <v>registerField(Fields::IRQFORCE, "IRQFORCE", 15, 1, 0);</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B233">
+        <v>1</v>
+      </c>
+      <c r="C233" t="s">
+        <v>175</v>
+      </c>
+      <c r="D233">
+        <v>16</v>
+      </c>
+      <c r="E233">
+        <v>1</v>
+      </c>
+      <c r="F233">
+        <v>0</v>
+      </c>
+      <c r="I233" t="str">
+        <f t="shared" ref="I233:I248" si="51">"static constexpr u8 "&amp;C233&amp;" = "&amp;B233&amp;";"</f>
+        <v>static constexpr u8 IRQ0_EN = 1;</v>
+      </c>
+      <c r="J233" t="str">
+        <f t="shared" ref="J233:J248" si="52">"registerField(Fields::"&amp;C233&amp;", """&amp;C233&amp;""", "&amp;D233&amp;", "&amp;E233&amp;", "&amp;F233&amp;");"</f>
+        <v>registerField(Fields::IRQ0_EN, "IRQ0_EN", 16, 1, 0);</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B234">
+        <v>2</v>
+      </c>
+      <c r="C234" t="s">
         <v>176</v>
       </c>
-      <c r="B202">
-        <v>0</v>
-      </c>
-      <c r="C202" t="s">
+      <c r="D234">
+        <v>17</v>
+      </c>
+      <c r="E234">
+        <v>1</v>
+      </c>
+      <c r="F234">
+        <v>0</v>
+      </c>
+      <c r="I234" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQ1_EN = 2;</v>
+      </c>
+      <c r="J234" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQ1_EN, "IRQ1_EN", 17, 1, 0);</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B235">
+        <v>3</v>
+      </c>
+      <c r="C235" t="s">
         <v>177</v>
       </c>
-      <c r="D202">
+      <c r="D235">
+        <v>18</v>
+      </c>
+      <c r="E235">
+        <v>1</v>
+      </c>
+      <c r="F235">
+        <v>0</v>
+      </c>
+      <c r="I235" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQ2_EN = 3;</v>
+      </c>
+      <c r="J235" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQ2_EN, "IRQ2_EN", 18, 1, 0);</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B236">
+        <v>4</v>
+      </c>
+      <c r="C236" t="s">
+        <v>178</v>
+      </c>
+      <c r="D236">
+        <v>19</v>
+      </c>
+      <c r="E236">
+        <v>1</v>
+      </c>
+      <c r="F236">
+        <v>0</v>
+      </c>
+      <c r="I236" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQ3_EN = 4;</v>
+      </c>
+      <c r="J236" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQ3_EN, "IRQ3_EN", 19, 1, 0);</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B237">
+        <v>5</v>
+      </c>
+      <c r="C237" t="s">
+        <v>179</v>
+      </c>
+      <c r="D237">
+        <v>20</v>
+      </c>
+      <c r="E237">
+        <v>1</v>
+      </c>
+      <c r="F237">
+        <v>0</v>
+      </c>
+      <c r="I237" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQ4_EN = 5;</v>
+      </c>
+      <c r="J237" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQ4_EN, "IRQ4_EN", 20, 1, 0);</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B238">
+        <v>6</v>
+      </c>
+      <c r="C238" t="s">
+        <v>180</v>
+      </c>
+      <c r="D238">
+        <v>21</v>
+      </c>
+      <c r="E238">
+        <v>1</v>
+      </c>
+      <c r="F238">
+        <v>0</v>
+      </c>
+      <c r="I238" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQ5_EN = 6;</v>
+      </c>
+      <c r="J238" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQ5_EN, "IRQ5_EN", 21, 1, 0);</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B239">
+        <v>7</v>
+      </c>
+      <c r="C239" t="s">
+        <v>181</v>
+      </c>
+      <c r="D239">
+        <v>22</v>
+      </c>
+      <c r="E239">
+        <v>1</v>
+      </c>
+      <c r="F239">
+        <v>0</v>
+      </c>
+      <c r="I239" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQ6_EN = 7;</v>
+      </c>
+      <c r="J239" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQ6_EN, "IRQ6_EN", 22, 1, 0);</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B240">
+        <v>8</v>
+      </c>
+      <c r="C240" t="s">
+        <v>190</v>
+      </c>
+      <c r="D240">
+        <v>23</v>
+      </c>
+      <c r="E240">
+        <v>1</v>
+      </c>
+      <c r="F240">
+        <v>0</v>
+      </c>
+      <c r="I240" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQENABLE = 8;</v>
+      </c>
+      <c r="J240" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQENABLE, "IRQENABLE", 23, 1, 0);</v>
+      </c>
+    </row>
+    <row r="241" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B241">
+        <v>9</v>
+      </c>
+      <c r="C241" t="s">
+        <v>182</v>
+      </c>
+      <c r="D241">
+        <v>24</v>
+      </c>
+      <c r="E241">
+        <v>1</v>
+      </c>
+      <c r="F241">
+        <v>0</v>
+      </c>
+      <c r="I241" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQ0_FL = 9;</v>
+      </c>
+      <c r="J241" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQ0_FL, "IRQ0_FL", 24, 1, 0);</v>
+      </c>
+    </row>
+    <row r="242" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B242">
+        <v>10</v>
+      </c>
+      <c r="C242" t="s">
+        <v>183</v>
+      </c>
+      <c r="D242">
+        <v>25</v>
+      </c>
+      <c r="E242">
+        <v>1</v>
+      </c>
+      <c r="F242">
+        <v>0</v>
+      </c>
+      <c r="I242" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQ1_FL = 10;</v>
+      </c>
+      <c r="J242" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQ1_FL, "IRQ1_FL", 25, 1, 0);</v>
+      </c>
+    </row>
+    <row r="243" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B243">
+        <v>11</v>
+      </c>
+      <c r="C243" t="s">
+        <v>184</v>
+      </c>
+      <c r="D243">
+        <v>26</v>
+      </c>
+      <c r="E243">
+        <v>1</v>
+      </c>
+      <c r="F243">
+        <v>0</v>
+      </c>
+      <c r="I243" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQ2_FL = 11;</v>
+      </c>
+      <c r="J243" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQ2_FL, "IRQ2_FL", 26, 1, 0);</v>
+      </c>
+    </row>
+    <row r="244" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B244">
+        <v>12</v>
+      </c>
+      <c r="C244" t="s">
+        <v>185</v>
+      </c>
+      <c r="D244">
+        <v>27</v>
+      </c>
+      <c r="E244">
+        <v>1</v>
+      </c>
+      <c r="F244">
+        <v>0</v>
+      </c>
+      <c r="I244" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQ3_FL = 12;</v>
+      </c>
+      <c r="J244" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQ3_FL, "IRQ3_FL", 27, 1, 0);</v>
+      </c>
+    </row>
+    <row r="245" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B245">
+        <v>13</v>
+      </c>
+      <c r="C245" t="s">
+        <v>186</v>
+      </c>
+      <c r="D245">
+        <v>28</v>
+      </c>
+      <c r="E245">
+        <v>1</v>
+      </c>
+      <c r="F245">
+        <v>0</v>
+      </c>
+      <c r="I245" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQ4_FL = 13;</v>
+      </c>
+      <c r="J245" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQ4_FL, "IRQ4_FL", 28, 1, 0);</v>
+      </c>
+    </row>
+    <row r="246" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B246">
+        <v>14</v>
+      </c>
+      <c r="C246" t="s">
+        <v>187</v>
+      </c>
+      <c r="D246">
+        <v>29</v>
+      </c>
+      <c r="E246">
+        <v>1</v>
+      </c>
+      <c r="F246">
+        <v>0</v>
+      </c>
+      <c r="I246" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQ5_FL = 14;</v>
+      </c>
+      <c r="J246" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQ5_FL, "IRQ5_FL", 29, 1, 0);</v>
+      </c>
+    </row>
+    <row r="247" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B247">
         <v>15</v>
       </c>
-      <c r="E202">
-        <v>1</v>
-      </c>
-      <c r="F202">
-        <v>0</v>
-      </c>
-      <c r="H202" t="str">
-        <f>"class IOPDmacRegister_"&amp;A202&amp;"_t;"</f>
-        <v>class IOPDmacRegister_ICR_t;</v>
-      </c>
-      <c r="I202" t="str">
-        <f t="shared" ref="I202" si="43">"static constexpr u8 "&amp;C202&amp;" = "&amp;B202&amp;";"</f>
-        <v>static constexpr u8 IRQFORCE = 0;</v>
-      </c>
-      <c r="J202" t="str">
-        <f t="shared" ref="J202" si="44">"registerField(Fields::"&amp;C202&amp;", """&amp;C202&amp;""", "&amp;D202&amp;", "&amp;E202&amp;", "&amp;F202&amp;");"</f>
-        <v>registerField(Fields::IRQFORCE, "IRQFORCE", 15, 1, 0);</v>
-      </c>
-    </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B203">
-        <v>1</v>
-      </c>
-      <c r="C203" t="s">
-        <v>178</v>
-      </c>
-      <c r="D203">
+      <c r="C247" t="s">
+        <v>188</v>
+      </c>
+      <c r="D247">
+        <v>30</v>
+      </c>
+      <c r="E247">
+        <v>1</v>
+      </c>
+      <c r="F247">
+        <v>0</v>
+      </c>
+      <c r="I247" t="str">
+        <f t="shared" si="51"/>
+        <v>static constexpr u8 IRQ6_FL = 15;</v>
+      </c>
+      <c r="J247" t="str">
+        <f t="shared" si="52"/>
+        <v>registerField(Fields::IRQ6_FL, "IRQ6_FL", 30, 1, 0);</v>
+      </c>
+    </row>
+    <row r="248" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B248">
         <v>16</v>
       </c>
-      <c r="E203">
-        <v>1</v>
-      </c>
-      <c r="F203">
-        <v>0</v>
-      </c>
-      <c r="I203" t="str">
-        <f t="shared" ref="I203:I218" si="45">"static constexpr u8 "&amp;C203&amp;" = "&amp;B203&amp;";"</f>
-        <v>static constexpr u8 IRQ0_EN = 1;</v>
-      </c>
-      <c r="J203" t="str">
-        <f t="shared" ref="J203:J218" si="46">"registerField(Fields::"&amp;C203&amp;", """&amp;C203&amp;""", "&amp;D203&amp;", "&amp;E203&amp;", "&amp;F203&amp;");"</f>
-        <v>registerField(Fields::IRQ0_EN, "IRQ0_EN", 16, 1, 0);</v>
-      </c>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B204">
-        <v>2</v>
-      </c>
-      <c r="C204" t="s">
-        <v>179</v>
-      </c>
-      <c r="D204">
-        <v>17</v>
-      </c>
-      <c r="E204">
-        <v>1</v>
-      </c>
-      <c r="F204">
-        <v>0</v>
-      </c>
-      <c r="I204" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQ1_EN = 2;</v>
-      </c>
-      <c r="J204" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQ1_EN, "IRQ1_EN", 17, 1, 0);</v>
-      </c>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B205">
-        <v>3</v>
-      </c>
-      <c r="C205" t="s">
-        <v>180</v>
-      </c>
-      <c r="D205">
-        <v>18</v>
-      </c>
-      <c r="E205">
-        <v>1</v>
-      </c>
-      <c r="F205">
-        <v>0</v>
-      </c>
-      <c r="I205" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQ2_EN = 3;</v>
-      </c>
-      <c r="J205" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQ2_EN, "IRQ2_EN", 18, 1, 0);</v>
-      </c>
-    </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B206">
-        <v>4</v>
-      </c>
-      <c r="C206" t="s">
-        <v>181</v>
-      </c>
-      <c r="D206">
-        <v>19</v>
-      </c>
-      <c r="E206">
-        <v>1</v>
-      </c>
-      <c r="F206">
-        <v>0</v>
-      </c>
-      <c r="I206" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQ3_EN = 4;</v>
-      </c>
-      <c r="J206" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQ3_EN, "IRQ3_EN", 19, 1, 0);</v>
-      </c>
-    </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B207">
-        <v>5</v>
-      </c>
-      <c r="C207" t="s">
-        <v>182</v>
-      </c>
-      <c r="D207">
-        <v>20</v>
-      </c>
-      <c r="E207">
-        <v>1</v>
-      </c>
-      <c r="F207">
-        <v>0</v>
-      </c>
-      <c r="I207" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQ4_EN = 5;</v>
-      </c>
-      <c r="J207" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQ4_EN, "IRQ4_EN", 20, 1, 0);</v>
-      </c>
-    </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B208">
-        <v>6</v>
-      </c>
-      <c r="C208" t="s">
-        <v>183</v>
-      </c>
-      <c r="D208">
-        <v>21</v>
-      </c>
-      <c r="E208">
-        <v>1</v>
-      </c>
-      <c r="F208">
-        <v>0</v>
-      </c>
-      <c r="I208" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQ5_EN = 6;</v>
-      </c>
-      <c r="J208" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQ5_EN, "IRQ5_EN", 21, 1, 0);</v>
-      </c>
-    </row>
-    <row r="209" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B209">
-        <v>7</v>
-      </c>
-      <c r="C209" t="s">
-        <v>184</v>
-      </c>
-      <c r="D209">
-        <v>22</v>
-      </c>
-      <c r="E209">
-        <v>1</v>
-      </c>
-      <c r="F209">
-        <v>0</v>
-      </c>
-      <c r="I209" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQ6_EN = 7;</v>
-      </c>
-      <c r="J209" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQ6_EN, "IRQ6_EN", 22, 1, 0);</v>
-      </c>
-    </row>
-    <row r="210" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B210">
-        <v>8</v>
-      </c>
-      <c r="C210" t="s">
-        <v>193</v>
-      </c>
-      <c r="D210">
-        <v>23</v>
-      </c>
-      <c r="E210">
-        <v>1</v>
-      </c>
-      <c r="F210">
-        <v>0</v>
-      </c>
-      <c r="I210" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQENABLE = 8;</v>
-      </c>
-      <c r="J210" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQENABLE, "IRQENABLE", 23, 1, 0);</v>
-      </c>
-    </row>
-    <row r="211" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B211">
-        <v>9</v>
-      </c>
-      <c r="C211" t="s">
-        <v>185</v>
-      </c>
-      <c r="D211">
-        <v>24</v>
-      </c>
-      <c r="E211">
-        <v>1</v>
-      </c>
-      <c r="F211">
-        <v>0</v>
-      </c>
-      <c r="I211" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQ0_FL = 9;</v>
-      </c>
-      <c r="J211" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQ0_FL, "IRQ0_FL", 24, 1, 0);</v>
-      </c>
-    </row>
-    <row r="212" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B212">
-        <v>10</v>
-      </c>
-      <c r="C212" t="s">
-        <v>186</v>
-      </c>
-      <c r="D212">
-        <v>25</v>
-      </c>
-      <c r="E212">
-        <v>1</v>
-      </c>
-      <c r="F212">
-        <v>0</v>
-      </c>
-      <c r="I212" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQ1_FL = 10;</v>
-      </c>
-      <c r="J212" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQ1_FL, "IRQ1_FL", 25, 1, 0);</v>
-      </c>
-    </row>
-    <row r="213" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B213">
-        <v>11</v>
-      </c>
-      <c r="C213" t="s">
-        <v>187</v>
-      </c>
-      <c r="D213">
-        <v>26</v>
-      </c>
-      <c r="E213">
-        <v>1</v>
-      </c>
-      <c r="F213">
-        <v>0</v>
-      </c>
-      <c r="I213" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQ2_FL = 11;</v>
-      </c>
-      <c r="J213" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQ2_FL, "IRQ2_FL", 26, 1, 0);</v>
-      </c>
-    </row>
-    <row r="214" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B214">
-        <v>12</v>
-      </c>
-      <c r="C214" t="s">
-        <v>188</v>
-      </c>
-      <c r="D214">
-        <v>27</v>
-      </c>
-      <c r="E214">
-        <v>1</v>
-      </c>
-      <c r="F214">
-        <v>0</v>
-      </c>
-      <c r="I214" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQ3_FL = 12;</v>
-      </c>
-      <c r="J214" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQ3_FL, "IRQ3_FL", 27, 1, 0);</v>
-      </c>
-    </row>
-    <row r="215" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B215">
-        <v>13</v>
-      </c>
-      <c r="C215" t="s">
+      <c r="C248" t="s">
         <v>189</v>
       </c>
-      <c r="D215">
-        <v>28</v>
-      </c>
-      <c r="E215">
-        <v>1</v>
-      </c>
-      <c r="F215">
-        <v>0</v>
-      </c>
-      <c r="I215" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQ4_FL = 13;</v>
-      </c>
-      <c r="J215" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQ4_FL, "IRQ4_FL", 28, 1, 0);</v>
-      </c>
-    </row>
-    <row r="216" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B216">
-        <v>14</v>
-      </c>
-      <c r="C216" t="s">
-        <v>190</v>
-      </c>
-      <c r="D216">
-        <v>29</v>
-      </c>
-      <c r="E216">
-        <v>1</v>
-      </c>
-      <c r="F216">
-        <v>0</v>
-      </c>
-      <c r="I216" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQ5_FL = 14;</v>
-      </c>
-      <c r="J216" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQ5_FL, "IRQ5_FL", 29, 1, 0);</v>
-      </c>
-    </row>
-    <row r="217" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B217">
-        <v>15</v>
-      </c>
-      <c r="C217" t="s">
-        <v>191</v>
-      </c>
-      <c r="D217">
-        <v>30</v>
-      </c>
-      <c r="E217">
-        <v>1</v>
-      </c>
-      <c r="F217">
-        <v>0</v>
-      </c>
-      <c r="I217" t="str">
-        <f t="shared" si="45"/>
-        <v>static constexpr u8 IRQ6_FL = 15;</v>
-      </c>
-      <c r="J217" t="str">
-        <f t="shared" si="46"/>
-        <v>registerField(Fields::IRQ6_FL, "IRQ6_FL", 30, 1, 0);</v>
-      </c>
-    </row>
-    <row r="218" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B218">
-        <v>16</v>
-      </c>
-      <c r="C218" t="s">
-        <v>192</v>
-      </c>
-      <c r="D218">
+      <c r="D248">
         <v>31</v>
       </c>
-      <c r="E218">
-        <v>1</v>
-      </c>
-      <c r="F218">
-        <v>0</v>
-      </c>
-      <c r="I218" t="str">
-        <f t="shared" si="45"/>
+      <c r="E248">
+        <v>1</v>
+      </c>
+      <c r="F248">
+        <v>0</v>
+      </c>
+      <c r="I248" t="str">
+        <f t="shared" si="51"/>
         <v>static constexpr u8 IRQMASTER = 16;</v>
       </c>
-      <c r="J218" t="str">
-        <f t="shared" si="46"/>
+      <c r="J248" t="str">
+        <f t="shared" si="52"/>
         <v>registerField(Fields::IRQMASTER, "IRQMASTER", 31, 1, 0);</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initial commit of working IOP timers.. still a lot left unimplemented, but basics (sysclock count, interrupting) working.
</commit_message>
<xml_diff>
--- a/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
+++ b/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\Dev\Projects\PCSX2_Rewrite\PCSX2_Core\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="229">
   <si>
     <t>Field Name</t>
   </si>
@@ -672,6 +672,45 @@
   </si>
   <si>
     <t>FDMA</t>
+  </si>
+  <si>
+    <t>SyncMode</t>
+  </si>
+  <si>
+    <t>SyncEnable</t>
+  </si>
+  <si>
+    <t>ResetMode</t>
+  </si>
+  <si>
+    <t>IrqOnTarget</t>
+  </si>
+  <si>
+    <t>IrqOnOF</t>
+  </si>
+  <si>
+    <t>IrqToggle</t>
+  </si>
+  <si>
+    <t>IrqRepeat</t>
+  </si>
+  <si>
+    <t>ClockSrc</t>
+  </si>
+  <si>
+    <t>IrqRequest</t>
+  </si>
+  <si>
+    <t>ReachTarget</t>
+  </si>
+  <si>
+    <t>ReachOF</t>
+  </si>
+  <si>
+    <t>Prescale0</t>
+  </si>
+  <si>
+    <t>Prescale1</t>
   </si>
 </sst>
 </file>
@@ -989,26 +1028,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J248"/>
+  <dimension ref="A1:J262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="I186" sqref="I186"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="E263" sqref="E263"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="46.5703125" customWidth="1"/>
     <col min="9" max="9" width="32" customWidth="1"/>
-    <col min="10" max="10" width="43.109375" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1037,7 +1076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -1069,7 +1108,7 @@
         <v>registerField(Fields::R, "R", 0, 32, 0);</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1101,7 +1140,7 @@
         <v>registerField(Fields::C, "C", 0, 32, 0);</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1133,7 +1172,7 @@
         <v>registerField(Fields::CL, "CL", 0, 8, 0);</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1</v>
       </c>
@@ -1158,7 +1197,7 @@
         <v>registerField(Fields::WL, "WL", 8, 8, 0);</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1190,7 +1229,7 @@
         <v>registerField(Fields::m0, "m0", 0, 2, 0);</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1</v>
       </c>
@@ -1215,7 +1254,7 @@
         <v>registerField(Fields::m1, "m1", 2, 2, 0);</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2</v>
       </c>
@@ -1240,7 +1279,7 @@
         <v>registerField(Fields::m2, "m2", 4, 2, 0);</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>3</v>
       </c>
@@ -1265,7 +1304,7 @@
         <v>registerField(Fields::m3, "m3", 6, 2, 0);</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>4</v>
       </c>
@@ -1290,7 +1329,7 @@
         <v>registerField(Fields::m4, "m4", 8, 2, 0);</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>5</v>
       </c>
@@ -1315,7 +1354,7 @@
         <v>registerField(Fields::m5, "m5", 10, 2, 0);</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>6</v>
       </c>
@@ -1340,7 +1379,7 @@
         <v>registerField(Fields::m6, "m6", 12, 2, 0);</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>7</v>
       </c>
@@ -1365,7 +1404,7 @@
         <v>registerField(Fields::m7, "m7", 14, 2, 0);</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>8</v>
       </c>
@@ -1390,7 +1429,7 @@
         <v>registerField(Fields::m8, "m8", 16, 2, 0);</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>9</v>
       </c>
@@ -1415,7 +1454,7 @@
         <v>registerField(Fields::m9, "m9", 18, 2, 0);</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>10</v>
       </c>
@@ -1440,7 +1479,7 @@
         <v>registerField(Fields::m10, "m10", 20, 2, 0);</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>11</v>
       </c>
@@ -1465,7 +1504,7 @@
         <v>registerField(Fields::m11, "m11", 22, 2, 0);</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>12</v>
       </c>
@@ -1490,7 +1529,7 @@
         <v>registerField(Fields::m12, "m12", 24, 2, 0);</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>13</v>
       </c>
@@ -1515,7 +1554,7 @@
         <v>registerField(Fields::m13, "m13", 26, 2, 0);</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>14</v>
       </c>
@@ -1540,7 +1579,7 @@
         <v>registerField(Fields::m14, "m14", 28, 2, 0);</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>15</v>
       </c>
@@ -1565,7 +1604,7 @@
         <v>registerField(Fields::m15, "m15", 30, 2, 0);</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1597,7 +1636,7 @@
         <v>registerField(Fields::MOD, "MOD", 0, 2, 0);</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1629,7 +1668,7 @@
         <v>registerField(Fields::ITOP, "ITOP", 0, 10, 0);</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1661,7 +1700,7 @@
         <v>registerField(Fields::ITOPS, "ITOPS", 0, 10, 0);</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1693,7 +1732,7 @@
         <v>registerField(Fields::BASE, "BASE", 0, 10, 0);</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1725,7 +1764,7 @@
         <v>registerField(Fields::OFFSET, "OFFSET", 0, 10, 0);</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1757,7 +1796,7 @@
         <v>registerField(Fields::TOP, "TOP", 0, 10, 0);</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1789,7 +1828,7 @@
         <v>registerField(Fields::TOPS, "TOPS", 0, 10, 0);</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1821,7 +1860,7 @@
         <v>registerField(Fields::MARK, "MARK", 0, 16, 0);</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1853,7 +1892,7 @@
         <v>registerField(Fields::NUM, "NUM", 0, 8, 0);</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -1885,7 +1924,7 @@
         <v>registerField(Fields::IMMEDIATE, "IMMEDIATE", 0, 16, 0);</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>1</v>
       </c>
@@ -1910,7 +1949,7 @@
         <v>registerField(Fields::NUM, "NUM", 16, 8, 0);</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>2</v>
       </c>
@@ -1935,7 +1974,7 @@
         <v>registerField(Fields::CMD, "CMD", 24, 8, 0);</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -1967,7 +2006,7 @@
         <v>registerField(Fields::VPS, "VPS", 0, 2, 0);</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>1</v>
       </c>
@@ -1992,7 +2031,7 @@
         <v>registerField(Fields::VEW, "VEW", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>2</v>
       </c>
@@ -2017,7 +2056,7 @@
         <v>registerField(Fields::VGW, "VGW", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>3</v>
       </c>
@@ -2042,7 +2081,7 @@
         <v>registerField(Fields::MRK, "MRK", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>4</v>
       </c>
@@ -2067,7 +2106,7 @@
         <v>registerField(Fields::DBF, "DBF", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>5</v>
       </c>
@@ -2092,7 +2131,7 @@
         <v>registerField(Fields::VSS, "VSS", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>6</v>
       </c>
@@ -2117,7 +2156,7 @@
         <v>registerField(Fields::VFS, "VFS", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>7</v>
       </c>
@@ -2142,7 +2181,7 @@
         <v>registerField(Fields::VIS, "VIS", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>8</v>
       </c>
@@ -2167,7 +2206,7 @@
         <v>registerField(Fields::INT, "INT", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>9</v>
       </c>
@@ -2192,7 +2231,7 @@
         <v>registerField(Fields::ER0, "ER0", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>10</v>
       </c>
@@ -2217,7 +2256,7 @@
         <v>registerField(Fields::ER1, "ER1", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>11</v>
       </c>
@@ -2242,7 +2281,7 @@
         <v>registerField(Fields::FDR, "FDR", 23, 1, 0);</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>12</v>
       </c>
@@ -2267,7 +2306,7 @@
         <v>registerField(Fields::FQC, "FQC", 24, 4, 0);</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>55</v>
       </c>
@@ -2299,7 +2338,7 @@
         <v>registerField(Fields::RST, "RST", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>1</v>
       </c>
@@ -2324,7 +2363,7 @@
         <v>registerField(Fields::FBK, "FBK", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>2</v>
       </c>
@@ -2349,7 +2388,7 @@
         <v>registerField(Fields::STP, "STP", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>3</v>
       </c>
@@ -2374,7 +2413,7 @@
         <v>registerField(Fields::STC, "STC", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>60</v>
       </c>
@@ -2406,7 +2445,7 @@
         <v>registerField(Fields::MII, "MII", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>1</v>
       </c>
@@ -2431,7 +2470,7 @@
         <v>registerField(Fields::ME0, "ME0", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>2</v>
       </c>
@@ -2456,7 +2495,7 @@
         <v>registerField(Fields::ME1, "ME1", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -2488,7 +2527,7 @@
         <v>registerField(Fields::Zw, "Zw", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>1</v>
       </c>
@@ -2513,7 +2552,7 @@
         <v>registerField(Fields::Zz, "Zz", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>2</v>
       </c>
@@ -2538,7 +2577,7 @@
         <v>registerField(Fields::Zy, "Zy", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>3</v>
       </c>
@@ -2563,7 +2602,7 @@
         <v>registerField(Fields::Zx, "Zx", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>4</v>
       </c>
@@ -2588,7 +2627,7 @@
         <v>registerField(Fields::Sw, "Sw", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>5</v>
       </c>
@@ -2613,7 +2652,7 @@
         <v>registerField(Fields::Sz, "Sz", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>6</v>
       </c>
@@ -2638,7 +2677,7 @@
         <v>registerField(Fields::Sy, "Sy", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>7</v>
       </c>
@@ -2663,7 +2702,7 @@
         <v>registerField(Fields::Sx, "Sx", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>8</v>
       </c>
@@ -2688,7 +2727,7 @@
         <v>registerField(Fields::Uw, "Uw", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>9</v>
       </c>
@@ -2713,7 +2752,7 @@
         <v>registerField(Fields::Uz, "Uz", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>10</v>
       </c>
@@ -2738,7 +2777,7 @@
         <v>registerField(Fields::Uy, "Uy", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>11</v>
       </c>
@@ -2763,7 +2802,7 @@
         <v>registerField(Fields::Ux, "Ux", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>12</v>
       </c>
@@ -2788,7 +2827,7 @@
         <v>registerField(Fields::Ow, "Ow", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>13</v>
       </c>
@@ -2813,7 +2852,7 @@
         <v>registerField(Fields::Oz, "Oz", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>14</v>
       </c>
@@ -2838,7 +2877,7 @@
         <v>registerField(Fields::Oy, "Oy", 14, 1, 0);</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>15</v>
       </c>
@@ -2863,7 +2902,7 @@
         <v>registerField(Fields::Ox, "Ox", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>85</v>
       </c>
@@ -2895,7 +2934,7 @@
         <v>registerField(Fields::Z, "Z", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>1</v>
       </c>
@@ -2920,7 +2959,7 @@
         <v>registerField(Fields::S, "S", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>2</v>
       </c>
@@ -2945,7 +2984,7 @@
         <v>registerField(Fields::U, "U", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>3</v>
       </c>
@@ -2970,7 +3009,7 @@
         <v>registerField(Fields::O, "O", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>4</v>
       </c>
@@ -2995,7 +3034,7 @@
         <v>registerField(Fields::I, "I", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>5</v>
       </c>
@@ -3020,7 +3059,7 @@
         <v>registerField(Fields::D, "D", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>6</v>
       </c>
@@ -3045,7 +3084,7 @@
         <v>registerField(Fields::ZS, "ZS", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>7</v>
       </c>
@@ -3070,7 +3109,7 @@
         <v>registerField(Fields::SS, "SS", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>8</v>
       </c>
@@ -3095,7 +3134,7 @@
         <v>registerField(Fields::US, "US", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>9</v>
       </c>
@@ -3120,7 +3159,7 @@
         <v>registerField(Fields::OS, "OS", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>10</v>
       </c>
@@ -3145,7 +3184,7 @@
         <v>registerField(Fields::IS, "IS", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>11</v>
       </c>
@@ -3170,7 +3209,7 @@
         <v>registerField(Fields::DS, "DS", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>98</v>
       </c>
@@ -3202,7 +3241,7 @@
         <v>registerField(Fields::NegX_0, "NegX_0", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>1</v>
       </c>
@@ -3227,7 +3266,7 @@
         <v>registerField(Fields::PosX_0, "PosX_0", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>2</v>
       </c>
@@ -3252,7 +3291,7 @@
         <v>registerField(Fields::NegY_0, "NegY_0", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>3</v>
       </c>
@@ -3277,7 +3316,7 @@
         <v>registerField(Fields::PosY_0, "PosY_0", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>4</v>
       </c>
@@ -3302,7 +3341,7 @@
         <v>registerField(Fields::NegZ_0, "NegZ_0", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>5</v>
       </c>
@@ -3327,7 +3366,7 @@
         <v>registerField(Fields::PosZ_0, "PosZ_0", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>6</v>
       </c>
@@ -3352,7 +3391,7 @@
         <v>registerField(Fields::NegX_1, "NegX_1", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>7</v>
       </c>
@@ -3377,7 +3416,7 @@
         <v>registerField(Fields::PosX_1, "PosX_1", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>8</v>
       </c>
@@ -3402,7 +3441,7 @@
         <v>registerField(Fields::NegY_1, "NegY_1", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>9</v>
       </c>
@@ -3427,7 +3466,7 @@
         <v>registerField(Fields::PosY_1, "PosY_1", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>10</v>
       </c>
@@ -3452,7 +3491,7 @@
         <v>registerField(Fields::NegZ_1, "NegZ_1", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B112">
         <v>11</v>
       </c>
@@ -3477,7 +3516,7 @@
         <v>registerField(Fields::PosZ_1, "PosZ_1", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B113">
         <v>12</v>
       </c>
@@ -3502,7 +3541,7 @@
         <v>registerField(Fields::NegX_2, "NegX_2", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B114">
         <v>13</v>
       </c>
@@ -3527,7 +3566,7 @@
         <v>registerField(Fields::PosX_2, "PosX_2", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B115">
         <v>14</v>
       </c>
@@ -3552,7 +3591,7 @@
         <v>registerField(Fields::NegY_2, "NegY_2", 14, 1, 0);</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B116">
         <v>15</v>
       </c>
@@ -3577,7 +3616,7 @@
         <v>registerField(Fields::PosY_2, "PosY_2", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B117">
         <v>16</v>
       </c>
@@ -3602,7 +3641,7 @@
         <v>registerField(Fields::NegZ_2, "NegZ_2", 16, 1, 0);</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B118">
         <v>17</v>
       </c>
@@ -3627,7 +3666,7 @@
         <v>registerField(Fields::PosZ_2, "PosZ_2", 17, 1, 0);</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B119">
         <v>18</v>
       </c>
@@ -3652,7 +3691,7 @@
         <v>registerField(Fields::NegX_3, "NegX_3", 18, 1, 0);</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B120">
         <v>19</v>
       </c>
@@ -3677,7 +3716,7 @@
         <v>registerField(Fields::PosX_3, "PosX_3", 19, 1, 0);</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B121">
         <v>20</v>
       </c>
@@ -3702,7 +3741,7 @@
         <v>registerField(Fields::NegY_3, "NegY_3", 20, 1, 0);</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>21</v>
       </c>
@@ -3727,7 +3766,7 @@
         <v>registerField(Fields::PosY_3, "PosY_3", 21, 1, 0);</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>22</v>
       </c>
@@ -3752,7 +3791,7 @@
         <v>registerField(Fields::NegZ_3, "NegZ_3", 22, 1, 0);</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>23</v>
       </c>
@@ -3777,7 +3816,7 @@
         <v>registerField(Fields::PosZ_3, "PosZ_3", 23, 1, 0);</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>123</v>
       </c>
@@ -3809,7 +3848,7 @@
         <v>registerField(Fields::CMSAR, "CMSAR", 0, 16, 0);</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>55</v>
       </c>
@@ -3841,7 +3880,7 @@
         <v>registerField(Fields::FB0, "FB0", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B129">
         <v>1</v>
       </c>
@@ -3866,7 +3905,7 @@
         <v>registerField(Fields::RS0, "RS0", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B130">
         <v>2</v>
       </c>
@@ -3891,7 +3930,7 @@
         <v>registerField(Fields::DE0, "DE0", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B131">
         <v>3</v>
       </c>
@@ -3916,7 +3955,7 @@
         <v>registerField(Fields::TE0, "TE0", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B132">
         <v>4</v>
       </c>
@@ -3941,7 +3980,7 @@
         <v>registerField(Fields::FB1, "FB1", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B133">
         <v>5</v>
       </c>
@@ -3966,7 +4005,7 @@
         <v>registerField(Fields::RS1, "RS1", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B134">
         <v>6</v>
       </c>
@@ -3991,7 +4030,7 @@
         <v>registerField(Fields::DE1, "DE1", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B135">
         <v>7</v>
       </c>
@@ -4016,7 +4055,7 @@
         <v>registerField(Fields::TE1, "TE1", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>44</v>
       </c>
@@ -4048,7 +4087,7 @@
         <v>registerField(Fields::VBS0, "VBS0", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B138">
         <v>1</v>
       </c>
@@ -4073,7 +4112,7 @@
         <v>registerField(Fields::VDS0, "VDS0", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B139">
         <v>2</v>
       </c>
@@ -4098,7 +4137,7 @@
         <v>registerField(Fields::VTS0, "VTS0", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B140">
         <v>3</v>
       </c>
@@ -4123,7 +4162,7 @@
         <v>registerField(Fields::VFS0, "VFS0", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B141">
         <v>4</v>
       </c>
@@ -4148,7 +4187,7 @@
         <v>registerField(Fields::DIV0, "DIV0", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B142">
         <v>5</v>
       </c>
@@ -4173,7 +4212,7 @@
         <v>registerField(Fields::IBS0, "IBS0", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B143">
         <v>6</v>
       </c>
@@ -4198,7 +4237,7 @@
         <v>registerField(Fields::VBS1, "VBS1", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B144">
         <v>7</v>
       </c>
@@ -4223,7 +4262,7 @@
         <v>registerField(Fields::VDS1, "VDS1", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B145">
         <v>8</v>
       </c>
@@ -4248,7 +4287,7 @@
         <v>registerField(Fields::VTS1, "VTS1", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B146">
         <v>9</v>
       </c>
@@ -4273,7 +4312,7 @@
         <v>registerField(Fields::VFS1, "VFS1", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B147">
         <v>10</v>
       </c>
@@ -4298,7 +4337,7 @@
         <v>registerField(Fields::VGW1, "VGW1", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B148">
         <v>11</v>
       </c>
@@ -4323,7 +4362,7 @@
         <v>registerField(Fields::DIV1, "DIV1", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B149">
         <v>12</v>
       </c>
@@ -4348,7 +4387,7 @@
         <v>registerField(Fields::EFU1, "EFU1", 14, 1, 0);</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>145</v>
       </c>
@@ -4380,7 +4419,7 @@
         <v>registerField(Fields::BS, "BS", 0, 16, 0);</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B152">
         <v>1</v>
       </c>
@@ -4405,7 +4444,7 @@
         <v>registerField(Fields::BA, "BA", 16, 16, 0);</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>148</v>
       </c>
@@ -4437,7 +4476,7 @@
         <v>registerField(Fields::TD, "TD", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B155">
         <v>1</v>
       </c>
@@ -4462,7 +4501,7 @@
         <v>registerField(Fields::MAS, "MAS", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B156">
         <v>2</v>
       </c>
@@ -4487,7 +4526,7 @@
         <v>registerField(Fields::CE, "CE", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B157">
         <v>3</v>
       </c>
@@ -4512,7 +4551,7 @@
         <v>registerField(Fields::SM, "SM", 9, 2, 0);</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B158">
         <v>4</v>
       </c>
@@ -4537,7 +4576,7 @@
         <v>registerField(Fields::C_DWS, "C_DWS", 16, 3, 0);</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B159">
         <v>5</v>
       </c>
@@ -4562,7 +4601,7 @@
         <v>registerField(Fields::C_CWS, "C_CWS", 20, 3, 0);</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B160">
         <v>6</v>
       </c>
@@ -4587,7 +4626,7 @@
         <v>registerField(Fields::START_B, "START_B", 24, 1, 0);</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B161">
         <v>7</v>
       </c>
@@ -4612,7 +4651,7 @@
         <v>registerField(Fields::START_T, "START_T", 28, 1, 0);</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>44</v>
       </c>
@@ -4644,7 +4683,7 @@
         <v>registerField(Fields::VBLNK, "VBLNK", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B164">
         <v>1</v>
       </c>
@@ -4669,7 +4708,7 @@
         <v>registerField(Fields::GPU, "GPU", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B165">
         <v>2</v>
       </c>
@@ -4694,7 +4733,7 @@
         <v>registerField(Fields::CDROM, "CDROM", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B166">
         <v>3</v>
       </c>
@@ -4719,7 +4758,7 @@
         <v>registerField(Fields::DMA, "DMA", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B167">
         <v>4</v>
       </c>
@@ -4744,7 +4783,7 @@
         <v>registerField(Fields::TMR0, "TMR0", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B168">
         <v>5</v>
       </c>
@@ -4769,7 +4808,7 @@
         <v>registerField(Fields::TMR1, "TMR1", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B169">
         <v>6</v>
       </c>
@@ -4794,7 +4833,7 @@
         <v>registerField(Fields::TMR2, "TMR2", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B170">
         <v>7</v>
       </c>
@@ -4819,7 +4858,7 @@
         <v>registerField(Fields::SIO0, "SIO0", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B171">
         <v>8</v>
       </c>
@@ -4844,7 +4883,7 @@
         <v>registerField(Fields::SIO1, "SIO1", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B172">
         <v>9</v>
       </c>
@@ -4869,7 +4908,7 @@
         <v>registerField(Fields::SPU, "SPU", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B173">
         <v>10</v>
       </c>
@@ -4894,7 +4933,7 @@
         <v>registerField(Fields::PIO, "PIO", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B174">
         <v>11</v>
       </c>
@@ -4919,7 +4958,7 @@
         <v>registerField(Fields::EVBLANK, "EVBLANK", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B175">
         <v>12</v>
       </c>
@@ -4944,7 +4983,7 @@
         <v>registerField(Fields::DVD, "DVD", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B176">
         <v>13</v>
       </c>
@@ -4969,7 +5008,7 @@
         <v>registerField(Fields::PCMCIA, "PCMCIA", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B177">
         <v>14</v>
       </c>
@@ -4994,7 +5033,7 @@
         <v>registerField(Fields::TMR3, "TMR3", 14, 1, 0);</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B178">
         <v>15</v>
       </c>
@@ -5019,7 +5058,7 @@
         <v>registerField(Fields::TMR4, "TMR4", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B179">
         <v>16</v>
       </c>
@@ -5044,7 +5083,7 @@
         <v>registerField(Fields::TMR5, "TMR5", 16, 1, 0);</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B180">
         <v>17</v>
       </c>
@@ -5069,7 +5108,7 @@
         <v>registerField(Fields::SIO2, "SIO2", 17, 1, 0);</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B181">
         <v>18</v>
       </c>
@@ -5094,7 +5133,7 @@
         <v>registerField(Fields::HTR0, "HTR0", 18, 1, 0);</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B182">
         <v>19</v>
       </c>
@@ -5119,7 +5158,7 @@
         <v>registerField(Fields::HTR1, "HTR1", 19, 1, 0);</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B183">
         <v>20</v>
       </c>
@@ -5144,7 +5183,7 @@
         <v>registerField(Fields::HTR2, "HTR2", 20, 1, 0);</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B184">
         <v>21</v>
       </c>
@@ -5169,7 +5208,7 @@
         <v>registerField(Fields::HTR3, "HTR3", 21, 1, 0);</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B185">
         <v>22</v>
       </c>
@@ -5194,7 +5233,7 @@
         <v>registerField(Fields::USB, "USB", 22, 1, 0);</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B186">
         <v>23</v>
       </c>
@@ -5219,7 +5258,7 @@
         <v>registerField(Fields::EXTR, "EXTR", 23, 1, 0);</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B187">
         <v>24</v>
       </c>
@@ -5244,7 +5283,7 @@
         <v>registerField(Fields::FWRE, "FWRE", 24, 1, 0);</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B188">
         <v>25</v>
       </c>
@@ -5269,7 +5308,7 @@
         <v>registerField(Fields::FDMA, "FDMA", 25, 1, 0);</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>13</v>
       </c>
@@ -5301,7 +5340,7 @@
         <v>registerField(Fields::VBLNK, "VBLNK", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B191">
         <v>1</v>
       </c>
@@ -5326,7 +5365,7 @@
         <v>registerField(Fields::GPU, "GPU", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B192">
         <v>2</v>
       </c>
@@ -5351,7 +5390,7 @@
         <v>registerField(Fields::CDROM, "CDROM", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="193" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B193">
         <v>3</v>
       </c>
@@ -5376,7 +5415,7 @@
         <v>registerField(Fields::DMA, "DMA", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="194" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B194">
         <v>4</v>
       </c>
@@ -5401,7 +5440,7 @@
         <v>registerField(Fields::TMR0, "TMR0", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="195" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B195">
         <v>5</v>
       </c>
@@ -5426,7 +5465,7 @@
         <v>registerField(Fields::TMR1, "TMR1", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="196" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B196">
         <v>6</v>
       </c>
@@ -5451,7 +5490,7 @@
         <v>registerField(Fields::TMR2, "TMR2", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="197" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B197">
         <v>7</v>
       </c>
@@ -5476,7 +5515,7 @@
         <v>registerField(Fields::SIO0, "SIO0", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="198" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B198">
         <v>8</v>
       </c>
@@ -5501,7 +5540,7 @@
         <v>registerField(Fields::SIO1, "SIO1", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="199" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B199">
         <v>9</v>
       </c>
@@ -5526,7 +5565,7 @@
         <v>registerField(Fields::SPU, "SPU", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="200" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B200">
         <v>10</v>
       </c>
@@ -5551,7 +5590,7 @@
         <v>registerField(Fields::PIO, "PIO", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="201" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B201">
         <v>11</v>
       </c>
@@ -5576,7 +5615,7 @@
         <v>registerField(Fields::EVBLANK, "EVBLANK", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="202" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B202">
         <v>12</v>
       </c>
@@ -5601,7 +5640,7 @@
         <v>registerField(Fields::DVD, "DVD", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="203" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B203">
         <v>13</v>
       </c>
@@ -5626,7 +5665,7 @@
         <v>registerField(Fields::PCMCIA, "PCMCIA", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="204" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B204">
         <v>14</v>
       </c>
@@ -5651,7 +5690,7 @@
         <v>registerField(Fields::TMR3, "TMR3", 14, 1, 0);</v>
       </c>
     </row>
-    <row r="205" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B205">
         <v>15</v>
       </c>
@@ -5676,7 +5715,7 @@
         <v>registerField(Fields::TMR4, "TMR4", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="206" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B206">
         <v>16</v>
       </c>
@@ -5701,7 +5740,7 @@
         <v>registerField(Fields::TMR5, "TMR5", 16, 1, 0);</v>
       </c>
     </row>
-    <row r="207" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B207">
         <v>17</v>
       </c>
@@ -5726,7 +5765,7 @@
         <v>registerField(Fields::SIO2, "SIO2", 17, 1, 0);</v>
       </c>
     </row>
-    <row r="208" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B208">
         <v>18</v>
       </c>
@@ -5751,7 +5790,7 @@
         <v>registerField(Fields::HTR0, "HTR0", 18, 1, 0);</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B209">
         <v>19</v>
       </c>
@@ -5776,7 +5815,7 @@
         <v>registerField(Fields::HTR1, "HTR1", 19, 1, 0);</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B210">
         <v>20</v>
       </c>
@@ -5801,7 +5840,7 @@
         <v>registerField(Fields::HTR2, "HTR2", 20, 1, 0);</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B211">
         <v>21</v>
       </c>
@@ -5826,7 +5865,7 @@
         <v>registerField(Fields::HTR3, "HTR3", 21, 1, 0);</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B212">
         <v>22</v>
       </c>
@@ -5851,7 +5890,7 @@
         <v>registerField(Fields::USB, "USB", 22, 1, 0);</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B213">
         <v>23</v>
       </c>
@@ -5876,7 +5915,7 @@
         <v>registerField(Fields::EXTR, "EXTR", 23, 1, 0);</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B214">
         <v>24</v>
       </c>
@@ -5901,7 +5940,7 @@
         <v>registerField(Fields::FWRE, "FWRE", 24, 1, 0);</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B215">
         <v>25</v>
       </c>
@@ -5926,7 +5965,7 @@
         <v>registerField(Fields::FDMA, "FDMA", 25, 1, 0);</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>158</v>
       </c>
@@ -5958,7 +5997,7 @@
         <v>registerField(Fields::PRI0, "PRI0", 0, 3, 0);</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B218">
         <v>1</v>
       </c>
@@ -5983,7 +6022,7 @@
         <v>registerField(Fields::ENA0, "ENA0", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B219">
         <v>2</v>
       </c>
@@ -6008,7 +6047,7 @@
         <v>registerField(Fields::PRI1, "PRI1", 4, 3, 0);</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B220">
         <v>3</v>
       </c>
@@ -6033,7 +6072,7 @@
         <v>registerField(Fields::ENA1, "ENA1", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B221">
         <v>4</v>
       </c>
@@ -6058,7 +6097,7 @@
         <v>registerField(Fields::PRI2, "PRI2", 8, 3, 0);</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B222">
         <v>5</v>
       </c>
@@ -6083,7 +6122,7 @@
         <v>registerField(Fields::ENA2, "ENA2", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B223">
         <v>6</v>
       </c>
@@ -6108,7 +6147,7 @@
         <v>registerField(Fields::PRI3, "PRI3", 12, 3, 0);</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B224">
         <v>7</v>
       </c>
@@ -6133,7 +6172,7 @@
         <v>registerField(Fields::ENA3, "ENA3", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B225">
         <v>8</v>
       </c>
@@ -6158,7 +6197,7 @@
         <v>registerField(Fields::PRI4, "PRI4", 16, 3, 0);</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B226">
         <v>9</v>
       </c>
@@ -6183,7 +6222,7 @@
         <v>registerField(Fields::ENA4, "ENA4", 19, 1, 0);</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B227">
         <v>10</v>
       </c>
@@ -6208,7 +6247,7 @@
         <v>registerField(Fields::PRI5, "PRI5", 20, 3, 0);</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B228">
         <v>11</v>
       </c>
@@ -6233,7 +6272,7 @@
         <v>registerField(Fields::ENA5, "ENA5", 23, 1, 0);</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B229">
         <v>12</v>
       </c>
@@ -6258,7 +6297,7 @@
         <v>registerField(Fields::PRI6, "PRI6", 24, 3, 0);</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B230">
         <v>13</v>
       </c>
@@ -6283,7 +6322,7 @@
         <v>registerField(Fields::ENA6, "ENA6", 27, 1, 0);</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>173</v>
       </c>
@@ -6315,7 +6354,7 @@
         <v>registerField(Fields::IRQFORCE, "IRQFORCE", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B233">
         <v>1</v>
       </c>
@@ -6340,7 +6379,7 @@
         <v>registerField(Fields::IRQ0_EN, "IRQ0_EN", 16, 1, 0);</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B234">
         <v>2</v>
       </c>
@@ -6365,7 +6404,7 @@
         <v>registerField(Fields::IRQ1_EN, "IRQ1_EN", 17, 1, 0);</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B235">
         <v>3</v>
       </c>
@@ -6390,7 +6429,7 @@
         <v>registerField(Fields::IRQ2_EN, "IRQ2_EN", 18, 1, 0);</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B236">
         <v>4</v>
       </c>
@@ -6415,7 +6454,7 @@
         <v>registerField(Fields::IRQ3_EN, "IRQ3_EN", 19, 1, 0);</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B237">
         <v>5</v>
       </c>
@@ -6440,7 +6479,7 @@
         <v>registerField(Fields::IRQ4_EN, "IRQ4_EN", 20, 1, 0);</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B238">
         <v>6</v>
       </c>
@@ -6465,7 +6504,7 @@
         <v>registerField(Fields::IRQ5_EN, "IRQ5_EN", 21, 1, 0);</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B239">
         <v>7</v>
       </c>
@@ -6490,7 +6529,7 @@
         <v>registerField(Fields::IRQ6_EN, "IRQ6_EN", 22, 1, 0);</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B240">
         <v>8</v>
       </c>
@@ -6515,7 +6554,7 @@
         <v>registerField(Fields::IRQENABLE, "IRQENABLE", 23, 1, 0);</v>
       </c>
     </row>
-    <row r="241" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B241">
         <v>9</v>
       </c>
@@ -6540,7 +6579,7 @@
         <v>registerField(Fields::IRQ0_FL, "IRQ0_FL", 24, 1, 0);</v>
       </c>
     </row>
-    <row r="242" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B242">
         <v>10</v>
       </c>
@@ -6565,7 +6604,7 @@
         <v>registerField(Fields::IRQ1_FL, "IRQ1_FL", 25, 1, 0);</v>
       </c>
     </row>
-    <row r="243" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B243">
         <v>11</v>
       </c>
@@ -6590,7 +6629,7 @@
         <v>registerField(Fields::IRQ2_FL, "IRQ2_FL", 26, 1, 0);</v>
       </c>
     </row>
-    <row r="244" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B244">
         <v>12</v>
       </c>
@@ -6615,7 +6654,7 @@
         <v>registerField(Fields::IRQ3_FL, "IRQ3_FL", 27, 1, 0);</v>
       </c>
     </row>
-    <row r="245" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B245">
         <v>13</v>
       </c>
@@ -6640,7 +6679,7 @@
         <v>registerField(Fields::IRQ4_FL, "IRQ4_FL", 28, 1, 0);</v>
       </c>
     </row>
-    <row r="246" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B246">
         <v>14</v>
       </c>
@@ -6665,7 +6704,7 @@
         <v>registerField(Fields::IRQ5_FL, "IRQ5_FL", 29, 1, 0);</v>
       </c>
     </row>
-    <row r="247" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B247">
         <v>15</v>
       </c>
@@ -6690,7 +6729,7 @@
         <v>registerField(Fields::IRQ6_FL, "IRQ6_FL", 30, 1, 0);</v>
       </c>
     </row>
-    <row r="248" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B248">
         <v>16</v>
       </c>
@@ -6713,6 +6752,338 @@
       <c r="J248" t="str">
         <f t="shared" si="52"/>
         <v>registerField(Fields::IRQMASTER, "IRQMASTER", 31, 1, 0);</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>30</v>
+      </c>
+      <c r="B250">
+        <v>0</v>
+      </c>
+      <c r="C250" t="s">
+        <v>217</v>
+      </c>
+      <c r="D250">
+        <v>0</v>
+      </c>
+      <c r="E250">
+        <v>1</v>
+      </c>
+      <c r="F250">
+        <v>0</v>
+      </c>
+      <c r="H250" t="str">
+        <f>"class IOPTimersTimerRegister_"&amp;A250&amp;"_t;"</f>
+        <v>class IOPTimersTimerRegister_MODE_t;</v>
+      </c>
+      <c r="I250" t="str">
+        <f t="shared" ref="I250" si="53">"static constexpr u8 "&amp;C250&amp;" = "&amp;B250&amp;";"</f>
+        <v>static constexpr u8 SyncEnable = 0;</v>
+      </c>
+      <c r="J250" t="str">
+        <f t="shared" ref="J250" si="54">"registerField(Fields::"&amp;C250&amp;", """&amp;C250&amp;""", "&amp;D250&amp;", "&amp;E250&amp;", "&amp;F250&amp;");"</f>
+        <v>registerField(Fields::SyncEnable, "SyncEnable", 0, 1, 0);</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B251">
+        <v>1</v>
+      </c>
+      <c r="C251" t="s">
+        <v>216</v>
+      </c>
+      <c r="D251">
+        <v>1</v>
+      </c>
+      <c r="E251">
+        <v>2</v>
+      </c>
+      <c r="F251">
+        <v>0</v>
+      </c>
+      <c r="I251" t="str">
+        <f t="shared" ref="I251:I262" si="55">"static constexpr u8 "&amp;C251&amp;" = "&amp;B251&amp;";"</f>
+        <v>static constexpr u8 SyncMode = 1;</v>
+      </c>
+      <c r="J251" t="str">
+        <f t="shared" ref="J251:J262" si="56">"registerField(Fields::"&amp;C251&amp;", """&amp;C251&amp;""", "&amp;D251&amp;", "&amp;E251&amp;", "&amp;F251&amp;");"</f>
+        <v>registerField(Fields::SyncMode, "SyncMode", 1, 2, 0);</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B252">
+        <v>2</v>
+      </c>
+      <c r="C252" t="s">
+        <v>218</v>
+      </c>
+      <c r="D252">
+        <v>3</v>
+      </c>
+      <c r="E252">
+        <v>1</v>
+      </c>
+      <c r="F252">
+        <v>0</v>
+      </c>
+      <c r="I252" t="str">
+        <f t="shared" si="55"/>
+        <v>static constexpr u8 ResetMode = 2;</v>
+      </c>
+      <c r="J252" t="str">
+        <f t="shared" si="56"/>
+        <v>registerField(Fields::ResetMode, "ResetMode", 3, 1, 0);</v>
+      </c>
+    </row>
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B253">
+        <v>3</v>
+      </c>
+      <c r="C253" t="s">
+        <v>219</v>
+      </c>
+      <c r="D253">
+        <v>4</v>
+      </c>
+      <c r="E253">
+        <v>1</v>
+      </c>
+      <c r="F253">
+        <v>0</v>
+      </c>
+      <c r="I253" t="str">
+        <f t="shared" si="55"/>
+        <v>static constexpr u8 IrqOnTarget = 3;</v>
+      </c>
+      <c r="J253" t="str">
+        <f t="shared" si="56"/>
+        <v>registerField(Fields::IrqOnTarget, "IrqOnTarget", 4, 1, 0);</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B254">
+        <v>4</v>
+      </c>
+      <c r="C254" t="s">
+        <v>220</v>
+      </c>
+      <c r="D254">
+        <v>5</v>
+      </c>
+      <c r="E254">
+        <v>1</v>
+      </c>
+      <c r="F254">
+        <v>0</v>
+      </c>
+      <c r="I254" t="str">
+        <f t="shared" si="55"/>
+        <v>static constexpr u8 IrqOnOF = 4;</v>
+      </c>
+      <c r="J254" t="str">
+        <f t="shared" si="56"/>
+        <v>registerField(Fields::IrqOnOF, "IrqOnOF", 5, 1, 0);</v>
+      </c>
+    </row>
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B255">
+        <v>5</v>
+      </c>
+      <c r="C255" t="s">
+        <v>222</v>
+      </c>
+      <c r="D255">
+        <v>6</v>
+      </c>
+      <c r="E255">
+        <v>1</v>
+      </c>
+      <c r="F255">
+        <v>0</v>
+      </c>
+      <c r="I255" t="str">
+        <f t="shared" si="55"/>
+        <v>static constexpr u8 IrqRepeat = 5;</v>
+      </c>
+      <c r="J255" t="str">
+        <f t="shared" si="56"/>
+        <v>registerField(Fields::IrqRepeat, "IrqRepeat", 6, 1, 0);</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B256">
+        <v>6</v>
+      </c>
+      <c r="C256" t="s">
+        <v>221</v>
+      </c>
+      <c r="D256">
+        <v>7</v>
+      </c>
+      <c r="E256">
+        <v>1</v>
+      </c>
+      <c r="F256">
+        <v>0</v>
+      </c>
+      <c r="I256" t="str">
+        <f t="shared" si="55"/>
+        <v>static constexpr u8 IrqToggle = 6;</v>
+      </c>
+      <c r="J256" t="str">
+        <f t="shared" si="56"/>
+        <v>registerField(Fields::IrqToggle, "IrqToggle", 7, 1, 0);</v>
+      </c>
+    </row>
+    <row r="257" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B257">
+        <v>7</v>
+      </c>
+      <c r="C257" t="s">
+        <v>223</v>
+      </c>
+      <c r="D257">
+        <v>8</v>
+      </c>
+      <c r="E257">
+        <v>1</v>
+      </c>
+      <c r="F257">
+        <v>0</v>
+      </c>
+      <c r="I257" t="str">
+        <f t="shared" si="55"/>
+        <v>static constexpr u8 ClockSrc = 7;</v>
+      </c>
+      <c r="J257" t="str">
+        <f t="shared" si="56"/>
+        <v>registerField(Fields::ClockSrc, "ClockSrc", 8, 1, 0);</v>
+      </c>
+    </row>
+    <row r="258" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B258">
+        <v>8</v>
+      </c>
+      <c r="C258" t="s">
+        <v>227</v>
+      </c>
+      <c r="D258">
+        <v>9</v>
+      </c>
+      <c r="E258">
+        <v>1</v>
+      </c>
+      <c r="F258">
+        <v>0</v>
+      </c>
+      <c r="I258" t="str">
+        <f t="shared" si="55"/>
+        <v>static constexpr u8 Prescale0 = 8;</v>
+      </c>
+      <c r="J258" t="str">
+        <f t="shared" si="56"/>
+        <v>registerField(Fields::Prescale0, "Prescale0", 9, 1, 0);</v>
+      </c>
+    </row>
+    <row r="259" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B259">
+        <v>9</v>
+      </c>
+      <c r="C259" t="s">
+        <v>224</v>
+      </c>
+      <c r="D259">
+        <v>10</v>
+      </c>
+      <c r="E259">
+        <v>1</v>
+      </c>
+      <c r="F259">
+        <v>0</v>
+      </c>
+      <c r="I259" t="str">
+        <f t="shared" si="55"/>
+        <v>static constexpr u8 IrqRequest = 9;</v>
+      </c>
+      <c r="J259" t="str">
+        <f t="shared" si="56"/>
+        <v>registerField(Fields::IrqRequest, "IrqRequest", 10, 1, 0);</v>
+      </c>
+    </row>
+    <row r="260" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B260">
+        <v>10</v>
+      </c>
+      <c r="C260" t="s">
+        <v>225</v>
+      </c>
+      <c r="D260">
+        <v>11</v>
+      </c>
+      <c r="E260">
+        <v>1</v>
+      </c>
+      <c r="F260">
+        <v>0</v>
+      </c>
+      <c r="I260" t="str">
+        <f t="shared" si="55"/>
+        <v>static constexpr u8 ReachTarget = 10;</v>
+      </c>
+      <c r="J260" t="str">
+        <f t="shared" si="56"/>
+        <v>registerField(Fields::ReachTarget, "ReachTarget", 11, 1, 0);</v>
+      </c>
+    </row>
+    <row r="261" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B261">
+        <v>11</v>
+      </c>
+      <c r="C261" t="s">
+        <v>226</v>
+      </c>
+      <c r="D261">
+        <v>12</v>
+      </c>
+      <c r="E261">
+        <v>1</v>
+      </c>
+      <c r="F261">
+        <v>0</v>
+      </c>
+      <c r="I261" t="str">
+        <f t="shared" si="55"/>
+        <v>static constexpr u8 ReachOF = 11;</v>
+      </c>
+      <c r="J261" t="str">
+        <f t="shared" si="56"/>
+        <v>registerField(Fields::ReachOF, "ReachOF", 12, 1, 0);</v>
+      </c>
+    </row>
+    <row r="262" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B262">
+        <v>12</v>
+      </c>
+      <c r="C262" t="s">
+        <v>228</v>
+      </c>
+      <c r="D262">
+        <v>13</v>
+      </c>
+      <c r="E262">
+        <v>2</v>
+      </c>
+      <c r="F262">
+        <v>0</v>
+      </c>
+      <c r="I262" t="str">
+        <f t="shared" si="55"/>
+        <v>static constexpr u8 Prescale1 = 12;</v>
+      </c>
+      <c r="J262" t="str">
+        <f t="shared" si="56"/>
+        <v>registerField(Fields::Prescale1, "Prescale1", 13, 2, 0);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got IOP DMAC channel SIF1 to recieve data properly in (dest) chain mode - now working on implementing source chain mode to work (for SIF0).
</commit_message>
<xml_diff>
--- a/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
+++ b/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
@@ -1201,8 +1201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A288" workbookViewId="0">
-      <selection activeCell="G319" sqref="G319"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="H157" sqref="H157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4730,7 +4730,7 @@
         <v>194</v>
       </c>
       <c r="D158">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E158">
         <v>1</v>
@@ -4744,7 +4744,7 @@
       </c>
       <c r="J158" t="str">
         <f t="shared" si="34"/>
-        <v>registerField(Fields::ILinkUnk, "ILinkUnk", 10, 1, 0);</v>
+        <v>registerField(Fields::ILinkUnk, "ILinkUnk", 11, 1, 0);</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
@@ -7017,7 +7017,7 @@
         <v>0</v>
       </c>
       <c r="I252" t="str">
-        <f>"static constexpr u8 "&amp;C252&amp;" = "&amp;B252&amp;";"</f>
+        <f t="shared" ref="I252:I261" si="51">"static constexpr u8 "&amp;C252&amp;" = "&amp;B252&amp;";"</f>
         <v>static constexpr u8 TCM6 = 14;</v>
       </c>
       <c r="J252" t="str">
@@ -7042,7 +7042,7 @@
         <v>0</v>
       </c>
       <c r="I253" t="str">
-        <f>"static constexpr u8 "&amp;C253&amp;" = "&amp;B253&amp;";"</f>
+        <f t="shared" si="51"/>
         <v>static constexpr u8 MasterEnable = 15;</v>
       </c>
       <c r="J253" t="str">
@@ -7067,7 +7067,7 @@
         <v>0</v>
       </c>
       <c r="I254" t="str">
-        <f>"static constexpr u8 "&amp;C254&amp;" = "&amp;B254&amp;";"</f>
+        <f t="shared" si="51"/>
         <v>static constexpr u8 TCI0 = 16;</v>
       </c>
       <c r="J254" t="str">
@@ -7092,7 +7092,7 @@
         <v>0</v>
       </c>
       <c r="I255" t="str">
-        <f>"static constexpr u8 "&amp;C255&amp;" = "&amp;B255&amp;";"</f>
+        <f t="shared" si="51"/>
         <v>static constexpr u8 TCI1 = 17;</v>
       </c>
       <c r="J255" t="str">
@@ -7117,7 +7117,7 @@
         <v>0</v>
       </c>
       <c r="I256" t="str">
-        <f>"static constexpr u8 "&amp;C256&amp;" = "&amp;B256&amp;";"</f>
+        <f t="shared" si="51"/>
         <v>static constexpr u8 TCI2 = 18;</v>
       </c>
       <c r="J256" t="str">
@@ -7142,7 +7142,7 @@
         <v>0</v>
       </c>
       <c r="I257" t="str">
-        <f>"static constexpr u8 "&amp;C257&amp;" = "&amp;B257&amp;";"</f>
+        <f t="shared" si="51"/>
         <v>static constexpr u8 TCI3 = 19;</v>
       </c>
       <c r="J257" t="str">
@@ -7167,7 +7167,7 @@
         <v>0</v>
       </c>
       <c r="I258" t="str">
-        <f>"static constexpr u8 "&amp;C258&amp;" = "&amp;B258&amp;";"</f>
+        <f t="shared" si="51"/>
         <v>static constexpr u8 TCI4 = 20;</v>
       </c>
       <c r="J258" t="str">
@@ -7192,7 +7192,7 @@
         <v>0</v>
       </c>
       <c r="I259" t="str">
-        <f>"static constexpr u8 "&amp;C259&amp;" = "&amp;B259&amp;";"</f>
+        <f t="shared" si="51"/>
         <v>static constexpr u8 TCI5 = 21;</v>
       </c>
       <c r="J259" t="str">
@@ -7217,7 +7217,7 @@
         <v>0</v>
       </c>
       <c r="I260" t="str">
-        <f>"static constexpr u8 "&amp;C260&amp;" = "&amp;B260&amp;";"</f>
+        <f t="shared" si="51"/>
         <v>static constexpr u8 TCI6 = 22;</v>
       </c>
       <c r="J260" t="str">
@@ -7242,7 +7242,7 @@
         <v>0</v>
       </c>
       <c r="I261" t="str">
-        <f>"static constexpr u8 "&amp;C261&amp;" = "&amp;B261&amp;";"</f>
+        <f t="shared" si="51"/>
         <v>static constexpr u8 MasterInterrupt = 23;</v>
       </c>
       <c r="J261" t="str">
@@ -7274,11 +7274,11 @@
         <v>class IOPTimersTimerRegister_MODE_t;</v>
       </c>
       <c r="I263" t="str">
-        <f t="shared" ref="I263" si="51">"static constexpr u8 "&amp;C263&amp;" = "&amp;B263&amp;";"</f>
+        <f t="shared" ref="I263" si="52">"static constexpr u8 "&amp;C263&amp;" = "&amp;B263&amp;";"</f>
         <v>static constexpr u8 SyncEnable = 0;</v>
       </c>
       <c r="J263" t="str">
-        <f t="shared" ref="J263" si="52">"registerField(Fields::"&amp;C263&amp;", """&amp;C263&amp;""", "&amp;D263&amp;", "&amp;E263&amp;", "&amp;F263&amp;");"</f>
+        <f t="shared" ref="J263" si="53">"registerField(Fields::"&amp;C263&amp;", """&amp;C263&amp;""", "&amp;D263&amp;", "&amp;E263&amp;", "&amp;F263&amp;");"</f>
         <v>registerField(Fields::SyncEnable, "SyncEnable", 0, 1, 0);</v>
       </c>
     </row>
@@ -7299,11 +7299,11 @@
         <v>0</v>
       </c>
       <c r="I264" t="str">
-        <f t="shared" ref="I264:I275" si="53">"static constexpr u8 "&amp;C264&amp;" = "&amp;B264&amp;";"</f>
+        <f t="shared" ref="I264:I275" si="54">"static constexpr u8 "&amp;C264&amp;" = "&amp;B264&amp;";"</f>
         <v>static constexpr u8 SyncMode = 1;</v>
       </c>
       <c r="J264" t="str">
-        <f t="shared" ref="J264:J275" si="54">"registerField(Fields::"&amp;C264&amp;", """&amp;C264&amp;""", "&amp;D264&amp;", "&amp;E264&amp;", "&amp;F264&amp;");"</f>
+        <f t="shared" ref="J264:J275" si="55">"registerField(Fields::"&amp;C264&amp;", """&amp;C264&amp;""", "&amp;D264&amp;", "&amp;E264&amp;", "&amp;F264&amp;");"</f>
         <v>registerField(Fields::SyncMode, "SyncMode", 1, 2, 0);</v>
       </c>
     </row>
@@ -7324,11 +7324,11 @@
         <v>0</v>
       </c>
       <c r="I265" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>static constexpr u8 ResetMode = 2;</v>
       </c>
       <c r="J265" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>registerField(Fields::ResetMode, "ResetMode", 3, 1, 0);</v>
       </c>
     </row>
@@ -7349,11 +7349,11 @@
         <v>0</v>
       </c>
       <c r="I266" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>static constexpr u8 IrqOnTarget = 3;</v>
       </c>
       <c r="J266" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>registerField(Fields::IrqOnTarget, "IrqOnTarget", 4, 1, 0);</v>
       </c>
     </row>
@@ -7374,11 +7374,11 @@
         <v>0</v>
       </c>
       <c r="I267" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>static constexpr u8 IrqOnOF = 4;</v>
       </c>
       <c r="J267" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>registerField(Fields::IrqOnOF, "IrqOnOF", 5, 1, 0);</v>
       </c>
     </row>
@@ -7399,11 +7399,11 @@
         <v>0</v>
       </c>
       <c r="I268" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>static constexpr u8 IrqRepeat = 5;</v>
       </c>
       <c r="J268" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>registerField(Fields::IrqRepeat, "IrqRepeat", 6, 1, 0);</v>
       </c>
     </row>
@@ -7424,11 +7424,11 @@
         <v>0</v>
       </c>
       <c r="I269" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>static constexpr u8 IrqToggle = 6;</v>
       </c>
       <c r="J269" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>registerField(Fields::IrqToggle, "IrqToggle", 7, 1, 0);</v>
       </c>
     </row>
@@ -7449,11 +7449,11 @@
         <v>0</v>
       </c>
       <c r="I270" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>static constexpr u8 ClockSrc = 7;</v>
       </c>
       <c r="J270" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>registerField(Fields::ClockSrc, "ClockSrc", 8, 1, 0);</v>
       </c>
     </row>
@@ -7474,11 +7474,11 @@
         <v>0</v>
       </c>
       <c r="I271" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>static constexpr u8 Prescale0 = 8;</v>
       </c>
       <c r="J271" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>registerField(Fields::Prescale0, "Prescale0", 9, 1, 0);</v>
       </c>
     </row>
@@ -7499,11 +7499,11 @@
         <v>0</v>
       </c>
       <c r="I272" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>static constexpr u8 IrqRequest = 9;</v>
       </c>
       <c r="J272" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>registerField(Fields::IrqRequest, "IrqRequest", 10, 1, 0);</v>
       </c>
     </row>
@@ -7524,11 +7524,11 @@
         <v>0</v>
       </c>
       <c r="I273" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>static constexpr u8 ReachTarget = 10;</v>
       </c>
       <c r="J273" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>registerField(Fields::ReachTarget, "ReachTarget", 11, 1, 0);</v>
       </c>
     </row>
@@ -7549,11 +7549,11 @@
         <v>0</v>
       </c>
       <c r="I274" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>static constexpr u8 ReachOF = 11;</v>
       </c>
       <c r="J274" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>registerField(Fields::ReachOF, "ReachOF", 12, 1, 0);</v>
       </c>
     </row>
@@ -7574,11 +7574,11 @@
         <v>0</v>
       </c>
       <c r="I275" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>static constexpr u8 Prescale1 = 12;</v>
       </c>
       <c r="J275" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>registerField(Fields::Prescale1, "Prescale1", 13, 2, 0);</v>
       </c>
     </row>
@@ -7606,11 +7606,11 @@
         <v>class IOPDmacRegister_PCR1_t;</v>
       </c>
       <c r="I277" t="str">
-        <f t="shared" ref="I277:I290" si="55">"static constexpr u8 "&amp;C277&amp;" = "&amp;B277&amp;";"</f>
+        <f t="shared" ref="I277:I290" si="56">"static constexpr u8 "&amp;C277&amp;" = "&amp;B277&amp;";"</f>
         <v>static constexpr u8 Priority7 = 0;</v>
       </c>
       <c r="J277" t="str">
-        <f t="shared" ref="J277:J290" si="56">"registerField(Fields::"&amp;C277&amp;", """&amp;C277&amp;""", "&amp;D277&amp;", "&amp;E277&amp;", "&amp;F277&amp;");"</f>
+        <f t="shared" ref="J277:J290" si="57">"registerField(Fields::"&amp;C277&amp;", """&amp;C277&amp;""", "&amp;D277&amp;", "&amp;E277&amp;", "&amp;F277&amp;");"</f>
         <v>registerField(Fields::Priority7, "Priority7", 0, 3, 0);</v>
       </c>
     </row>
@@ -7631,11 +7631,11 @@
         <v>0</v>
       </c>
       <c r="I278" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>static constexpr u8 Enable7 = 1;</v>
       </c>
       <c r="J278" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>registerField(Fields::Enable7, "Enable7", 3, 1, 0);</v>
       </c>
     </row>
@@ -7656,11 +7656,11 @@
         <v>0</v>
       </c>
       <c r="I279" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>static constexpr u8 Priority8 = 2;</v>
       </c>
       <c r="J279" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>registerField(Fields::Priority8, "Priority8", 4, 3, 0);</v>
       </c>
     </row>
@@ -7681,11 +7681,11 @@
         <v>0</v>
       </c>
       <c r="I280" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>static constexpr u8 Enable8 = 3;</v>
       </c>
       <c r="J280" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>registerField(Fields::Enable8, "Enable8", 7, 1, 0);</v>
       </c>
     </row>
@@ -7706,11 +7706,11 @@
         <v>0</v>
       </c>
       <c r="I281" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>static constexpr u8 Priority9 = 4;</v>
       </c>
       <c r="J281" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>registerField(Fields::Priority9, "Priority9", 8, 3, 0);</v>
       </c>
     </row>
@@ -7731,11 +7731,11 @@
         <v>0</v>
       </c>
       <c r="I282" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>static constexpr u8 Enable9 = 5;</v>
       </c>
       <c r="J282" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>registerField(Fields::Enable9, "Enable9", 11, 1, 0);</v>
       </c>
     </row>
@@ -7756,11 +7756,11 @@
         <v>0</v>
       </c>
       <c r="I283" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>static constexpr u8 Priority10 = 6;</v>
       </c>
       <c r="J283" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>registerField(Fields::Priority10, "Priority10", 12, 3, 0);</v>
       </c>
     </row>
@@ -7781,11 +7781,11 @@
         <v>0</v>
       </c>
       <c r="I284" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>static constexpr u8 Enable10 = 7;</v>
       </c>
       <c r="J284" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>registerField(Fields::Enable10, "Enable10", 15, 1, 0);</v>
       </c>
     </row>
@@ -7806,11 +7806,11 @@
         <v>0</v>
       </c>
       <c r="I285" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>static constexpr u8 Priority11 = 8;</v>
       </c>
       <c r="J285" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>registerField(Fields::Priority11, "Priority11", 16, 3, 0);</v>
       </c>
     </row>
@@ -7831,11 +7831,11 @@
         <v>0</v>
       </c>
       <c r="I286" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>static constexpr u8 Enable11 = 9;</v>
       </c>
       <c r="J286" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>registerField(Fields::Enable11, "Enable11", 19, 1, 0);</v>
       </c>
     </row>
@@ -7856,11 +7856,11 @@
         <v>0</v>
       </c>
       <c r="I287" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>static constexpr u8 Priority12 = 10;</v>
       </c>
       <c r="J287" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>registerField(Fields::Priority12, "Priority12", 20, 3, 0);</v>
       </c>
     </row>
@@ -7881,11 +7881,11 @@
         <v>0</v>
       </c>
       <c r="I288" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>static constexpr u8 Enable12 = 11;</v>
       </c>
       <c r="J288" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>registerField(Fields::Enable12, "Enable12", 23, 1, 0);</v>
       </c>
     </row>
@@ -7906,11 +7906,11 @@
         <v>0</v>
       </c>
       <c r="I289" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>static constexpr u8 Priority13 = 12;</v>
       </c>
       <c r="J289" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>registerField(Fields::Priority13, "Priority13", 24, 3, 0);</v>
       </c>
     </row>
@@ -7931,11 +7931,11 @@
         <v>0</v>
       </c>
       <c r="I290" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>static constexpr u8 Enable13 = 13;</v>
       </c>
       <c r="J290" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>registerField(Fields::Enable13, "Enable13", 27, 1, 0);</v>
       </c>
     </row>
@@ -7992,7 +7992,7 @@
         <v>static constexpr u8 IQE1 = 1;</v>
       </c>
       <c r="J293" t="str">
-        <f t="shared" ref="J293:J319" si="57">"registerField(Fields::"&amp;C293&amp;", """&amp;C293&amp;""", "&amp;D293&amp;", "&amp;E293&amp;", "&amp;F293&amp;");"</f>
+        <f t="shared" ref="J293:J319" si="58">"registerField(Fields::"&amp;C293&amp;", """&amp;C293&amp;""", "&amp;D293&amp;", "&amp;E293&amp;", "&amp;F293&amp;");"</f>
         <v>registerField(Fields::IQE1, "IQE1", 1, 1, 0);</v>
       </c>
     </row>
@@ -8017,7 +8017,7 @@
         <v>static constexpr u8 IQE2 = 2;</v>
       </c>
       <c r="J294" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>registerField(Fields::IQE2, "IQE2", 2, 1, 0);</v>
       </c>
     </row>
@@ -8042,7 +8042,7 @@
         <v>static constexpr u8 IQE3 = 3;</v>
       </c>
       <c r="J295" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>registerField(Fields::IQE3, "IQE3", 3, 1, 0);</v>
       </c>
     </row>
@@ -8063,11 +8063,11 @@
         <v>0</v>
       </c>
       <c r="I296" t="str">
-        <f t="shared" ref="I296:I312" si="58">"static constexpr u8 "&amp;C296&amp;" = "&amp;B296&amp;";"</f>
+        <f t="shared" ref="I296:I312" si="59">"static constexpr u8 "&amp;C296&amp;" = "&amp;B296&amp;";"</f>
         <v>static constexpr u8 IQE4 = 4;</v>
       </c>
       <c r="J296" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>registerField(Fields::IQE4, "IQE4", 4, 1, 0);</v>
       </c>
     </row>
@@ -8088,11 +8088,11 @@
         <v>0</v>
       </c>
       <c r="I297" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 IQE5 = 5;</v>
+      </c>
+      <c r="J297" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 IQE5 = 5;</v>
-      </c>
-      <c r="J297" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::IQE5, "IQE5", 5, 1, 0);</v>
       </c>
     </row>
@@ -8113,11 +8113,11 @@
         <v>0</v>
       </c>
       <c r="I298" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 IQE6 = 6;</v>
+      </c>
+      <c r="J298" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 IQE6 = 6;</v>
-      </c>
-      <c r="J298" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::IQE6, "IQE6", 6, 1, 0);</v>
       </c>
     </row>
@@ -8138,11 +8138,11 @@
         <v>0</v>
       </c>
       <c r="I299" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 IQE7 = 7;</v>
+      </c>
+      <c r="J299" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 IQE7 = 7;</v>
-      </c>
-      <c r="J299" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::IQE7, "IQE7", 7, 1, 0);</v>
       </c>
     </row>
@@ -8163,11 +8163,11 @@
         <v>0</v>
       </c>
       <c r="I300" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 IQE8 = 8;</v>
+      </c>
+      <c r="J300" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 IQE8 = 8;</v>
-      </c>
-      <c r="J300" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::IQE8, "IQE8", 8, 1, 0);</v>
       </c>
     </row>
@@ -8188,11 +8188,11 @@
         <v>0</v>
       </c>
       <c r="I301" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 IQE9 = 9;</v>
+      </c>
+      <c r="J301" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 IQE9 = 9;</v>
-      </c>
-      <c r="J301" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::IQE9, "IQE9", 9, 1, 0);</v>
       </c>
     </row>
@@ -8213,11 +8213,11 @@
         <v>0</v>
       </c>
       <c r="I302" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 IQE10 = 10;</v>
+      </c>
+      <c r="J302" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 IQE10 = 10;</v>
-      </c>
-      <c r="J302" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::IQE10, "IQE10", 10, 1, 0);</v>
       </c>
     </row>
@@ -8238,11 +8238,11 @@
         <v>0</v>
       </c>
       <c r="I303" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 IQE11 = 11;</v>
+      </c>
+      <c r="J303" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 IQE11 = 11;</v>
-      </c>
-      <c r="J303" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::IQE11, "IQE11", 11, 1, 0);</v>
       </c>
     </row>
@@ -8263,11 +8263,11 @@
         <v>0</v>
       </c>
       <c r="I304" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 IQE12 = 12;</v>
+      </c>
+      <c r="J304" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 IQE12 = 12;</v>
-      </c>
-      <c r="J304" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::IQE12, "IQE12", 12, 1, 0);</v>
       </c>
     </row>
@@ -8288,11 +8288,11 @@
         <v>0</v>
       </c>
       <c r="I305" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 IQE13 = 13;</v>
+      </c>
+      <c r="J305" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 IQE13 = 13;</v>
-      </c>
-      <c r="J305" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::IQE13, "IQE13", 13, 1, 0);</v>
       </c>
     </row>
@@ -8313,11 +8313,11 @@
         <v>0</v>
       </c>
       <c r="I306" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 TCM7 = 14;</v>
+      </c>
+      <c r="J306" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 TCM7 = 14;</v>
-      </c>
-      <c r="J306" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::TCM7, "TCM7", 16, 1, 0);</v>
       </c>
     </row>
@@ -8338,11 +8338,11 @@
         <v>0</v>
       </c>
       <c r="I307" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 TCM8 = 15;</v>
+      </c>
+      <c r="J307" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 TCM8 = 15;</v>
-      </c>
-      <c r="J307" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::TCM8, "TCM8", 17, 1, 0);</v>
       </c>
     </row>
@@ -8363,11 +8363,11 @@
         <v>0</v>
       </c>
       <c r="I308" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 TCM9 = 16;</v>
+      </c>
+      <c r="J308" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 TCM9 = 16;</v>
-      </c>
-      <c r="J308" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::TCM9, "TCM9", 18, 1, 0);</v>
       </c>
     </row>
@@ -8388,11 +8388,11 @@
         <v>0</v>
       </c>
       <c r="I309" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 TCM10 = 17;</v>
+      </c>
+      <c r="J309" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 TCM10 = 17;</v>
-      </c>
-      <c r="J309" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::TCM10, "TCM10", 19, 1, 0);</v>
       </c>
     </row>
@@ -8413,11 +8413,11 @@
         <v>0</v>
       </c>
       <c r="I310" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 TCM11 = 18;</v>
+      </c>
+      <c r="J310" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 TCM11 = 18;</v>
-      </c>
-      <c r="J310" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::TCM11, "TCM11", 20, 1, 0);</v>
       </c>
     </row>
@@ -8438,11 +8438,11 @@
         <v>0</v>
       </c>
       <c r="I311" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 TCM12 = 19;</v>
+      </c>
+      <c r="J311" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 TCM12 = 19;</v>
-      </c>
-      <c r="J311" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::TCM12, "TCM12", 21, 1, 0);</v>
       </c>
     </row>
@@ -8463,11 +8463,11 @@
         <v>0</v>
       </c>
       <c r="I312" t="str">
+        <f t="shared" si="59"/>
+        <v>static constexpr u8 TCM13 = 20;</v>
+      </c>
+      <c r="J312" t="str">
         <f t="shared" si="58"/>
-        <v>static constexpr u8 TCM13 = 20;</v>
-      </c>
-      <c r="J312" t="str">
-        <f t="shared" si="57"/>
         <v>registerField(Fields::TCM13, "TCM13", 22, 1, 0);</v>
       </c>
     </row>
@@ -8488,11 +8488,11 @@
         <v>0</v>
       </c>
       <c r="I313" t="str">
-        <f>"static constexpr u8 "&amp;C313&amp;" = "&amp;B313&amp;";"</f>
+        <f t="shared" ref="I313:I319" si="60">"static constexpr u8 "&amp;C313&amp;" = "&amp;B313&amp;";"</f>
         <v>static constexpr u8 TCI7 = 21;</v>
       </c>
       <c r="J313" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>registerField(Fields::TCI7, "TCI7", 24, 1, 0);</v>
       </c>
     </row>
@@ -8513,11 +8513,11 @@
         <v>0</v>
       </c>
       <c r="I314" t="str">
-        <f>"static constexpr u8 "&amp;C314&amp;" = "&amp;B314&amp;";"</f>
+        <f t="shared" si="60"/>
         <v>static constexpr u8 TCI8 = 22;</v>
       </c>
       <c r="J314" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>registerField(Fields::TCI8, "TCI8", 25, 1, 0);</v>
       </c>
     </row>
@@ -8538,11 +8538,11 @@
         <v>0</v>
       </c>
       <c r="I315" t="str">
-        <f>"static constexpr u8 "&amp;C315&amp;" = "&amp;B315&amp;";"</f>
+        <f t="shared" si="60"/>
         <v>static constexpr u8 TCI9 = 23;</v>
       </c>
       <c r="J315" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>registerField(Fields::TCI9, "TCI9", 26, 1, 0);</v>
       </c>
     </row>
@@ -8563,11 +8563,11 @@
         <v>0</v>
       </c>
       <c r="I316" t="str">
-        <f>"static constexpr u8 "&amp;C316&amp;" = "&amp;B316&amp;";"</f>
+        <f t="shared" si="60"/>
         <v>static constexpr u8 TCI10 = 24;</v>
       </c>
       <c r="J316" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>registerField(Fields::TCI10, "TCI10", 27, 1, 0);</v>
       </c>
     </row>
@@ -8588,11 +8588,11 @@
         <v>0</v>
       </c>
       <c r="I317" t="str">
-        <f>"static constexpr u8 "&amp;C317&amp;" = "&amp;B317&amp;";"</f>
+        <f t="shared" si="60"/>
         <v>static constexpr u8 TCI11 = 25;</v>
       </c>
       <c r="J317" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>registerField(Fields::TCI11, "TCI11", 28, 1, 0);</v>
       </c>
     </row>
@@ -8613,11 +8613,11 @@
         <v>0</v>
       </c>
       <c r="I318" t="str">
-        <f>"static constexpr u8 "&amp;C318&amp;" = "&amp;B318&amp;";"</f>
+        <f t="shared" si="60"/>
         <v>static constexpr u8 TCI12 = 26;</v>
       </c>
       <c r="J318" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>registerField(Fields::TCI12, "TCI12", 29, 1, 0);</v>
       </c>
     </row>
@@ -8638,11 +8638,11 @@
         <v>0</v>
       </c>
       <c r="I319" t="str">
-        <f>"static constexpr u8 "&amp;C319&amp;" = "&amp;B319&amp;";"</f>
+        <f t="shared" si="60"/>
         <v>static constexpr u8 TCI13 = 27;</v>
       </c>
       <c r="J319" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>registerField(Fields::TCI13, "TCI13", 30, 1, 0);</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Looking into the SPU2 debug data... All looks ok, data is being sent to the fifo, but logic hasn't been done yet (although it is all 0's... may need a look). IOP INTC mask bits set are now CDROM, DMA and SPU, so looks like I'm done with the IOP for now.
</commit_message>
<xml_diff>
--- a/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
+++ b/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\Dev\Projects\PCSX2_Rewrite\PCSX2_Core\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="350">
   <si>
     <t>Field Name</t>
   </si>
@@ -1055,16 +1055,25 @@
     <t>ATTR</t>
   </si>
   <si>
-    <t>IRQ</t>
-  </si>
-  <si>
-    <t>ReverbEn</t>
-  </si>
-  <si>
     <t>NoiseClock</t>
   </si>
   <si>
     <t>Mute</t>
+  </si>
+  <si>
+    <t>DMABits</t>
+  </si>
+  <si>
+    <t>DMAMode</t>
+  </si>
+  <si>
+    <t>IRQEnable</t>
+  </si>
+  <si>
+    <t>FxEnable</t>
+  </si>
+  <si>
+    <t>CoreEnable</t>
   </si>
 </sst>
 </file>
@@ -1382,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L380"/>
+  <dimension ref="A1:L382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A360" workbookViewId="0">
-      <selection activeCell="J376" sqref="J376:J380"/>
+    <sheetView tabSelected="1" topLeftCell="G360" workbookViewId="0">
+      <selection activeCell="J376" sqref="J376:J382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9960,24 +9969,24 @@
         <v>0</v>
       </c>
       <c r="D376" t="s">
-        <v>151</v>
+        <v>345</v>
       </c>
       <c r="E376">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F376">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G376">
         <v>0</v>
       </c>
       <c r="I376" t="str">
         <f t="shared" ref="I376" si="63">"static constexpr int "&amp;D376&amp;" = "&amp;C376&amp;";"</f>
-        <v>static constexpr int DMA = 0;</v>
+        <v>static constexpr int DMABits = 0;</v>
       </c>
       <c r="J376" t="str">
         <f t="shared" ref="J376" si="64">"registerField(Fields::"&amp;D376&amp;", """&amp;D376&amp;""", "&amp;E376&amp;", "&amp;F376&amp;", "&amp;G376&amp;");"</f>
-        <v>registerField(Fields::DMA, "DMA", 4, 2, 0);</v>
+        <v>registerField(Fields::DMABits, "DMABits", 1, 3, 0);</v>
       </c>
     </row>
     <row r="377" spans="2:10" x14ac:dyDescent="0.25">
@@ -9985,24 +9994,24 @@
         <v>1</v>
       </c>
       <c r="D377" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="E377">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F377">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G377">
         <v>0</v>
       </c>
       <c r="I377" t="str">
-        <f t="shared" ref="I377:I380" si="65">"static constexpr int "&amp;D377&amp;" = "&amp;C377&amp;";"</f>
-        <v>static constexpr int IRQ = 1;</v>
+        <f t="shared" ref="I377" si="65">"static constexpr int "&amp;D377&amp;" = "&amp;C377&amp;";"</f>
+        <v>static constexpr int DMAMode = 1;</v>
       </c>
       <c r="J377" t="str">
-        <f t="shared" ref="J377:J380" si="66">"registerField(Fields::"&amp;D377&amp;", """&amp;D377&amp;""", "&amp;E377&amp;", "&amp;F377&amp;", "&amp;G377&amp;");"</f>
-        <v>registerField(Fields::IRQ, "IRQ", 6, 1, 0);</v>
+        <f t="shared" ref="J377" si="66">"registerField(Fields::"&amp;D377&amp;", """&amp;D377&amp;""", "&amp;E377&amp;", "&amp;F377&amp;", "&amp;G377&amp;");"</f>
+        <v>registerField(Fields::DMAMode, "DMAMode", 4, 2, 0);</v>
       </c>
     </row>
     <row r="378" spans="2:10" x14ac:dyDescent="0.25">
@@ -10010,10 +10019,10 @@
         <v>2</v>
       </c>
       <c r="D378" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="E378">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F378">
         <v>1</v>
@@ -10022,12 +10031,12 @@
         <v>0</v>
       </c>
       <c r="I378" t="str">
-        <f t="shared" si="65"/>
-        <v>static constexpr int ReverbEn = 2;</v>
+        <f t="shared" ref="I378:I382" si="67">"static constexpr int "&amp;D378&amp;" = "&amp;C378&amp;";"</f>
+        <v>static constexpr int IRQEnable = 2;</v>
       </c>
       <c r="J378" t="str">
-        <f t="shared" si="66"/>
-        <v>registerField(Fields::ReverbEn, "ReverbEn", 7, 1, 0);</v>
+        <f t="shared" ref="J378:J382" si="68">"registerField(Fields::"&amp;D378&amp;", """&amp;D378&amp;""", "&amp;E378&amp;", "&amp;F378&amp;", "&amp;G378&amp;");"</f>
+        <v>registerField(Fields::IRQEnable, "IRQEnable", 6, 1, 0);</v>
       </c>
     </row>
     <row r="379" spans="2:10" x14ac:dyDescent="0.25">
@@ -10035,24 +10044,24 @@
         <v>3</v>
       </c>
       <c r="D379" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="E379">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F379">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G379">
         <v>0</v>
       </c>
       <c r="I379" t="str">
-        <f t="shared" si="65"/>
-        <v>static constexpr int NoiseClock = 3;</v>
+        <f t="shared" si="67"/>
+        <v>static constexpr int FxEnable = 3;</v>
       </c>
       <c r="J379" t="str">
-        <f t="shared" si="66"/>
-        <v>registerField(Fields::NoiseClock, "NoiseClock", 8, 6, 0);</v>
+        <f t="shared" si="68"/>
+        <v>registerField(Fields::FxEnable, "FxEnable", 7, 1, 0);</v>
       </c>
     </row>
     <row r="380" spans="2:10" x14ac:dyDescent="0.25">
@@ -10060,24 +10069,74 @@
         <v>4</v>
       </c>
       <c r="D380" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E380">
+        <v>8</v>
+      </c>
+      <c r="F380">
+        <v>6</v>
+      </c>
+      <c r="G380">
+        <v>0</v>
+      </c>
+      <c r="I380" t="str">
+        <f t="shared" si="67"/>
+        <v>static constexpr int NoiseClock = 4;</v>
+      </c>
+      <c r="J380" t="str">
+        <f t="shared" si="68"/>
+        <v>registerField(Fields::NoiseClock, "NoiseClock", 8, 6, 0);</v>
+      </c>
+    </row>
+    <row r="381" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C381">
+        <v>5</v>
+      </c>
+      <c r="D381" t="s">
+        <v>344</v>
+      </c>
+      <c r="E381">
         <v>14</v>
       </c>
-      <c r="F380">
-        <v>1</v>
-      </c>
-      <c r="G380">
-        <v>0</v>
-      </c>
-      <c r="I380" t="str">
-        <f t="shared" si="65"/>
-        <v>static constexpr int Mute = 4;</v>
-      </c>
-      <c r="J380" t="str">
-        <f t="shared" si="66"/>
+      <c r="F381">
+        <v>1</v>
+      </c>
+      <c r="G381">
+        <v>0</v>
+      </c>
+      <c r="I381" t="str">
+        <f t="shared" si="67"/>
+        <v>static constexpr int Mute = 5;</v>
+      </c>
+      <c r="J381" t="str">
+        <f t="shared" si="68"/>
         <v>registerField(Fields::Mute, "Mute", 14, 1, 0);</v>
+      </c>
+    </row>
+    <row r="382" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C382">
+        <v>6</v>
+      </c>
+      <c r="D382" t="s">
+        <v>349</v>
+      </c>
+      <c r="E382">
+        <v>15</v>
+      </c>
+      <c r="F382">
+        <v>1</v>
+      </c>
+      <c r="G382">
+        <v>0</v>
+      </c>
+      <c r="I382" t="str">
+        <f t="shared" si="67"/>
+        <v>static constexpr int CoreEnable = 6;</v>
+      </c>
+      <c r="J382" t="str">
+        <f t="shared" si="68"/>
+        <v>registerField(Fields::CoreEnable, "CoreEnable", 15, 1, 0);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A bit of work on the SPU2 core STATX register. Don't fully understand it for now, though.
</commit_message>
<xml_diff>
--- a/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
+++ b/PCSX2_Core/Docs/Bitfield Register Creation Helper.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.satti\Documents\Marco\PCSX2_rewrite\PCSX2_Core\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\Dev\Projects\PCSX2_Rewrite\PCSX2_Core\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9198"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="355">
   <si>
     <t>Field Name</t>
   </si>
@@ -1083,6 +1083,12 @@
   </si>
   <si>
     <t>IrqCore1</t>
+  </si>
+  <si>
+    <t>STATX</t>
+  </si>
+  <si>
+    <t>NeedData</t>
   </si>
 </sst>
 </file>
@@ -1400,25 +1406,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L385"/>
+  <dimension ref="A1:L387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A360" workbookViewId="0">
-      <selection activeCell="J384" sqref="J384:J385"/>
+    <sheetView tabSelected="1" topLeftCell="A362" workbookViewId="0">
+      <selection activeCell="H375" sqref="H375"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.15625" customWidth="1"/>
-    <col min="3" max="3" width="14.83984375" customWidth="1"/>
-    <col min="4" max="4" width="15.26171875" customWidth="1"/>
-    <col min="5" max="5" width="15.15625" customWidth="1"/>
-    <col min="6" max="6" width="13.15625" customWidth="1"/>
-    <col min="7" max="7" width="12.41796875" customWidth="1"/>
-    <col min="9" max="9" width="35.15625" customWidth="1"/>
-    <col min="10" max="10" width="43.15625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="35.140625" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>8</v>
       </c>
@@ -1444,7 +1450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>65</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>registerField(Fields::R, "R", 0, 32, 0);</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1500,7 +1506,7 @@
         <v>registerField(Fields::C, "C", 0, 32, 0);</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -1528,7 +1534,7 @@
         <v>registerField(Fields::CL, "CL", 0, 8, 0);</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>1</v>
       </c>
@@ -1553,7 +1559,7 @@
         <v>registerField(Fields::WL, "WL", 8, 8, 0);</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -1581,7 +1587,7 @@
         <v>registerField(Fields::m0, "m0", 0, 2, 0);</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>1</v>
       </c>
@@ -1606,7 +1612,7 @@
         <v>registerField(Fields::m1, "m1", 2, 2, 0);</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>2</v>
       </c>
@@ -1631,7 +1637,7 @@
         <v>registerField(Fields::m2, "m2", 4, 2, 0);</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>3</v>
       </c>
@@ -1656,7 +1662,7 @@
         <v>registerField(Fields::m3, "m3", 6, 2, 0);</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>4</v>
       </c>
@@ -1681,7 +1687,7 @@
         <v>registerField(Fields::m4, "m4", 8, 2, 0);</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>5</v>
       </c>
@@ -1706,7 +1712,7 @@
         <v>registerField(Fields::m5, "m5", 10, 2, 0);</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>6</v>
       </c>
@@ -1731,7 +1737,7 @@
         <v>registerField(Fields::m6, "m6", 12, 2, 0);</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>7</v>
       </c>
@@ -1756,7 +1762,7 @@
         <v>registerField(Fields::m7, "m7", 14, 2, 0);</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>8</v>
       </c>
@@ -1781,7 +1787,7 @@
         <v>registerField(Fields::m8, "m8", 16, 2, 0);</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>9</v>
       </c>
@@ -1806,7 +1812,7 @@
         <v>registerField(Fields::m9, "m9", 18, 2, 0);</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>10</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>registerField(Fields::m10, "m10", 20, 2, 0);</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>11</v>
       </c>
@@ -1856,7 +1862,7 @@
         <v>registerField(Fields::m11, "m11", 22, 2, 0);</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>12</v>
       </c>
@@ -1881,7 +1887,7 @@
         <v>registerField(Fields::m12, "m12", 24, 2, 0);</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>13</v>
       </c>
@@ -1906,7 +1912,7 @@
         <v>registerField(Fields::m13, "m13", 26, 2, 0);</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>14</v>
       </c>
@@ -1931,7 +1937,7 @@
         <v>registerField(Fields::m14, "m14", 28, 2, 0);</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>15</v>
       </c>
@@ -1956,7 +1962,7 @@
         <v>registerField(Fields::m15, "m15", 30, 2, 0);</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>29</v>
       </c>
@@ -1984,7 +1990,7 @@
         <v>registerField(Fields::MOD, "MOD", 0, 2, 0);</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>31</v>
       </c>
@@ -2012,7 +2018,7 @@
         <v>registerField(Fields::ITOP, "ITOP", 0, 10, 0);</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>32</v>
       </c>
@@ -2040,7 +2046,7 @@
         <v>registerField(Fields::ITOPS, "ITOPS", 0, 10, 0);</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>33</v>
       </c>
@@ -2068,7 +2074,7 @@
         <v>registerField(Fields::BASE, "BASE", 0, 10, 0);</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>34</v>
       </c>
@@ -2096,7 +2102,7 @@
         <v>registerField(Fields::OFFSET, "OFFSET", 0, 10, 0);</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>36</v>
       </c>
@@ -2124,7 +2130,7 @@
         <v>registerField(Fields::TOP, "TOP", 0, 10, 0);</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -2152,7 +2158,7 @@
         <v>registerField(Fields::TOPS, "TOPS", 0, 10, 0);</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -2180,7 +2186,7 @@
         <v>registerField(Fields::MARK, "MARK", 0, 16, 0);</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>39</v>
       </c>
@@ -2208,7 +2214,7 @@
         <v>registerField(Fields::NUM, "NUM", 0, 8, 0);</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>40</v>
       </c>
@@ -2236,7 +2242,7 @@
         <v>registerField(Fields::IMMEDIATE, "IMMEDIATE", 0, 16, 0);</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>1</v>
       </c>
@@ -2261,7 +2267,7 @@
         <v>registerField(Fields::NUM, "NUM", 16, 8, 0);</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>2</v>
       </c>
@@ -2286,7 +2292,7 @@
         <v>registerField(Fields::CMD, "CMD", 24, 8, 0);</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>43</v>
       </c>
@@ -2314,7 +2320,7 @@
         <v>registerField(Fields::VPS, "VPS", 0, 2, 0);</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>1</v>
       </c>
@@ -2339,7 +2345,7 @@
         <v>registerField(Fields::VEW, "VEW", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>2</v>
       </c>
@@ -2364,7 +2370,7 @@
         <v>registerField(Fields::VGW, "VGW", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>3</v>
       </c>
@@ -2389,7 +2395,7 @@
         <v>registerField(Fields::MRK, "MRK", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>4</v>
       </c>
@@ -2414,7 +2420,7 @@
         <v>registerField(Fields::DBF, "DBF", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>5</v>
       </c>
@@ -2439,7 +2445,7 @@
         <v>registerField(Fields::VSS, "VSS", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>6</v>
       </c>
@@ -2464,7 +2470,7 @@
         <v>registerField(Fields::VFS, "VFS", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C55">
         <v>7</v>
       </c>
@@ -2489,7 +2495,7 @@
         <v>registerField(Fields::VIS, "VIS", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>8</v>
       </c>
@@ -2514,7 +2520,7 @@
         <v>registerField(Fields::INT, "INT", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>9</v>
       </c>
@@ -2539,7 +2545,7 @@
         <v>registerField(Fields::ER0, "ER0", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>10</v>
       </c>
@@ -2564,7 +2570,7 @@
         <v>registerField(Fields::ER1, "ER1", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>11</v>
       </c>
@@ -2589,7 +2595,7 @@
         <v>registerField(Fields::FDR, "FDR", 23, 1, 0);</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>12</v>
       </c>
@@ -2614,7 +2620,7 @@
         <v>registerField(Fields::FQC, "FQC", 24, 4, 0);</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>54</v>
       </c>
@@ -2642,7 +2648,7 @@
         <v>registerField(Fields::RST, "RST", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C63">
         <v>1</v>
       </c>
@@ -2667,7 +2673,7 @@
         <v>registerField(Fields::FBK, "FBK", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C64">
         <v>2</v>
       </c>
@@ -2692,7 +2698,7 @@
         <v>registerField(Fields::STP, "STP", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C65">
         <v>3</v>
       </c>
@@ -2717,7 +2723,7 @@
         <v>registerField(Fields::STC, "STC", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>59</v>
       </c>
@@ -2745,7 +2751,7 @@
         <v>registerField(Fields::MII, "MII", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C68">
         <v>1</v>
       </c>
@@ -2770,7 +2776,7 @@
         <v>registerField(Fields::ME0, "ME0", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>2</v>
       </c>
@@ -2795,7 +2801,7 @@
         <v>registerField(Fields::ME1, "ME1", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>67</v>
       </c>
@@ -2823,7 +2829,7 @@
         <v>registerField(Fields::Zw, "Zw", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>1</v>
       </c>
@@ -2848,7 +2854,7 @@
         <v>registerField(Fields::Zz, "Zz", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C73">
         <v>2</v>
       </c>
@@ -2873,7 +2879,7 @@
         <v>registerField(Fields::Zy, "Zy", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C74">
         <v>3</v>
       </c>
@@ -2898,7 +2904,7 @@
         <v>registerField(Fields::Zx, "Zx", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C75">
         <v>4</v>
       </c>
@@ -2923,7 +2929,7 @@
         <v>registerField(Fields::Sw, "Sw", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C76">
         <v>5</v>
       </c>
@@ -2948,7 +2954,7 @@
         <v>registerField(Fields::Sz, "Sz", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C77">
         <v>6</v>
       </c>
@@ -2973,7 +2979,7 @@
         <v>registerField(Fields::Sy, "Sy", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C78">
         <v>7</v>
       </c>
@@ -2998,7 +3004,7 @@
         <v>registerField(Fields::Sx, "Sx", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C79">
         <v>8</v>
       </c>
@@ -3023,7 +3029,7 @@
         <v>registerField(Fields::Uw, "Uw", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C80">
         <v>9</v>
       </c>
@@ -3048,7 +3054,7 @@
         <v>registerField(Fields::Uz, "Uz", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C81">
         <v>10</v>
       </c>
@@ -3073,7 +3079,7 @@
         <v>registerField(Fields::Uy, "Uy", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C82">
         <v>11</v>
       </c>
@@ -3098,7 +3104,7 @@
         <v>registerField(Fields::Ux, "Ux", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C83">
         <v>12</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>registerField(Fields::Ow, "Ow", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C84">
         <v>13</v>
       </c>
@@ -3148,7 +3154,7 @@
         <v>registerField(Fields::Oz, "Oz", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C85">
         <v>14</v>
       </c>
@@ -3173,7 +3179,7 @@
         <v>registerField(Fields::Oy, "Oy", 14, 1, 0);</v>
       </c>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C86">
         <v>15</v>
       </c>
@@ -3198,7 +3204,7 @@
         <v>registerField(Fields::Ox, "Ox", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>84</v>
       </c>
@@ -3226,7 +3232,7 @@
         <v>registerField(Fields::Z, "Z", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C89">
         <v>1</v>
       </c>
@@ -3251,7 +3257,7 @@
         <v>registerField(Fields::S, "S", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C90">
         <v>2</v>
       </c>
@@ -3276,7 +3282,7 @@
         <v>registerField(Fields::U, "U", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C91">
         <v>3</v>
       </c>
@@ -3301,7 +3307,7 @@
         <v>registerField(Fields::O, "O", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C92">
         <v>4</v>
       </c>
@@ -3326,7 +3332,7 @@
         <v>registerField(Fields::I, "I", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C93">
         <v>5</v>
       </c>
@@ -3351,7 +3357,7 @@
         <v>registerField(Fields::D, "D", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C94">
         <v>6</v>
       </c>
@@ -3376,7 +3382,7 @@
         <v>registerField(Fields::ZS, "ZS", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C95">
         <v>7</v>
       </c>
@@ -3401,7 +3407,7 @@
         <v>registerField(Fields::SS, "SS", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C96">
         <v>8</v>
       </c>
@@ -3426,7 +3432,7 @@
         <v>registerField(Fields::US, "US", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C97">
         <v>9</v>
       </c>
@@ -3451,7 +3457,7 @@
         <v>registerField(Fields::OS, "OS", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C98">
         <v>10</v>
       </c>
@@ -3476,7 +3482,7 @@
         <v>registerField(Fields::IS, "IS", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C99">
         <v>11</v>
       </c>
@@ -3501,7 +3507,7 @@
         <v>registerField(Fields::DS, "DS", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>97</v>
       </c>
@@ -3529,7 +3535,7 @@
         <v>registerField(Fields::NegX_0, "NegX_0", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C102">
         <v>1</v>
       </c>
@@ -3554,7 +3560,7 @@
         <v>registerField(Fields::PosX_0, "PosX_0", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C103">
         <v>2</v>
       </c>
@@ -3579,7 +3585,7 @@
         <v>registerField(Fields::NegY_0, "NegY_0", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C104">
         <v>3</v>
       </c>
@@ -3604,7 +3610,7 @@
         <v>registerField(Fields::PosY_0, "PosY_0", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C105">
         <v>4</v>
       </c>
@@ -3629,7 +3635,7 @@
         <v>registerField(Fields::NegZ_0, "NegZ_0", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C106">
         <v>5</v>
       </c>
@@ -3654,7 +3660,7 @@
         <v>registerField(Fields::PosZ_0, "PosZ_0", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C107">
         <v>6</v>
       </c>
@@ -3679,7 +3685,7 @@
         <v>registerField(Fields::NegX_1, "NegX_1", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C108">
         <v>7</v>
       </c>
@@ -3704,7 +3710,7 @@
         <v>registerField(Fields::PosX_1, "PosX_1", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C109">
         <v>8</v>
       </c>
@@ -3729,7 +3735,7 @@
         <v>registerField(Fields::NegY_1, "NegY_1", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C110">
         <v>9</v>
       </c>
@@ -3754,7 +3760,7 @@
         <v>registerField(Fields::PosY_1, "PosY_1", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C111">
         <v>10</v>
       </c>
@@ -3779,7 +3785,7 @@
         <v>registerField(Fields::NegZ_1, "NegZ_1", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C112">
         <v>11</v>
       </c>
@@ -3804,7 +3810,7 @@
         <v>registerField(Fields::PosZ_1, "PosZ_1", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="113" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C113">
         <v>12</v>
       </c>
@@ -3829,7 +3835,7 @@
         <v>registerField(Fields::NegX_2, "NegX_2", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="114" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C114">
         <v>13</v>
       </c>
@@ -3854,7 +3860,7 @@
         <v>registerField(Fields::PosX_2, "PosX_2", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="115" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C115">
         <v>14</v>
       </c>
@@ -3879,7 +3885,7 @@
         <v>registerField(Fields::NegY_2, "NegY_2", 14, 1, 0);</v>
       </c>
     </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C116">
         <v>15</v>
       </c>
@@ -3904,7 +3910,7 @@
         <v>registerField(Fields::PosY_2, "PosY_2", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C117">
         <v>16</v>
       </c>
@@ -3929,7 +3935,7 @@
         <v>registerField(Fields::NegZ_2, "NegZ_2", 16, 1, 0);</v>
       </c>
     </row>
-    <row r="118" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C118">
         <v>17</v>
       </c>
@@ -3954,7 +3960,7 @@
         <v>registerField(Fields::PosZ_2, "PosZ_2", 17, 1, 0);</v>
       </c>
     </row>
-    <row r="119" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C119">
         <v>18</v>
       </c>
@@ -3979,7 +3985,7 @@
         <v>registerField(Fields::NegX_3, "NegX_3", 18, 1, 0);</v>
       </c>
     </row>
-    <row r="120" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C120">
         <v>19</v>
       </c>
@@ -4004,7 +4010,7 @@
         <v>registerField(Fields::PosX_3, "PosX_3", 19, 1, 0);</v>
       </c>
     </row>
-    <row r="121" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C121">
         <v>20</v>
       </c>
@@ -4029,7 +4035,7 @@
         <v>registerField(Fields::NegY_3, "NegY_3", 20, 1, 0);</v>
       </c>
     </row>
-    <row r="122" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C122">
         <v>21</v>
       </c>
@@ -4054,7 +4060,7 @@
         <v>registerField(Fields::PosY_3, "PosY_3", 21, 1, 0);</v>
       </c>
     </row>
-    <row r="123" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C123">
         <v>22</v>
       </c>
@@ -4079,7 +4085,7 @@
         <v>registerField(Fields::NegZ_3, "NegZ_3", 22, 1, 0);</v>
       </c>
     </row>
-    <row r="124" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C124">
         <v>23</v>
       </c>
@@ -4104,7 +4110,7 @@
         <v>registerField(Fields::PosZ_3, "PosZ_3", 23, 1, 0);</v>
       </c>
     </row>
-    <row r="126" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>122</v>
       </c>
@@ -4132,7 +4138,7 @@
         <v>registerField(Fields::CMSAR, "CMSAR", 0, 16, 0);</v>
       </c>
     </row>
-    <row r="128" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>54</v>
       </c>
@@ -4160,7 +4166,7 @@
         <v>registerField(Fields::FB0, "FB0", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="129" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C129">
         <v>1</v>
       </c>
@@ -4185,7 +4191,7 @@
         <v>registerField(Fields::RS0, "RS0", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="130" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C130">
         <v>2</v>
       </c>
@@ -4210,7 +4216,7 @@
         <v>registerField(Fields::DE0, "DE0", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="131" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C131">
         <v>3</v>
       </c>
@@ -4235,7 +4241,7 @@
         <v>registerField(Fields::TE0, "TE0", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="132" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C132">
         <v>4</v>
       </c>
@@ -4260,7 +4266,7 @@
         <v>registerField(Fields::FB1, "FB1", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="133" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C133">
         <v>5</v>
       </c>
@@ -4285,7 +4291,7 @@
         <v>registerField(Fields::RS1, "RS1", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="134" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C134">
         <v>6</v>
       </c>
@@ -4310,7 +4316,7 @@
         <v>registerField(Fields::DE1, "DE1", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="135" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C135">
         <v>7</v>
       </c>
@@ -4335,7 +4341,7 @@
         <v>registerField(Fields::TE1, "TE1", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="137" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>43</v>
       </c>
@@ -4363,7 +4369,7 @@
         <v>registerField(Fields::VBS0, "VBS0", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="138" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C138">
         <v>1</v>
       </c>
@@ -4388,7 +4394,7 @@
         <v>registerField(Fields::VDS0, "VDS0", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="139" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C139">
         <v>2</v>
       </c>
@@ -4413,7 +4419,7 @@
         <v>registerField(Fields::VTS0, "VTS0", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="140" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C140">
         <v>3</v>
       </c>
@@ -4438,7 +4444,7 @@
         <v>registerField(Fields::VFS0, "VFS0", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="141" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C141">
         <v>4</v>
       </c>
@@ -4463,7 +4469,7 @@
         <v>registerField(Fields::DIV0, "DIV0", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="142" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C142">
         <v>5</v>
       </c>
@@ -4488,7 +4494,7 @@
         <v>registerField(Fields::IBS0, "IBS0", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="143" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C143">
         <v>6</v>
       </c>
@@ -4513,7 +4519,7 @@
         <v>registerField(Fields::VBS1, "VBS1", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="144" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C144">
         <v>7</v>
       </c>
@@ -4538,7 +4544,7 @@
         <v>registerField(Fields::VDS1, "VDS1", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="145" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C145">
         <v>8</v>
       </c>
@@ -4563,7 +4569,7 @@
         <v>registerField(Fields::VTS1, "VTS1", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="146" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C146">
         <v>9</v>
       </c>
@@ -4588,7 +4594,7 @@
         <v>registerField(Fields::VFS1, "VFS1", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="147" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C147">
         <v>10</v>
       </c>
@@ -4613,7 +4619,7 @@
         <v>registerField(Fields::VGW1, "VGW1", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="148" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C148">
         <v>11</v>
       </c>
@@ -4638,7 +4644,7 @@
         <v>registerField(Fields::DIV1, "DIV1", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="149" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C149">
         <v>12</v>
       </c>
@@ -4663,7 +4669,7 @@
         <v>registerField(Fields::EFU1, "EFU1", 14, 1, 0);</v>
       </c>
     </row>
-    <row r="151" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>144</v>
       </c>
@@ -4691,7 +4697,7 @@
         <v>registerField(Fields::BS, "BS", 0, 16, 0);</v>
       </c>
     </row>
-    <row r="152" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C152">
         <v>1</v>
       </c>
@@ -4716,7 +4722,7 @@
         <v>registerField(Fields::BA, "BA", 16, 16, 0);</v>
       </c>
     </row>
-    <row r="154" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>147</v>
       </c>
@@ -4744,7 +4750,7 @@
         <v>registerField(Fields::TD, "TD", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="155" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C155">
         <v>1</v>
       </c>
@@ -4769,7 +4775,7 @@
         <v>registerField(Fields::MAS, "MAS", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="156" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C156">
         <v>2</v>
       </c>
@@ -4794,7 +4800,7 @@
         <v>registerField(Fields::CE, "CE", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="157" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C157">
         <v>3</v>
       </c>
@@ -4819,7 +4825,7 @@
         <v>registerField(Fields::SM, "SM", 9, 2, 0);</v>
       </c>
     </row>
-    <row r="158" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C158">
         <v>4</v>
       </c>
@@ -4844,7 +4850,7 @@
         <v>registerField(Fields::ILinkUnk, "ILinkUnk", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="159" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C159">
         <v>5</v>
       </c>
@@ -4869,7 +4875,7 @@
         <v>registerField(Fields::C_DWS, "C_DWS", 16, 3, 0);</v>
       </c>
     </row>
-    <row r="160" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C160">
         <v>6</v>
       </c>
@@ -4894,7 +4900,7 @@
         <v>registerField(Fields::C_CWS, "C_CWS", 20, 3, 0);</v>
       </c>
     </row>
-    <row r="161" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C161">
         <v>7</v>
       </c>
@@ -4919,7 +4925,7 @@
         <v>registerField(Fields::Start, "Start", 24, 1, 0);</v>
       </c>
     </row>
-    <row r="162" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C162">
         <v>8</v>
       </c>
@@ -4944,7 +4950,7 @@
         <v>registerField(Fields::Force, "Force", 28, 1, 0);</v>
       </c>
     </row>
-    <row r="163" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C163">
         <v>9</v>
       </c>
@@ -4969,7 +4975,7 @@
         <v>registerField(Fields::ForceSlice, "ForceSlice", 29, 1, 0);</v>
       </c>
     </row>
-    <row r="164" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C164">
         <v>10</v>
       </c>
@@ -4994,7 +5000,7 @@
         <v>registerField(Fields::BusSnooping, "BusSnooping", 30, 1, 0);</v>
       </c>
     </row>
-    <row r="165" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C165">
         <v>11</v>
       </c>
@@ -5019,7 +5025,7 @@
         <v>registerField(Fields::ILinkAR, "ILinkAR", 31, 1, 0);</v>
       </c>
     </row>
-    <row r="167" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>43</v>
       </c>
@@ -5047,7 +5053,7 @@
         <v>registerField(Fields::VBLNK, "VBLNK", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="168" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C168">
         <v>1</v>
       </c>
@@ -5072,7 +5078,7 @@
         <v>registerField(Fields::GPU, "GPU", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="169" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C169">
         <v>2</v>
       </c>
@@ -5097,7 +5103,7 @@
         <v>registerField(Fields::CDROM, "CDROM", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="170" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C170">
         <v>3</v>
       </c>
@@ -5122,7 +5128,7 @@
         <v>registerField(Fields::DMA, "DMA", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="171" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C171">
         <v>4</v>
       </c>
@@ -5147,7 +5153,7 @@
         <v>registerField(Fields::TMR0, "TMR0", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="172" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C172">
         <v>5</v>
       </c>
@@ -5172,7 +5178,7 @@
         <v>registerField(Fields::TMR1, "TMR1", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="173" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C173">
         <v>6</v>
       </c>
@@ -5197,7 +5203,7 @@
         <v>registerField(Fields::TMR2, "TMR2", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="174" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C174">
         <v>7</v>
       </c>
@@ -5222,7 +5228,7 @@
         <v>registerField(Fields::SIO0, "SIO0", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="175" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C175">
         <v>8</v>
       </c>
@@ -5247,7 +5253,7 @@
         <v>registerField(Fields::SIO1, "SIO1", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="176" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C176">
         <v>9</v>
       </c>
@@ -5272,7 +5278,7 @@
         <v>registerField(Fields::SPU, "SPU", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="177" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C177">
         <v>10</v>
       </c>
@@ -5297,7 +5303,7 @@
         <v>registerField(Fields::PIO, "PIO", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="178" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C178">
         <v>11</v>
       </c>
@@ -5322,7 +5328,7 @@
         <v>registerField(Fields::EVBLANK, "EVBLANK", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="179" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C179">
         <v>12</v>
       </c>
@@ -5347,7 +5353,7 @@
         <v>registerField(Fields::DVD, "DVD", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="180" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C180">
         <v>13</v>
       </c>
@@ -5372,7 +5378,7 @@
         <v>registerField(Fields::PCMCIA, "PCMCIA", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="181" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C181">
         <v>14</v>
       </c>
@@ -5397,7 +5403,7 @@
         <v>registerField(Fields::TMR3, "TMR3", 14, 1, 0);</v>
       </c>
     </row>
-    <row r="182" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C182">
         <v>15</v>
       </c>
@@ -5422,7 +5428,7 @@
         <v>registerField(Fields::TMR4, "TMR4", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="183" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C183">
         <v>16</v>
       </c>
@@ -5447,7 +5453,7 @@
         <v>registerField(Fields::TMR5, "TMR5", 16, 1, 0);</v>
       </c>
     </row>
-    <row r="184" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C184">
         <v>17</v>
       </c>
@@ -5472,7 +5478,7 @@
         <v>registerField(Fields::SIO2, "SIO2", 17, 1, 0);</v>
       </c>
     </row>
-    <row r="185" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C185">
         <v>18</v>
       </c>
@@ -5497,7 +5503,7 @@
         <v>registerField(Fields::HTR0, "HTR0", 18, 1, 0);</v>
       </c>
     </row>
-    <row r="186" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C186">
         <v>19</v>
       </c>
@@ -5522,7 +5528,7 @@
         <v>registerField(Fields::HTR1, "HTR1", 19, 1, 0);</v>
       </c>
     </row>
-    <row r="187" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C187">
         <v>20</v>
       </c>
@@ -5547,7 +5553,7 @@
         <v>registerField(Fields::HTR2, "HTR2", 20, 1, 0);</v>
       </c>
     </row>
-    <row r="188" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C188">
         <v>21</v>
       </c>
@@ -5572,7 +5578,7 @@
         <v>registerField(Fields::HTR3, "HTR3", 21, 1, 0);</v>
       </c>
     </row>
-    <row r="189" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C189">
         <v>22</v>
       </c>
@@ -5597,7 +5603,7 @@
         <v>registerField(Fields::USB, "USB", 22, 1, 0);</v>
       </c>
     </row>
-    <row r="190" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C190">
         <v>23</v>
       </c>
@@ -5622,7 +5628,7 @@
         <v>registerField(Fields::EXTR, "EXTR", 23, 1, 0);</v>
       </c>
     </row>
-    <row r="191" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C191">
         <v>24</v>
       </c>
@@ -5647,7 +5653,7 @@
         <v>registerField(Fields::FWRE, "FWRE", 24, 1, 0);</v>
       </c>
     </row>
-    <row r="192" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C192">
         <v>25</v>
       </c>
@@ -5672,7 +5678,7 @@
         <v>registerField(Fields::FDMA, "FDMA", 25, 1, 0);</v>
       </c>
     </row>
-    <row r="194" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>12</v>
       </c>
@@ -5700,7 +5706,7 @@
         <v>registerField(Fields::VBLNK, "VBLNK", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="195" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C195">
         <v>1</v>
       </c>
@@ -5725,7 +5731,7 @@
         <v>registerField(Fields::GPU, "GPU", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="196" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C196">
         <v>2</v>
       </c>
@@ -5750,7 +5756,7 @@
         <v>registerField(Fields::CDROM, "CDROM", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="197" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C197">
         <v>3</v>
       </c>
@@ -5775,7 +5781,7 @@
         <v>registerField(Fields::DMA, "DMA", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="198" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C198">
         <v>4</v>
       </c>
@@ -5800,7 +5806,7 @@
         <v>registerField(Fields::TMR0, "TMR0", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="199" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C199">
         <v>5</v>
       </c>
@@ -5825,7 +5831,7 @@
         <v>registerField(Fields::TMR1, "TMR1", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="200" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C200">
         <v>6</v>
       </c>
@@ -5850,7 +5856,7 @@
         <v>registerField(Fields::TMR2, "TMR2", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="201" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C201">
         <v>7</v>
       </c>
@@ -5875,7 +5881,7 @@
         <v>registerField(Fields::SIO0, "SIO0", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="202" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C202">
         <v>8</v>
       </c>
@@ -5900,7 +5906,7 @@
         <v>registerField(Fields::SIO1, "SIO1", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="203" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C203">
         <v>9</v>
       </c>
@@ -5925,7 +5931,7 @@
         <v>registerField(Fields::SPU, "SPU", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="204" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C204">
         <v>10</v>
       </c>
@@ -5950,7 +5956,7 @@
         <v>registerField(Fields::PIO, "PIO", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="205" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C205">
         <v>11</v>
       </c>
@@ -5975,7 +5981,7 @@
         <v>registerField(Fields::EVBLANK, "EVBLANK", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="206" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C206">
         <v>12</v>
       </c>
@@ -6000,7 +6006,7 @@
         <v>registerField(Fields::DVD, "DVD", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="207" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C207">
         <v>13</v>
       </c>
@@ -6025,7 +6031,7 @@
         <v>registerField(Fields::PCMCIA, "PCMCIA", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="208" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C208">
         <v>14</v>
       </c>
@@ -6050,7 +6056,7 @@
         <v>registerField(Fields::TMR3, "TMR3", 14, 1, 0);</v>
       </c>
     </row>
-    <row r="209" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C209">
         <v>15</v>
       </c>
@@ -6075,7 +6081,7 @@
         <v>registerField(Fields::TMR4, "TMR4", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="210" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C210">
         <v>16</v>
       </c>
@@ -6100,7 +6106,7 @@
         <v>registerField(Fields::TMR5, "TMR5", 16, 1, 0);</v>
       </c>
     </row>
-    <row r="211" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C211">
         <v>17</v>
       </c>
@@ -6125,7 +6131,7 @@
         <v>registerField(Fields::SIO2, "SIO2", 17, 1, 0);</v>
       </c>
     </row>
-    <row r="212" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C212">
         <v>18</v>
       </c>
@@ -6150,7 +6156,7 @@
         <v>registerField(Fields::HTR0, "HTR0", 18, 1, 0);</v>
       </c>
     </row>
-    <row r="213" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C213">
         <v>19</v>
       </c>
@@ -6175,7 +6181,7 @@
         <v>registerField(Fields::HTR1, "HTR1", 19, 1, 0);</v>
       </c>
     </row>
-    <row r="214" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C214">
         <v>20</v>
       </c>
@@ -6200,7 +6206,7 @@
         <v>registerField(Fields::HTR2, "HTR2", 20, 1, 0);</v>
       </c>
     </row>
-    <row r="215" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C215">
         <v>21</v>
       </c>
@@ -6225,7 +6231,7 @@
         <v>registerField(Fields::HTR3, "HTR3", 21, 1, 0);</v>
       </c>
     </row>
-    <row r="216" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C216">
         <v>22</v>
       </c>
@@ -6250,7 +6256,7 @@
         <v>registerField(Fields::USB, "USB", 22, 1, 0);</v>
       </c>
     </row>
-    <row r="217" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C217">
         <v>23</v>
       </c>
@@ -6275,7 +6281,7 @@
         <v>registerField(Fields::EXTR, "EXTR", 23, 1, 0);</v>
       </c>
     </row>
-    <row r="218" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C218">
         <v>24</v>
       </c>
@@ -6300,7 +6306,7 @@
         <v>registerField(Fields::FWRE, "FWRE", 24, 1, 0);</v>
       </c>
     </row>
-    <row r="219" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C219">
         <v>25</v>
       </c>
@@ -6325,7 +6331,7 @@
         <v>registerField(Fields::FDMA, "FDMA", 25, 1, 0);</v>
       </c>
     </row>
-    <row r="221" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
         <v>239</v>
       </c>
@@ -6353,7 +6359,7 @@
         <v>registerField(Fields::Priority0, "Priority0", 0, 3, 0);</v>
       </c>
     </row>
-    <row r="222" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C222">
         <v>1</v>
       </c>
@@ -6378,7 +6384,7 @@
         <v>registerField(Fields::Enable0, "Enable0", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="223" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C223">
         <v>2</v>
       </c>
@@ -6403,7 +6409,7 @@
         <v>registerField(Fields::Priority1, "Priority1", 4, 3, 0);</v>
       </c>
     </row>
-    <row r="224" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C224">
         <v>3</v>
       </c>
@@ -6428,7 +6434,7 @@
         <v>registerField(Fields::Enable1, "Enable1", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="225" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C225">
         <v>4</v>
       </c>
@@ -6453,7 +6459,7 @@
         <v>registerField(Fields::Priority2, "Priority2", 8, 3, 0);</v>
       </c>
     </row>
-    <row r="226" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C226">
         <v>5</v>
       </c>
@@ -6478,7 +6484,7 @@
         <v>registerField(Fields::Enable2, "Enable2", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="227" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C227">
         <v>6</v>
       </c>
@@ -6503,7 +6509,7 @@
         <v>registerField(Fields::Priority3, "Priority3", 12, 3, 0);</v>
       </c>
     </row>
-    <row r="228" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C228">
         <v>7</v>
       </c>
@@ -6528,7 +6534,7 @@
         <v>registerField(Fields::Enable3, "Enable3", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="229" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C229">
         <v>8</v>
       </c>
@@ -6553,7 +6559,7 @@
         <v>registerField(Fields::Priority4, "Priority4", 16, 3, 0);</v>
       </c>
     </row>
-    <row r="230" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C230">
         <v>9</v>
       </c>
@@ -6578,7 +6584,7 @@
         <v>registerField(Fields::Enable4, "Enable4", 19, 1, 0);</v>
       </c>
     </row>
-    <row r="231" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C231">
         <v>10</v>
       </c>
@@ -6603,7 +6609,7 @@
         <v>registerField(Fields::Priority5, "Priority5", 20, 3, 0);</v>
       </c>
     </row>
-    <row r="232" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C232">
         <v>11</v>
       </c>
@@ -6628,7 +6634,7 @@
         <v>registerField(Fields::Enable5, "Enable5", 23, 1, 0);</v>
       </c>
     </row>
-    <row r="233" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C233">
         <v>12</v>
       </c>
@@ -6653,7 +6659,7 @@
         <v>registerField(Fields::Priority6, "Priority6", 24, 3, 0);</v>
       </c>
     </row>
-    <row r="234" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C234">
         <v>13</v>
       </c>
@@ -6678,7 +6684,7 @@
         <v>registerField(Fields::Enable6, "Enable6", 27, 1, 0);</v>
       </c>
     </row>
-    <row r="235" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C235">
         <v>14</v>
       </c>
@@ -6703,7 +6709,7 @@
         <v>registerField(Fields::PriorityCPU, "PriorityCPU", 28, 3, 0);</v>
       </c>
     </row>
-    <row r="236" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C236">
         <v>15</v>
       </c>
@@ -6728,7 +6734,7 @@
         <v>registerField(Fields::EnableCPU, "EnableCPU", 31, 1, 0);</v>
       </c>
     </row>
-    <row r="238" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
         <v>241</v>
       </c>
@@ -6756,7 +6762,7 @@
         <v>registerField(Fields::IRM0, "IRM0", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="239" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C239">
         <v>1</v>
       </c>
@@ -6781,7 +6787,7 @@
         <v>registerField(Fields::IRM1, "IRM1", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="240" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C240">
         <v>2</v>
       </c>
@@ -6806,7 +6812,7 @@
         <v>registerField(Fields::IRM2, "IRM2", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="241" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C241">
         <v>3</v>
       </c>
@@ -6831,7 +6837,7 @@
         <v>registerField(Fields::IRM3, "IRM3", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="242" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C242">
         <v>4</v>
       </c>
@@ -6856,7 +6862,7 @@
         <v>registerField(Fields::IRM4, "IRM4", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="243" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C243">
         <v>5</v>
       </c>
@@ -6881,7 +6887,7 @@
         <v>registerField(Fields::IRM5, "IRM5", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="244" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C244">
         <v>6</v>
       </c>
@@ -6906,7 +6912,7 @@
         <v>registerField(Fields::IRM6, "IRM6", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="245" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C245">
         <v>7</v>
       </c>
@@ -6931,7 +6937,7 @@
         <v>registerField(Fields::Error, "Error", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="246" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C246">
         <v>8</v>
       </c>
@@ -6956,7 +6962,7 @@
         <v>registerField(Fields::TCM0, "TCM0", 16, 1, 0);</v>
       </c>
     </row>
-    <row r="247" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C247">
         <v>9</v>
       </c>
@@ -6981,7 +6987,7 @@
         <v>registerField(Fields::TCM1, "TCM1", 17, 1, 0);</v>
       </c>
     </row>
-    <row r="248" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C248">
         <v>10</v>
       </c>
@@ -7006,7 +7012,7 @@
         <v>registerField(Fields::TCM2, "TCM2", 18, 1, 0);</v>
       </c>
     </row>
-    <row r="249" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C249">
         <v>11</v>
       </c>
@@ -7031,7 +7037,7 @@
         <v>registerField(Fields::TCM3, "TCM3", 19, 1, 0);</v>
       </c>
     </row>
-    <row r="250" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C250">
         <v>12</v>
       </c>
@@ -7056,7 +7062,7 @@
         <v>registerField(Fields::TCM4, "TCM4", 20, 1, 0);</v>
       </c>
     </row>
-    <row r="251" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C251">
         <v>13</v>
       </c>
@@ -7081,7 +7087,7 @@
         <v>registerField(Fields::TCM5, "TCM5", 21, 1, 0);</v>
       </c>
     </row>
-    <row r="252" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C252">
         <v>14</v>
       </c>
@@ -7106,7 +7112,7 @@
         <v>registerField(Fields::TCM6, "TCM6", 22, 1, 0);</v>
       </c>
     </row>
-    <row r="253" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C253">
         <v>15</v>
       </c>
@@ -7131,7 +7137,7 @@
         <v>registerField(Fields::MasterEnable, "MasterEnable", 23, 1, 0);</v>
       </c>
     </row>
-    <row r="254" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C254">
         <v>16</v>
       </c>
@@ -7156,7 +7162,7 @@
         <v>registerField(Fields::TCI0, "TCI0", 24, 1, 0);</v>
       </c>
     </row>
-    <row r="255" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C255">
         <v>17</v>
       </c>
@@ -7181,7 +7187,7 @@
         <v>registerField(Fields::TCI1, "TCI1", 25, 1, 0);</v>
       </c>
     </row>
-    <row r="256" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C256">
         <v>18</v>
       </c>
@@ -7206,7 +7212,7 @@
         <v>registerField(Fields::TCI2, "TCI2", 26, 1, 0);</v>
       </c>
     </row>
-    <row r="257" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C257">
         <v>19</v>
       </c>
@@ -7231,7 +7237,7 @@
         <v>registerField(Fields::TCI3, "TCI3", 27, 1, 0);</v>
       </c>
     </row>
-    <row r="258" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C258">
         <v>20</v>
       </c>
@@ -7256,7 +7262,7 @@
         <v>registerField(Fields::TCI4, "TCI4", 28, 1, 0);</v>
       </c>
     </row>
-    <row r="259" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C259">
         <v>21</v>
       </c>
@@ -7281,7 +7287,7 @@
         <v>registerField(Fields::TCI5, "TCI5", 29, 1, 0);</v>
       </c>
     </row>
-    <row r="260" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C260">
         <v>22</v>
       </c>
@@ -7306,7 +7312,7 @@
         <v>registerField(Fields::TCI6, "TCI6", 30, 1, 0);</v>
       </c>
     </row>
-    <row r="261" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C261">
         <v>23</v>
       </c>
@@ -7331,7 +7337,7 @@
         <v>registerField(Fields::MasterInterrupt, "MasterInterrupt", 31, 1, 0);</v>
       </c>
     </row>
-    <row r="263" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
         <v>29</v>
       </c>
@@ -7359,7 +7365,7 @@
         <v>registerField(Fields::SyncEnable, "SyncEnable", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="264" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C264">
         <v>1</v>
       </c>
@@ -7384,7 +7390,7 @@
         <v>registerField(Fields::SyncMode, "SyncMode", 1, 2, 0);</v>
       </c>
     </row>
-    <row r="265" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C265">
         <v>2</v>
       </c>
@@ -7409,7 +7415,7 @@
         <v>registerField(Fields::ResetMode, "ResetMode", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="266" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C266">
         <v>3</v>
       </c>
@@ -7434,7 +7440,7 @@
         <v>registerField(Fields::IrqOnTarget, "IrqOnTarget", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="267" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C267">
         <v>4</v>
       </c>
@@ -7459,7 +7465,7 @@
         <v>registerField(Fields::IrqOnOF, "IrqOnOF", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="268" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C268">
         <v>5</v>
       </c>
@@ -7484,7 +7490,7 @@
         <v>registerField(Fields::IrqRepeat, "IrqRepeat", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="269" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C269">
         <v>6</v>
       </c>
@@ -7509,7 +7515,7 @@
         <v>registerField(Fields::IrqToggle, "IrqToggle", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="270" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C270">
         <v>7</v>
       </c>
@@ -7534,7 +7540,7 @@
         <v>registerField(Fields::ClockSrc, "ClockSrc", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="271" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C271">
         <v>8</v>
       </c>
@@ -7559,7 +7565,7 @@
         <v>registerField(Fields::Prescale0, "Prescale0", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="272" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C272">
         <v>9</v>
       </c>
@@ -7584,7 +7590,7 @@
         <v>registerField(Fields::IrqRequest, "IrqRequest", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="273" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C273">
         <v>10</v>
       </c>
@@ -7609,7 +7615,7 @@
         <v>registerField(Fields::ReachTarget, "ReachTarget", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="274" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C274">
         <v>11</v>
       </c>
@@ -7634,7 +7640,7 @@
         <v>registerField(Fields::ReachOF, "ReachOF", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="275" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C275">
         <v>12</v>
       </c>
@@ -7659,7 +7665,7 @@
         <v>registerField(Fields::Prescale1, "Prescale1", 13, 2, 0);</v>
       </c>
     </row>
-    <row r="277" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
         <v>240</v>
       </c>
@@ -7687,7 +7693,7 @@
         <v>registerField(Fields::Priority7, "Priority7", 0, 3, 0);</v>
       </c>
     </row>
-    <row r="278" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C278">
         <v>1</v>
       </c>
@@ -7712,7 +7718,7 @@
         <v>registerField(Fields::Enable7, "Enable7", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="279" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C279">
         <v>2</v>
       </c>
@@ -7737,7 +7743,7 @@
         <v>registerField(Fields::Priority8, "Priority8", 4, 3, 0);</v>
       </c>
     </row>
-    <row r="280" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C280">
         <v>3</v>
       </c>
@@ -7762,7 +7768,7 @@
         <v>registerField(Fields::Enable8, "Enable8", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="281" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C281">
         <v>4</v>
       </c>
@@ -7787,7 +7793,7 @@
         <v>registerField(Fields::Priority9, "Priority9", 8, 3, 0);</v>
       </c>
     </row>
-    <row r="282" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C282">
         <v>5</v>
       </c>
@@ -7812,7 +7818,7 @@
         <v>registerField(Fields::Enable9, "Enable9", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="283" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C283">
         <v>6</v>
       </c>
@@ -7837,7 +7843,7 @@
         <v>registerField(Fields::Priority10, "Priority10", 12, 3, 0);</v>
       </c>
     </row>
-    <row r="284" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C284">
         <v>7</v>
       </c>
@@ -7862,7 +7868,7 @@
         <v>registerField(Fields::Enable10, "Enable10", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="285" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C285">
         <v>8</v>
       </c>
@@ -7887,7 +7893,7 @@
         <v>registerField(Fields::Priority11, "Priority11", 16, 3, 0);</v>
       </c>
     </row>
-    <row r="286" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C286">
         <v>9</v>
       </c>
@@ -7912,7 +7918,7 @@
         <v>registerField(Fields::Enable11, "Enable11", 19, 1, 0);</v>
       </c>
     </row>
-    <row r="287" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C287">
         <v>10</v>
       </c>
@@ -7937,7 +7943,7 @@
         <v>registerField(Fields::Priority12, "Priority12", 20, 3, 0);</v>
       </c>
     </row>
-    <row r="288" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C288">
         <v>11</v>
       </c>
@@ -7962,7 +7968,7 @@
         <v>registerField(Fields::Enable12, "Enable12", 23, 1, 0);</v>
       </c>
     </row>
-    <row r="289" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C289">
         <v>12</v>
       </c>
@@ -7987,7 +7993,7 @@
         <v>registerField(Fields::Priority13, "Priority13", 24, 3, 0);</v>
       </c>
     </row>
-    <row r="290" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C290">
         <v>13</v>
       </c>
@@ -8012,7 +8018,7 @@
         <v>registerField(Fields::Enable13, "Enable13", 27, 1, 0);</v>
       </c>
     </row>
-    <row r="292" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
         <v>242</v>
       </c>
@@ -8040,7 +8046,7 @@
         <v>registerField(Fields::IQE0, "IQE0", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="293" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C293">
         <v>1</v>
       </c>
@@ -8065,7 +8071,7 @@
         <v>registerField(Fields::IQE1, "IQE1", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="294" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C294">
         <v>2</v>
       </c>
@@ -8090,7 +8096,7 @@
         <v>registerField(Fields::IQE2, "IQE2", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="295" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C295">
         <v>3</v>
       </c>
@@ -8115,7 +8121,7 @@
         <v>registerField(Fields::IQE3, "IQE3", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="296" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C296">
         <v>4</v>
       </c>
@@ -8140,7 +8146,7 @@
         <v>registerField(Fields::IQE4, "IQE4", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="297" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C297">
         <v>5</v>
       </c>
@@ -8165,7 +8171,7 @@
         <v>registerField(Fields::IQE5, "IQE5", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="298" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C298">
         <v>6</v>
       </c>
@@ -8190,7 +8196,7 @@
         <v>registerField(Fields::IQE6, "IQE6", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="299" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C299">
         <v>7</v>
       </c>
@@ -8215,7 +8221,7 @@
         <v>registerField(Fields::IQE7, "IQE7", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="300" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C300">
         <v>8</v>
       </c>
@@ -8240,7 +8246,7 @@
         <v>registerField(Fields::IQE8, "IQE8", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="301" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C301">
         <v>9</v>
       </c>
@@ -8265,7 +8271,7 @@
         <v>registerField(Fields::IQE9, "IQE9", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="302" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C302">
         <v>10</v>
       </c>
@@ -8290,7 +8296,7 @@
         <v>registerField(Fields::IQE10, "IQE10", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="303" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C303">
         <v>11</v>
       </c>
@@ -8315,7 +8321,7 @@
         <v>registerField(Fields::IQE11, "IQE11", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="304" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C304">
         <v>12</v>
       </c>
@@ -8340,7 +8346,7 @@
         <v>registerField(Fields::IQE12, "IQE12", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="305" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C305">
         <v>13</v>
       </c>
@@ -8365,7 +8371,7 @@
         <v>registerField(Fields::IQE13, "IQE13", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="306" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C306">
         <v>14</v>
       </c>
@@ -8390,7 +8396,7 @@
         <v>registerField(Fields::TCM7, "TCM7", 16, 1, 0);</v>
       </c>
     </row>
-    <row r="307" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C307">
         <v>15</v>
       </c>
@@ -8415,7 +8421,7 @@
         <v>registerField(Fields::TCM8, "TCM8", 17, 1, 0);</v>
       </c>
     </row>
-    <row r="308" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C308">
         <v>16</v>
       </c>
@@ -8440,7 +8446,7 @@
         <v>registerField(Fields::TCM9, "TCM9", 18, 1, 0);</v>
       </c>
     </row>
-    <row r="309" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C309">
         <v>17</v>
       </c>
@@ -8465,7 +8471,7 @@
         <v>registerField(Fields::TCM10, "TCM10", 19, 1, 0);</v>
       </c>
     </row>
-    <row r="310" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C310">
         <v>18</v>
       </c>
@@ -8490,7 +8496,7 @@
         <v>registerField(Fields::TCM11, "TCM11", 20, 1, 0);</v>
       </c>
     </row>
-    <row r="311" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C311">
         <v>19</v>
       </c>
@@ -8515,7 +8521,7 @@
         <v>registerField(Fields::TCM12, "TCM12", 21, 1, 0);</v>
       </c>
     </row>
-    <row r="312" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C312">
         <v>20</v>
       </c>
@@ -8540,7 +8546,7 @@
         <v>registerField(Fields::TCM13, "TCM13", 22, 1, 0);</v>
       </c>
     </row>
-    <row r="313" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C313">
         <v>21</v>
       </c>
@@ -8565,7 +8571,7 @@
         <v>registerField(Fields::TCI7, "TCI7", 24, 1, 0);</v>
       </c>
     </row>
-    <row r="314" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C314">
         <v>22</v>
       </c>
@@ -8590,7 +8596,7 @@
         <v>registerField(Fields::TCI8, "TCI8", 25, 1, 0);</v>
       </c>
     </row>
-    <row r="315" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C315">
         <v>23</v>
       </c>
@@ -8615,7 +8621,7 @@
         <v>registerField(Fields::TCI9, "TCI9", 26, 1, 0);</v>
       </c>
     </row>
-    <row r="316" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C316">
         <v>24</v>
       </c>
@@ -8640,7 +8646,7 @@
         <v>registerField(Fields::TCI10, "TCI10", 27, 1, 0);</v>
       </c>
     </row>
-    <row r="317" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C317">
         <v>25</v>
       </c>
@@ -8665,7 +8671,7 @@
         <v>registerField(Fields::TCI11, "TCI11", 28, 1, 0);</v>
       </c>
     </row>
-    <row r="318" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C318">
         <v>26</v>
       </c>
@@ -8690,7 +8696,7 @@
         <v>registerField(Fields::TCI12, "TCI12", 29, 1, 0);</v>
       </c>
     </row>
-    <row r="319" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C319">
         <v>27</v>
       </c>
@@ -8715,7 +8721,7 @@
         <v>registerField(Fields::TCI13, "TCI13", 30, 1, 0);</v>
       </c>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>290</v>
       </c>
@@ -8749,7 +8755,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="322" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C322">
         <v>1</v>
       </c>
@@ -8774,7 +8780,7 @@
         <v>registerField(Fields::ConstToggle, "ConstToggle", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C323">
         <v>2</v>
       </c>
@@ -8799,7 +8805,7 @@
         <v>registerField(Fields::LinExpMode, "LinExpMode", 13, 2, 0);</v>
       </c>
     </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C324">
         <v>3</v>
       </c>
@@ -8824,7 +8830,7 @@
         <v>registerField(Fields::X, "X", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C325">
         <v>4</v>
       </c>
@@ -8849,7 +8855,7 @@
         <v>registerField(Fields::LinExpValue, "LinExpValue", 0, 7, 0);</v>
       </c>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
         <v>291</v>
       </c>
@@ -8877,7 +8883,7 @@
         <v>registerField(Fields::SL, "SL", 0, 4, 0);</v>
       </c>
     </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C328">
         <v>1</v>
       </c>
@@ -8902,7 +8908,7 @@
         <v>registerField(Fields::DR, "DR", 4, 4, 0);</v>
       </c>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C329">
         <v>2</v>
       </c>
@@ -8927,7 +8933,7 @@
         <v>registerField(Fields::AR, "AR", 8, 7, 0);</v>
       </c>
     </row>
-    <row r="330" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C330">
         <v>3</v>
       </c>
@@ -8952,7 +8958,7 @@
         <v>registerField(Fields::X, "X", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
         <v>295</v>
       </c>
@@ -8980,7 +8986,7 @@
         <v>registerField(Fields::RR, "RR", 0, 5, 0);</v>
       </c>
     </row>
-    <row r="333" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C333">
         <v>1</v>
       </c>
@@ -9005,7 +9011,7 @@
         <v>registerField(Fields::Z, "Z", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="334" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C334">
         <v>2</v>
       </c>
@@ -9030,7 +9036,7 @@
         <v>registerField(Fields::SR, "SR", 6, 7, 0);</v>
       </c>
     </row>
-    <row r="335" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="335" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C335">
         <v>3</v>
       </c>
@@ -9055,7 +9061,7 @@
         <v>registerField(Fields::Y, "Y", 13, 3, 0);</v>
       </c>
     </row>
-    <row r="337" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="337" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
         <v>324</v>
       </c>
@@ -9086,7 +9092,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="338" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C338">
         <v>1</v>
       </c>
@@ -9111,7 +9117,7 @@
         <v>registerField(Fields::V1, "V1", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="339" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="339" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C339">
         <v>2</v>
       </c>
@@ -9136,7 +9142,7 @@
         <v>registerField(Fields::V2, "V2", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="340" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C340">
         <v>3</v>
       </c>
@@ -9161,7 +9167,7 @@
         <v>registerField(Fields::V3, "V3", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="341" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="341" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C341">
         <v>4</v>
       </c>
@@ -9186,7 +9192,7 @@
         <v>registerField(Fields::V4, "V4", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="342" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C342">
         <v>5</v>
       </c>
@@ -9211,7 +9217,7 @@
         <v>registerField(Fields::V5, "V5", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="343" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="343" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C343">
         <v>6</v>
       </c>
@@ -9236,7 +9242,7 @@
         <v>registerField(Fields::V6, "V6", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="344" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="344" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C344">
         <v>7</v>
       </c>
@@ -9261,7 +9267,7 @@
         <v>registerField(Fields::V7, "V7", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="345" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="345" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C345">
         <v>8</v>
       </c>
@@ -9286,7 +9292,7 @@
         <v>registerField(Fields::V8, "V8", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="346" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="346" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C346">
         <v>9</v>
       </c>
@@ -9311,7 +9317,7 @@
         <v>registerField(Fields::V9, "V9", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="347" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="347" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C347">
         <v>10</v>
       </c>
@@ -9336,7 +9342,7 @@
         <v>registerField(Fields::V10, "V10", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="348" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="348" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C348">
         <v>11</v>
       </c>
@@ -9361,7 +9367,7 @@
         <v>registerField(Fields::V11, "V11", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="349" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="349" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C349">
         <v>12</v>
       </c>
@@ -9386,7 +9392,7 @@
         <v>registerField(Fields::V12, "V12", 12, 1, 0);</v>
       </c>
     </row>
-    <row r="350" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="350" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C350">
         <v>13</v>
       </c>
@@ -9411,7 +9417,7 @@
         <v>registerField(Fields::V13, "V13", 13, 1, 0);</v>
       </c>
     </row>
-    <row r="351" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="351" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C351">
         <v>14</v>
       </c>
@@ -9436,7 +9442,7 @@
         <v>registerField(Fields::V14, "V14", 14, 1, 0);</v>
       </c>
     </row>
-    <row r="352" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="352" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C352">
         <v>15</v>
       </c>
@@ -9461,7 +9467,7 @@
         <v>registerField(Fields::V15, "V15", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="354" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="354" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
         <v>325</v>
       </c>
@@ -9492,7 +9498,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="355" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="355" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C355">
         <v>1</v>
       </c>
@@ -9517,7 +9523,7 @@
         <v>registerField(Fields::V17, "V17", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="356" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C356">
         <v>2</v>
       </c>
@@ -9542,7 +9548,7 @@
         <v>registerField(Fields::V18, "V18", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="357" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="357" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C357">
         <v>3</v>
       </c>
@@ -9567,7 +9573,7 @@
         <v>registerField(Fields::V19, "V19", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="358" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="358" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C358">
         <v>4</v>
       </c>
@@ -9592,7 +9598,7 @@
         <v>registerField(Fields::V20, "V20", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="359" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="359" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C359">
         <v>5</v>
       </c>
@@ -9617,7 +9623,7 @@
         <v>registerField(Fields::V21, "V21", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="360" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="360" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C360">
         <v>6</v>
       </c>
@@ -9642,7 +9648,7 @@
         <v>registerField(Fields::V22, "V22", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="361" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="361" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C361">
         <v>7</v>
       </c>
@@ -9667,7 +9673,7 @@
         <v>registerField(Fields::V23, "V23", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="363" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="363" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
         <v>328</v>
       </c>
@@ -9695,7 +9701,7 @@
         <v>registerField(Fields::SINER, "SINER", 0, 1, 0);</v>
       </c>
     </row>
-    <row r="364" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="364" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C364">
         <v>1</v>
       </c>
@@ -9720,7 +9726,7 @@
         <v>registerField(Fields::SINEL, "SINEL", 1, 1, 0);</v>
       </c>
     </row>
-    <row r="365" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="365" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C365">
         <v>2</v>
       </c>
@@ -9745,7 +9751,7 @@
         <v>registerField(Fields::SINR, "SINR", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="366" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="366" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C366">
         <v>3</v>
       </c>
@@ -9770,7 +9776,7 @@
         <v>registerField(Fields::SINL, "SINL", 3, 1, 0);</v>
       </c>
     </row>
-    <row r="367" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C367">
         <v>4</v>
       </c>
@@ -9795,7 +9801,7 @@
         <v>registerField(Fields::MINER, "MINER", 4, 1, 0);</v>
       </c>
     </row>
-    <row r="368" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="368" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C368">
         <v>5</v>
       </c>
@@ -9820,7 +9826,7 @@
         <v>registerField(Fields::MINEL, "MINEL", 5, 1, 0);</v>
       </c>
     </row>
-    <row r="369" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="369" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C369">
         <v>6</v>
       </c>
@@ -9845,7 +9851,7 @@
         <v>registerField(Fields::MINR, "MINR", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="370" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="370" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C370">
         <v>7</v>
       </c>
@@ -9870,7 +9876,7 @@
         <v>registerField(Fields::MINL, "MINL", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="371" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="371" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C371">
         <v>8</v>
       </c>
@@ -9895,7 +9901,7 @@
         <v>registerField(Fields::MSNDER, "MSNDER", 8, 1, 0);</v>
       </c>
     </row>
-    <row r="372" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="372" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C372">
         <v>9</v>
       </c>
@@ -9920,7 +9926,7 @@
         <v>registerField(Fields::MSNDEL, "MSNDEL", 9, 1, 0);</v>
       </c>
     </row>
-    <row r="373" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="373" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C373">
         <v>10</v>
       </c>
@@ -9945,7 +9951,7 @@
         <v>registerField(Fields::MSNDR, "MSNDR", 10, 1, 0);</v>
       </c>
     </row>
-    <row r="374" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="374" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C374">
         <v>11</v>
       </c>
@@ -9970,7 +9976,7 @@
         <v>registerField(Fields::MSNDL, "MSNDL", 11, 1, 0);</v>
       </c>
     </row>
-    <row r="376" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="376" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
         <v>342</v>
       </c>
@@ -9998,7 +10004,7 @@
         <v>registerField(Fields::DMABits, "DMABits", 1, 3, 0);</v>
       </c>
     </row>
-    <row r="377" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="377" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C377">
         <v>1</v>
       </c>
@@ -10023,7 +10029,7 @@
         <v>registerField(Fields::DMAMode, "DMAMode", 4, 2, 0);</v>
       </c>
     </row>
-    <row r="378" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="378" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C378">
         <v>2</v>
       </c>
@@ -10048,7 +10054,7 @@
         <v>registerField(Fields::IRQEnable, "IRQEnable", 6, 1, 0);</v>
       </c>
     </row>
-    <row r="379" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="379" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C379">
         <v>3</v>
       </c>
@@ -10073,7 +10079,7 @@
         <v>registerField(Fields::FxEnable, "FxEnable", 7, 1, 0);</v>
       </c>
     </row>
-    <row r="380" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="380" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C380">
         <v>4</v>
       </c>
@@ -10098,7 +10104,7 @@
         <v>registerField(Fields::NoiseClock, "NoiseClock", 8, 6, 0);</v>
       </c>
     </row>
-    <row r="381" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="381" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C381">
         <v>5</v>
       </c>
@@ -10123,7 +10129,7 @@
         <v>registerField(Fields::Mute, "Mute", 14, 1, 0);</v>
       </c>
     </row>
-    <row r="382" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="382" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C382">
         <v>6</v>
       </c>
@@ -10148,7 +10154,7 @@
         <v>registerField(Fields::CoreEnable, "CoreEnable", 15, 1, 0);</v>
       </c>
     </row>
-    <row r="384" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="384" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B384" t="s">
         <v>350</v>
       </c>
@@ -10176,7 +10182,7 @@
         <v>registerField(Fields::IrqCore0, "IrqCore0", 2, 1, 0);</v>
       </c>
     </row>
-    <row r="385" spans="3:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="385" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C385">
         <v>1</v>
       </c>
@@ -10199,6 +10205,34 @@
       <c r="J385" t="str">
         <f t="shared" ref="J385" si="72">"registerField(Fields::"&amp;D385&amp;", """&amp;D385&amp;""", "&amp;E385&amp;", "&amp;F385&amp;", "&amp;G385&amp;");"</f>
         <v>registerField(Fields::IrqCore1, "IrqCore1", 3, 1, 0);</v>
+      </c>
+    </row>
+    <row r="387" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B387" t="s">
+        <v>353</v>
+      </c>
+      <c r="C387">
+        <v>0</v>
+      </c>
+      <c r="D387" t="s">
+        <v>354</v>
+      </c>
+      <c r="E387">
+        <v>7</v>
+      </c>
+      <c r="F387">
+        <v>1</v>
+      </c>
+      <c r="G387">
+        <v>1</v>
+      </c>
+      <c r="I387" t="str">
+        <f t="shared" ref="I387" si="73">"static constexpr int "&amp;D387&amp;" = "&amp;C387&amp;";"</f>
+        <v>static constexpr int NeedData = 0;</v>
+      </c>
+      <c r="J387" t="str">
+        <f t="shared" ref="J387" si="74">"registerField(Fields::"&amp;D387&amp;", """&amp;D387&amp;""", "&amp;E387&amp;", "&amp;F387&amp;", "&amp;G387&amp;");"</f>
+        <v>registerField(Fields::NeedData, "NeedData", 7, 1, 1);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>